<commit_message>
remove nonsensical stop conditions
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="700" yWindow="900" windowWidth="31780" windowHeight="20700" tabRatio="500" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="-28920" yWindow="940" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="9" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -54,7 +54,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'!!Compartments'!$A$2:$U$5</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'!!Init species concentrations'!$C$1:$L$127</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'!!Model'!$A$1:$B$13</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'!!Parameters'!$A$1:$K$97</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="16" hidden="1">'!!Parameters'!$A$1:$K$95</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'!!Rate laws'!$C$1:$L$169</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'!!Reactions'!$A$2:$N$178</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="21" hidden="1">'!!References'!$A$1:$R$23</definedName>
@@ -425,7 +425,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4715" uniqueCount="2087">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4705" uniqueCount="2081">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -5877,25 +5877,7 @@
     <t>RNA half life</t>
   </si>
   <si>
-    <t>stop_cond_p_1</t>
-  </si>
-  <si>
-    <t>stop_cond_p_2</t>
-  </si>
-  <si>
     <t>!!ObjTables type='Data' class='StopCondition' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
-  </si>
-  <si>
-    <t>stop_cond_1</t>
-  </si>
-  <si>
-    <t>AXP_c &gt;= stop_cond_p_1</t>
-  </si>
-  <si>
-    <t>stop_cond_2</t>
-  </si>
-  <si>
-    <t>AXP_c + NTP_c &lt;= stop_cond_p_2</t>
   </si>
   <si>
     <t>!!ObjTables type='Data' class='Observation' objTablesVersion='0.0.8' schema='wc_lang' tableFormat='row'</t>
@@ -6941,9 +6923,11 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="#REF"/>
+      <sheetName val="Taxon"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -6967,9 +6951,11 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="#REF"/>
+      <sheetName val="Model"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7051,9 +7037,11 @@
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="#REF"/>
+      <sheetName val="Submodels"/>
     </sheetNames>
     <sheetDataSet>
       <sheetData sheetId="0" refreshError="1"/>
+      <sheetData sheetId="1" refreshError="1"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -7590,7 +7578,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7712,7 +7702,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12787,7 +12779,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L169"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15965,7 +15959,7 @@
         <v>-34190.379999999997</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
       <c r="J3" s="10" t="s">
         <v>1589</v>
@@ -15991,7 +15985,7 @@
         <v>1035619</v>
       </c>
       <c r="F4" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16011,7 +16005,7 @@
         <v>-40890.379999999997</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16031,7 +16025,7 @@
         <v>-23190.38</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16051,7 +16045,7 @@
         <v>-24290.38</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16071,7 +16065,7 @@
         <v>-1101856</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16091,7 +16085,7 @@
         <v>1098019</v>
       </c>
       <c r="F9" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16111,7 +16105,7 @@
         <v>-1164906</v>
       </c>
       <c r="F10" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16131,7 +16125,7 @@
         <v>-22290.38</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16151,7 +16145,7 @@
         <v>581419.19999999995</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16171,7 +16165,7 @@
         <v>-24690.38</v>
       </c>
       <c r="F13" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16191,7 +16185,7 @@
         <v>-22690.38</v>
       </c>
       <c r="F14" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16211,7 +16205,7 @@
         <v>-31190.38</v>
       </c>
       <c r="F15" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16231,7 +16225,7 @@
         <v>1052899</v>
       </c>
       <c r="F16" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16251,7 +16245,7 @@
         <v>-1728316</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16271,7 +16265,7 @@
         <v>-1521617000</v>
       </c>
       <c r="F18" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16291,7 +16285,7 @@
         <v>4972350</v>
       </c>
       <c r="F19" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16311,7 +16305,7 @@
         <v>-21590.38</v>
       </c>
       <c r="F20" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16331,7 +16325,7 @@
         <v>-29290.38</v>
       </c>
       <c r="F21" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16351,7 +16345,7 @@
         <v>-41190.379999999997</v>
       </c>
       <c r="F22" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16371,7 +16365,7 @@
         <v>-21990.38</v>
       </c>
       <c r="F23" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16391,7 +16385,7 @@
         <v>-21390.38</v>
       </c>
       <c r="F24" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16411,7 +16405,7 @@
         <v>-23890.38</v>
       </c>
       <c r="F25" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16431,7 +16425,7 @@
         <v>471096.2</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16451,7 +16445,7 @@
         <v>4381069</v>
       </c>
       <c r="F27" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16471,7 +16465,7 @@
         <v>-34390.379999999997</v>
       </c>
       <c r="F28" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16491,7 +16485,7 @@
         <v>-44490.38</v>
       </c>
       <c r="F29" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16511,7 +16505,7 @@
         <v>-36190.379999999997</v>
       </c>
       <c r="F30" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16531,7 +16525,7 @@
         <v>-22190.38</v>
       </c>
       <c r="F31" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16551,7 +16545,7 @@
         <v>-21990.38</v>
       </c>
       <c r="F32" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16571,7 +16565,7 @@
         <v>1066339</v>
       </c>
       <c r="F33" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16591,7 +16585,7 @@
         <v>-1132896</v>
       </c>
       <c r="F34" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16611,7 +16605,7 @@
         <v>-33790.379999999997</v>
       </c>
       <c r="F35" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -16631,7 +16625,7 @@
         <v>4381069</v>
       </c>
       <c r="F36" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -16651,7 +16645,7 @@
         <v>1066339</v>
       </c>
       <c r="F37" s="13" t="s">
-        <v>2047</v>
+        <v>2041</v>
       </c>
     </row>
   </sheetData>
@@ -16662,9 +16656,12 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K97"/>
+  <dimension ref="A1:K95"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A96" sqref="A96:XFD97"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18419,30 +18416,8 @@
         <v>43</v>
       </c>
     </row>
-    <row r="96" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A96" s="1" t="s">
-        <v>1816</v>
-      </c>
-      <c r="D96" s="1">
-        <v>1</v>
-      </c>
-      <c r="F96" s="12" t="s">
-        <v>403</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A97" s="1" t="s">
-        <v>1817</v>
-      </c>
-      <c r="D97" s="1">
-        <v>-1</v>
-      </c>
-      <c r="F97" s="12" t="s">
-        <v>403</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:K97"/>
+  <autoFilter ref="A1:K95"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>
   <pageSetup firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
@@ -18450,13 +18425,15 @@
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.1640625" style="7" customWidth="1"/>
+    <col min="1" max="1" width="14.33203125" style="7" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" style="7" customWidth="1"/>
     <col min="3" max="3" width="30" style="7" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="7" customWidth="1"/>
@@ -18466,7 +18443,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1818</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -18497,36 +18474,6 @@
       <c r="I2" s="2" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>1819</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1" t="s">
-        <v>1820</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-    </row>
-    <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>1821</v>
-      </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>1822</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
@@ -18554,16 +18501,16 @@
   <sheetData>
     <row r="1" spans="1:23" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1823</v>
+        <v>1817</v>
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G2" s="33" t="s">
-        <v>1824</v>
+        <v>1818</v>
       </c>
       <c r="H2" s="34"/>
       <c r="I2" s="33" t="s">
-        <v>1825</v>
+        <v>1819</v>
       </c>
       <c r="J2" s="34"/>
       <c r="K2" s="34"/>
@@ -18571,11 +18518,11 @@
       <c r="M2" s="34"/>
       <c r="N2" s="34"/>
       <c r="Q2" s="33" t="s">
-        <v>1826</v>
+        <v>1820</v>
       </c>
       <c r="R2" s="34"/>
       <c r="S2" s="33" t="s">
-        <v>1827</v>
+        <v>1821</v>
       </c>
       <c r="T2" s="34"/>
     </row>
@@ -18599,10 +18546,10 @@
         <v>110</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>1828</v>
+        <v>1822</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>1829</v>
+        <v>1823</v>
       </c>
       <c r="I3" s="5" t="s">
         <v>56</v>
@@ -18614,19 +18561,19 @@
         <v>73</v>
       </c>
       <c r="L3" s="5" t="s">
-        <v>1830</v>
+        <v>1824</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>1831</v>
+        <v>1825</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>1832</v>
+        <v>1826</v>
       </c>
       <c r="O3" s="5" t="s">
-        <v>1833</v>
+        <v>1827</v>
       </c>
       <c r="P3" s="5" t="s">
-        <v>1834</v>
+        <v>1828</v>
       </c>
       <c r="Q3" s="5" t="s">
         <v>31</v>
@@ -18652,23 +18599,23 @@
     </row>
     <row r="4" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>1835</v>
+        <v>1829</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1836</v>
+        <v>1830</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>1837</v>
+        <v>1831</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="1" t="s">
         <v>581</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1838</v>
+        <v>1832</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1839</v>
+        <v>1833</v>
       </c>
       <c r="I4" s="1">
         <v>37</v>
@@ -18683,89 +18630,89 @@
         <v>94</v>
       </c>
       <c r="U4" s="1" t="s">
-        <v>1840</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>1841</v>
+        <v>1835</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1842</v>
+        <v>1836</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1843</v>
+        <v>1837</v>
       </c>
       <c r="D5" s="6"/>
       <c r="E5" s="1" t="s">
         <v>581</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1838</v>
+        <v>1832</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1839</v>
+        <v>1833</v>
       </c>
       <c r="I5" s="7"/>
     </row>
     <row r="6" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>1844</v>
+        <v>1838</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1845</v>
+        <v>1839</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>1846</v>
+        <v>1840</v>
       </c>
       <c r="D6" s="6"/>
       <c r="E6" s="1" t="s">
         <v>581</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>1838</v>
+        <v>1832</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>1839</v>
+        <v>1833</v>
       </c>
       <c r="I6" s="7"/>
     </row>
     <row r="7" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>1847</v>
+        <v>1841</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1848</v>
+        <v>1842</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>1849</v>
+        <v>1843</v>
       </c>
       <c r="D7" s="6"/>
       <c r="E7" s="1" t="s">
         <v>581</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>1838</v>
+        <v>1832</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>1839</v>
+        <v>1833</v>
       </c>
       <c r="I7" s="7"/>
     </row>
     <row r="8" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>1850</v>
+        <v>1844</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1851</v>
+        <v>1845</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
       <c r="F8" s="1" t="s">
-        <v>1852</v>
+        <v>1846</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>1853</v>
+        <v>1847</v>
       </c>
       <c r="I8" s="1">
         <v>37</v>
@@ -18776,18 +18723,18 @@
     </row>
     <row r="9" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>1854</v>
+        <v>1848</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1855</v>
+        <v>1849</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
       <c r="F9" s="1" t="s">
-        <v>1856</v>
+        <v>1850</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>1857</v>
+        <v>1851</v>
       </c>
       <c r="I9" s="1">
         <v>30</v>
@@ -18798,15 +18745,15 @@
     </row>
     <row r="10" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>1858</v>
+        <v>1852</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1859</v>
+        <v>1853</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="G10" s="1" t="s">
-        <v>1860</v>
+        <v>1854</v>
       </c>
       <c r="I10" s="1">
         <v>37</v>
@@ -18817,15 +18764,15 @@
     </row>
     <row r="11" spans="1:23" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>1861</v>
+        <v>1855</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1862</v>
+        <v>1856</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="G11" s="1" t="s">
-        <v>1863</v>
+        <v>1857</v>
       </c>
       <c r="I11" s="1">
         <v>40</v>
@@ -18978,7 +18925,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1864</v>
+        <v>1858</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -18989,7 +18936,7 @@
         <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>1865</v>
+        <v>1859</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>44</v>
@@ -19003,38 +18950,38 @@
     </row>
     <row r="3" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1866</v>
+        <v>1860</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1867</v>
+        <v>1861</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1868</v>
+        <v>1862</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1840</v>
+        <v>1834</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>1869</v>
+        <v>1863</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1870</v>
+        <v>1864</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1850</v>
+        <v>1844</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>1871</v>
+        <v>1865</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1872</v>
+        <v>1866</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1854</v>
+        <v>1848</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="15.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -19069,12 +19016,12 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1873</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="G2" s="33" t="s">
-        <v>1874</v>
+        <v>1868</v>
       </c>
       <c r="H2" s="34"/>
     </row>
@@ -19116,56 +19063,56 @@
         <v>53</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>1875</v>
+        <v>1869</v>
       </c>
       <c r="N3" s="5" t="s">
-        <v>1876</v>
+        <v>1870</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>1877</v>
+        <v>1871</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1878</v>
+        <v>1872</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>1837</v>
+        <v>1831</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>1879</v>
+        <v>1873</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>581</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>1880</v>
+        <v>1874</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>1881</v>
+        <v>1875</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>1882</v>
+        <v>1876</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1878</v>
+        <v>1872</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>1883</v>
+        <v>1877</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>1837</v>
+        <v>1831</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>43</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>1884</v>
+        <v>1878</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>1885</v>
+        <v>1879</v>
       </c>
     </row>
     <row r="6" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -19223,7 +19170,7 @@
   <sheetData>
     <row r="1" spans="1:18" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>1886</v>
+        <v>1880</v>
       </c>
     </row>
     <row r="2" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -19234,46 +19181,46 @@
         <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>1887</v>
+        <v>1881</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>1888</v>
+        <v>1882</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>1889</v>
+        <v>1883</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>1890</v>
+        <v>1884</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>110</v>
       </c>
       <c r="H2" s="2" t="s">
+        <v>1885</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>1886</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>1887</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>1888</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>1889</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>1890</v>
+      </c>
+      <c r="N2" s="2" t="s">
         <v>1891</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>1892</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>1893</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>1894</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>1895</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>1896</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>1897</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>1898</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>1899</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>44</v>
@@ -19284,68 +19231,68 @@
     </row>
     <row r="3" spans="1:18" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>1900</v>
+        <v>1894</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1901</v>
+        <v>1895</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>1902</v>
+        <v>1896</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>1903</v>
+        <v>1897</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1">
         <v>2008</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>1904</v>
+        <v>1898</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>1905</v>
+        <v>1899</v>
       </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
-        <v>1837</v>
+        <v>1831</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>1837</v>
+        <v>1831</v>
       </c>
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1" t="s">
-        <v>1906</v>
+        <v>1900</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>1907</v>
+        <v>1901</v>
       </c>
       <c r="R3" s="1"/>
     </row>
     <row r="4" spans="1:18" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>1908</v>
+        <v>1902</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1909</v>
+        <v>1903</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>1910</v>
+        <v>1904</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>1911</v>
+        <v>1905</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1">
         <v>2014</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>1904</v>
+        <v>1898</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>1912</v>
+        <v>1906</v>
       </c>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -19355,134 +19302,134 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1" t="s">
-        <v>1913</v>
+        <v>1907</v>
       </c>
       <c r="Q4" s="1" t="s">
-        <v>1914</v>
+        <v>1908</v>
       </c>
       <c r="R4" s="1"/>
     </row>
     <row r="5" spans="1:18" ht="299.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>1915</v>
+        <v>1909</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1916</v>
+        <v>1910</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>1917</v>
+        <v>1911</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>1918</v>
+        <v>1912</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1">
         <v>2004</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>1904</v>
+        <v>1898</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>1912</v>
+        <v>1906</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>1919</v>
+        <v>1913</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>1920</v>
+        <v>1914</v>
       </c>
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1" t="s">
-        <v>1921</v>
+        <v>1915</v>
       </c>
       <c r="Q5" s="1" t="s">
-        <v>1922</v>
+        <v>1916</v>
       </c>
       <c r="R5" s="1"/>
     </row>
     <row r="6" spans="1:18" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>1923</v>
+        <v>1917</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1924</v>
+        <v>1918</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>1925</v>
+        <v>1919</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>1926</v>
+        <v>1920</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1">
         <v>2009</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>1904</v>
+        <v>1898</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>1927</v>
+        <v>1921</v>
       </c>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1" t="s">
-        <v>1928</v>
+        <v>1922</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>1929</v>
+        <v>1923</v>
       </c>
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1" t="s">
-        <v>1930</v>
+        <v>1924</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>1931</v>
+        <v>1925</v>
       </c>
       <c r="R6" s="1"/>
     </row>
     <row r="7" spans="1:18" ht="267.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>1932</v>
+        <v>1926</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1933</v>
+        <v>1927</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>1934</v>
+        <v>1928</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>1935</v>
+        <v>1929</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1">
         <v>2007</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>1904</v>
+        <v>1898</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>1936</v>
+        <v>1930</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
-        <v>1937</v>
+        <v>1931</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>1837</v>
+        <v>1831</v>
       </c>
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
-        <v>1938</v>
+        <v>1932</v>
       </c>
       <c r="R7" s="1"/>
     </row>
@@ -19491,24 +19438,24 @@
         <v>1670</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>1939</v>
+        <v>1933</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>1940</v>
+        <v>1934</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>1941</v>
+        <v>1935</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1">
         <v>2001</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>1942</v>
+        <v>1936</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1" t="s">
-        <v>1943</v>
+        <v>1937</v>
       </c>
       <c r="J8" s="1"/>
       <c r="K8" s="1"/>
@@ -19518,7 +19465,7 @@
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
       <c r="Q8" s="1" t="s">
-        <v>1944</v>
+        <v>1938</v>
       </c>
       <c r="R8" s="1"/>
     </row>
@@ -19527,26 +19474,26 @@
         <v>1684</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>1945</v>
+        <v>1939</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>1946</v>
+        <v>1940</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>1947</v>
+        <v>1941</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1">
         <v>2006</v>
       </c>
       <c r="G9" s="1" t="s">
+        <v>1936</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>1942</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>1948</v>
-      </c>
       <c r="I9" s="1" t="s">
-        <v>1949</v>
+        <v>1943</v>
       </c>
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
@@ -19556,217 +19503,217 @@
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
       <c r="Q9" s="1" t="s">
-        <v>1950</v>
+        <v>1944</v>
       </c>
       <c r="R9" s="1"/>
     </row>
     <row r="10" spans="1:18" ht="220.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>1951</v>
+        <v>1945</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1952</v>
+        <v>1946</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>1953</v>
+        <v>1947</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>1954</v>
+        <v>1948</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
         <v>1993</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>1904</v>
+        <v>1898</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>1955</v>
+        <v>1949</v>
       </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
-        <v>1956</v>
+        <v>1950</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>1837</v>
+        <v>1831</v>
       </c>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1" t="s">
-        <v>1957</v>
+        <v>1951</v>
       </c>
       <c r="Q10" s="1" t="s">
-        <v>1958</v>
+        <v>1952</v>
       </c>
       <c r="R10" s="1"/>
     </row>
     <row r="11" spans="1:18" ht="236.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>1959</v>
+        <v>1953</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>1960</v>
+        <v>1954</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>1961</v>
+        <v>1955</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1962</v>
+        <v>1956</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1">
         <v>2010</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>1904</v>
+        <v>1898</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>1963</v>
+        <v>1957</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>1964</v>
+        <v>1958</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>1937</v>
+        <v>1931</v>
       </c>
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1" t="s">
-        <v>1965</v>
+        <v>1959</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>1966</v>
+        <v>1960</v>
       </c>
       <c r="R11" s="1"/>
     </row>
     <row r="12" spans="1:18" ht="236.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>1967</v>
+        <v>1961</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1968</v>
+        <v>1962</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>1969</v>
+        <v>1963</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>1970</v>
+        <v>1964</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1">
         <v>2000</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>1904</v>
+        <v>1898</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>1971</v>
+        <v>1965</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
-        <v>1972</v>
+        <v>1966</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>1973</v>
+        <v>1967</v>
       </c>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1" t="s">
-        <v>1974</v>
+        <v>1968</v>
       </c>
       <c r="Q12" s="1" t="s">
-        <v>1975</v>
+        <v>1969</v>
       </c>
       <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:18" ht="220.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>1976</v>
+        <v>1970</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>1977</v>
+        <v>1971</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>1978</v>
+        <v>1972</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>1979</v>
+        <v>1973</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1">
         <v>1999</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>1904</v>
+        <v>1898</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>1980</v>
+        <v>1974</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>1837</v>
+        <v>1831</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>1937</v>
+        <v>1931</v>
       </c>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1" t="s">
-        <v>1981</v>
+        <v>1975</v>
       </c>
       <c r="Q13" s="1" t="s">
-        <v>1982</v>
+        <v>1976</v>
       </c>
       <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:18" ht="283.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>1983</v>
+        <v>1977</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>1984</v>
+        <v>1978</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>1985</v>
+        <v>1979</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>1986</v>
+        <v>1980</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1">
         <v>1979</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>1904</v>
+        <v>1898</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>1971</v>
+        <v>1965</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
-        <v>1987</v>
+        <v>1981</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>1988</v>
+        <v>1982</v>
       </c>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1" t="s">
-        <v>1989</v>
+        <v>1983</v>
       </c>
       <c r="Q14" s="1" t="s">
-        <v>1990</v>
+        <v>1984</v>
       </c>
       <c r="R14" s="1"/>
     </row>
@@ -19775,40 +19722,40 @@
         <v>115</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>1991</v>
+        <v>1985</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>1992</v>
+        <v>1986</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>1993</v>
+        <v>1987</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1">
         <v>2012</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>1904</v>
+        <v>1898</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>1994</v>
+        <v>1988</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
-        <v>1995</v>
+        <v>1989</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>1929</v>
+        <v>1923</v>
       </c>
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1" t="s">
-        <v>1996</v>
+        <v>1990</v>
       </c>
       <c r="Q15" s="1" t="s">
-        <v>1997</v>
+        <v>1991</v>
       </c>
       <c r="R15" s="1"/>
     </row>
@@ -19817,56 +19764,56 @@
         <v>214</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>1998</v>
+        <v>1992</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>1999</v>
+        <v>1993</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>2000</v>
+        <v>1994</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1">
         <v>2009</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>1904</v>
+        <v>1898</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>2001</v>
+        <v>1995</v>
       </c>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
       <c r="K16" s="1" t="s">
-        <v>2002</v>
+        <v>1996</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>2003</v>
+        <v>1997</v>
       </c>
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1" t="s">
-        <v>2004</v>
+        <v>1998</v>
       </c>
       <c r="Q16" s="1" t="s">
-        <v>2005</v>
+        <v>1999</v>
       </c>
       <c r="R16" s="1"/>
     </row>
     <row r="17" spans="1:18" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>2006</v>
+        <v>2000</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="1" t="s">
-        <v>2007</v>
+        <v>2001</v>
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -19878,23 +19825,23 @@
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
       <c r="Q17" s="1" t="s">
-        <v>2009</v>
+        <v>2003</v>
       </c>
       <c r="R17" s="1"/>
     </row>
     <row r="18" spans="1:18" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>2010</v>
+        <v>2004</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1" t="s">
-        <v>2011</v>
+        <v>2005</v>
       </c>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1" t="s">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -19906,23 +19853,23 @@
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
       <c r="Q18" s="1" t="s">
-        <v>2012</v>
+        <v>2006</v>
       </c>
       <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:18" ht="126" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>2013</v>
+        <v>2007</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>2014</v>
+        <v>2008</v>
       </c>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1" t="s">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -19934,23 +19881,23 @@
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
       <c r="Q19" s="1" t="s">
-        <v>2015</v>
+        <v>2009</v>
       </c>
       <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:18" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="B20" s="1"/>
       <c r="C20" s="1" t="s">
-        <v>2017</v>
+        <v>2011</v>
       </c>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -19962,7 +19909,7 @@
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
       <c r="Q20" s="1" t="s">
-        <v>2018</v>
+        <v>2012</v>
       </c>
       <c r="R20" s="1"/>
     </row>
@@ -19972,13 +19919,13 @@
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="1" t="s">
-        <v>2019</v>
+        <v>2013</v>
       </c>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1" t="s">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -19990,54 +19937,54 @@
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
       <c r="Q21" s="1" t="s">
-        <v>2020</v>
+        <v>2014</v>
       </c>
       <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:18" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
-        <v>2021</v>
+        <v>2015</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>2022</v>
+        <v>2016</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>2023</v>
+        <v>2017</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>2024</v>
+        <v>2018</v>
       </c>
       <c r="F22" s="3">
         <v>2015</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="Q22" s="3" t="s">
-        <v>2025</v>
+        <v>2019</v>
       </c>
     </row>
     <row r="23" spans="1:18" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
-        <v>2026</v>
+        <v>2020</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>2027</v>
+        <v>2021</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>2028</v>
+        <v>2022</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>2029</v>
+        <v>2023</v>
       </c>
       <c r="F23" s="3">
         <v>2018</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="Q23" s="3" t="s">
-        <v>2030</v>
+        <v>2024</v>
       </c>
     </row>
   </sheetData>
@@ -20065,7 +20012,7 @@
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2031</v>
+        <v>2025</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -20076,28 +20023,28 @@
         <v>31</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>2026</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2027</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2028</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>1881</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2029</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>2030</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>2031</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>2032</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>2033</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2034</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>1887</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>2035</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>2036</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>2037</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>2038</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>44</v>
@@ -20125,7 +20072,7 @@
   <sheetData>
     <row r="1" spans="1:17" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>2039</v>
+        <v>2033</v>
       </c>
     </row>
     <row r="2" spans="1:17" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -20139,25 +20086,25 @@
         <v>110</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>2034</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>2035</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>2036</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>2037</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>2038</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>2039</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>2040</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>2041</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>2042</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>2043</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>2044</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>2045</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>2046</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>44</v>
@@ -20175,10 +20122,10 @@
         <v>53</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>1875</v>
+        <v>1869</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>1876</v>
+        <v>1870</v>
       </c>
     </row>
   </sheetData>
@@ -20190,7 +20137,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20673,10 +20622,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="880" topLeftCell="A54" activePane="bottomLeft"/>
-      <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="F62" sqref="F62"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="880" topLeftCell="A3" activePane="bottomLeft"/>
+      <selection activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20761,14 +20710,14 @@
         <v>112</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>2048</v>
+        <v>2042</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>2049</v>
+        <v>2043</v>
       </c>
       <c r="E4" s="19"/>
       <c r="F4" s="19" t="s">
-        <v>2050</v>
+        <v>2044</v>
       </c>
       <c r="G4" s="37">
         <v>135.13</v>
@@ -20852,7 +20801,7 @@
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>2051</v>
+        <v>2045</v>
       </c>
       <c r="G7" s="38">
         <v>427.2</v>
@@ -20880,7 +20829,7 @@
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="25" t="s">
-        <v>2052</v>
+        <v>2046</v>
       </c>
       <c r="G8" s="38">
         <v>89.09</v>
@@ -20908,7 +20857,7 @@
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="25" t="s">
-        <v>2053</v>
+        <v>2047</v>
       </c>
       <c r="G9" s="38">
         <v>160.16999999999999</v>
@@ -20940,7 +20889,7 @@
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="25" t="s">
-        <v>2054</v>
+        <v>2048</v>
       </c>
       <c r="G10" s="38">
         <v>347.22</v>
@@ -21020,7 +20969,7 @@
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="25" t="s">
-        <v>2055</v>
+        <v>2049</v>
       </c>
       <c r="G13" s="38">
         <v>174.2</v>
@@ -21048,7 +20997,7 @@
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="25" t="s">
-        <v>2056</v>
+        <v>2050</v>
       </c>
       <c r="G14" s="38">
         <v>330.39</v>
@@ -21080,7 +21029,7 @@
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="25" t="s">
-        <v>2057</v>
+        <v>2051</v>
       </c>
       <c r="G15" s="38">
         <v>133.1</v>
@@ -21108,7 +21057,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="25" t="s">
-        <v>2058</v>
+        <v>2052</v>
       </c>
       <c r="G16" s="38">
         <v>246.22</v>
@@ -21138,7 +21087,7 @@
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="25" t="s">
-        <v>2059</v>
+        <v>2053</v>
       </c>
       <c r="G17" s="38">
         <v>132.12</v>
@@ -21166,7 +21115,7 @@
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="25" t="s">
-        <v>2060</v>
+        <v>2054</v>
       </c>
       <c r="G18" s="38">
         <v>248.19</v>
@@ -21198,7 +21147,7 @@
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="25" t="s">
-        <v>2061</v>
+        <v>2055</v>
       </c>
       <c r="G19" s="38">
         <v>507.18</v>
@@ -21226,7 +21175,7 @@
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="25" t="s">
-        <v>2062</v>
+        <v>2056</v>
       </c>
       <c r="G20" s="38">
         <v>403.18</v>
@@ -21306,7 +21255,7 @@
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="25" t="s">
-        <v>2063</v>
+        <v>2057</v>
       </c>
       <c r="G23" s="38">
         <v>323.2</v>
@@ -21366,7 +21315,7 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="25" t="s">
-        <v>2064</v>
+        <v>2058</v>
       </c>
       <c r="G25" s="38">
         <v>483.16</v>
@@ -21394,7 +21343,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="25" t="s">
-        <v>2065</v>
+        <v>2059</v>
       </c>
       <c r="G26" s="38">
         <v>121.16</v>
@@ -21422,7 +21371,7 @@
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="25" t="s">
-        <v>2066</v>
+        <v>2060</v>
       </c>
       <c r="G27" s="38">
         <v>224.3</v>
@@ -21454,7 +21403,7 @@
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="25" t="s">
-        <v>2067</v>
+        <v>2061</v>
       </c>
       <c r="G28" s="38">
         <v>243.22</v>
@@ -21484,7 +21433,7 @@
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="25" t="s">
-        <v>2068</v>
+        <v>2062</v>
       </c>
       <c r="G29" s="38">
         <v>266.04000000000002</v>
@@ -21512,7 +21461,7 @@
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="25" t="s">
-        <v>2069</v>
+        <v>2063</v>
       </c>
       <c r="G30" s="38">
         <v>200.08</v>
@@ -21592,7 +21541,7 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="25" t="s">
-        <v>2070</v>
+        <v>2064</v>
       </c>
       <c r="G33" s="38">
         <v>260.14</v>
@@ -21672,7 +21621,7 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="25" t="s">
-        <v>2071</v>
+        <v>2065</v>
       </c>
       <c r="G36" s="38">
         <v>340.12</v>
@@ -21700,7 +21649,7 @@
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="25" t="s">
-        <v>2072</v>
+        <v>2066</v>
       </c>
       <c r="G37" s="38">
         <v>186.06</v>
@@ -21728,7 +21677,7 @@
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="25" t="s">
-        <v>2072</v>
+        <v>2066</v>
       </c>
       <c r="G38" s="38">
         <v>186.06</v>
@@ -21756,7 +21705,7 @@
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="25" t="s">
-        <v>2073</v>
+        <v>2067</v>
       </c>
       <c r="G39" s="38">
         <v>422.28</v>
@@ -21836,7 +21785,7 @@
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1" t="s">
-        <v>2074</v>
+        <v>2068</v>
       </c>
       <c r="G42" s="38">
         <v>443.2</v>
@@ -21916,7 +21865,7 @@
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="25" t="s">
-        <v>2075</v>
+        <v>2069</v>
       </c>
       <c r="G45" s="38">
         <v>180.16</v>
@@ -21948,7 +21897,7 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="25" t="s">
-        <v>2076</v>
+        <v>2070</v>
       </c>
       <c r="G46" s="38">
         <v>146.13999999999999</v>
@@ -21976,7 +21925,7 @@
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="25" t="s">
-        <v>2077</v>
+        <v>2071</v>
       </c>
       <c r="G47" s="38">
         <v>274.27</v>
@@ -22008,7 +21957,7 @@
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="25" t="s">
-        <v>2078</v>
+        <v>2072</v>
       </c>
       <c r="G48" s="38">
         <v>147.13</v>
@@ -22036,7 +21985,7 @@
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="25" t="s">
-        <v>2079</v>
+        <v>2073</v>
       </c>
       <c r="G49" s="38">
         <v>276.24</v>
@@ -22068,7 +22017,7 @@
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="25" t="s">
-        <v>2080</v>
+        <v>2074</v>
       </c>
       <c r="G50" s="38">
         <v>75.069999999999993</v>
@@ -22126,7 +22075,7 @@
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="25" t="s">
-        <v>2081</v>
+        <v>2075</v>
       </c>
       <c r="G52" s="38">
         <v>363.22</v>
@@ -22154,7 +22103,7 @@
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="25" t="s">
-        <v>2082</v>
+        <v>2076</v>
       </c>
       <c r="G53" s="38">
         <v>151.13</v>
@@ -22186,7 +22135,7 @@
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="25" t="s">
-        <v>2083</v>
+        <v>2077</v>
       </c>
       <c r="G54" s="38">
         <v>523.17899999999997</v>
@@ -22276,7 +22225,7 @@
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="25" t="s">
-        <v>2084</v>
+        <v>2078</v>
       </c>
       <c r="G57" s="38">
         <v>155.15</v>
@@ -22304,7 +22253,7 @@
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="25" t="s">
-        <v>2085</v>
+        <v>2079</v>
       </c>
       <c r="G58" s="38">
         <v>292.29000000000002</v>
@@ -22388,7 +22337,7 @@
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1" t="s">
-        <v>2086</v>
+        <v>2080</v>
       </c>
       <c r="G61" s="38">
         <v>131.16999999999999</v>
@@ -27376,8 +27325,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L128"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
replace (K_m_trl * Avogadro * volume_c + min_AAs) in RLs with translation_denom_const func.
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -9,7 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="460" windowWidth="25000" windowHeight="20600" tabRatio="500" firstSheet="1" activeTab="10"/>
+    <workbookView xWindow="2560" yWindow="460" windowWidth="25000" windowHeight="20600" tabRatio="500" firstSheet="2" activeTab="12"/>
+    <workbookView xWindow="-18980" yWindow="860" windowWidth="18400" windowHeight="19880" tabRatio="500" firstSheet="11" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -425,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4708" uniqueCount="2083">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4711" uniqueCount="2085">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -6588,94 +6589,100 @@
     <t>min_AAs</t>
   </si>
   <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Adk_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Apt_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Cmk_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Eno_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Fba_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Gap_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Gk_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Hpt_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * LacA_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Ldh_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Nox_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * PeptAbcTransporter_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Pfk_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * PgiB_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Pgk_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Pgm_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * PiAbcTransporter_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Ppa_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Prs_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Pts_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Pyk_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * PyrH_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Ribosome_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * RnaPolymerase_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Rnase_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Rpe_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Tim_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * TklB_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Udk_Rna[c] * Ribosome_Protein[c]</t>
-  </si>
-  <si>
-    <t>k_cat_trl * min_AAs / (K_m_trl * Avogadro * volume_c + min_AAs) * Upp_Rna[c] * Ribosome_Protein[c]</t>
+    <t>K_m_trl * Avogadro * volume_c + min_AAs</t>
+  </si>
+  <si>
+    <t>translation_denom_const</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Adk_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Apt_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Cmk_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Eno_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Fba_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Gap_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Gk_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Hpt_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * LacA_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Ldh_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Nox_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * PeptAbcTransporter_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Pfk_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * PgiB_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Pgk_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Pgm_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * PiAbcTransporter_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Ppa_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Prs_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Pts_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Pyk_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * PyrH_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Ribosome_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * RnaPolymerase_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Rnase_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Rpe_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Tim_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * TklB_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Udk_Rna[c] * Ribosome_Protein[c]</t>
+  </si>
+  <si>
+    <t>k_cat_trl * min_AAs / translation_denom_const * Upp_Rna[c] * Ribosome_Protein[c]</t>
   </si>
 </sst>
 </file>
@@ -7314,6 +7321,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" customHeight="1" zeroHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7587,6 +7595,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7706,15 +7715,16 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.5" style="3" customWidth="1"/>
+    <col min="1" max="1" width="24.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="8.6640625" style="3" customWidth="1"/>
     <col min="3" max="3" width="79.1640625" style="3" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" style="3" customWidth="1"/>
@@ -7801,7 +7811,7 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>723</v>
       </c>
@@ -7812,7 +7822,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>725</v>
       </c>
@@ -7831,6 +7841,17 @@
         <v>2051</v>
       </c>
       <c r="D8" s="25" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>2054</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2053</v>
+      </c>
+      <c r="D9" s="25" t="s">
         <v>403</v>
       </c>
     </row>
@@ -7854,6 +7875,7 @@
       <selection activeCell="A3" sqref="A3"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12796,9 +12818,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L169"/>
   <sheetViews>
-    <sheetView topLeftCell="A124" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <selection activeCell="F160" sqref="F160"/>
+    <sheetView tabSelected="1" topLeftCell="A124" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <selection activeCell="F131" sqref="F131"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15053,7 +15076,7 @@
         <v>1268</v>
       </c>
       <c r="F131" s="1" t="s">
-        <v>2053</v>
+        <v>2055</v>
       </c>
       <c r="G131" s="1" t="s">
         <v>738</v>
@@ -15070,7 +15093,7 @@
         <v>1268</v>
       </c>
       <c r="F132" s="1" t="s">
-        <v>2054</v>
+        <v>2056</v>
       </c>
       <c r="G132" s="1" t="s">
         <v>738</v>
@@ -15087,7 +15110,7 @@
         <v>1268</v>
       </c>
       <c r="F133" s="1" t="s">
-        <v>2055</v>
+        <v>2057</v>
       </c>
       <c r="G133" s="1" t="s">
         <v>738</v>
@@ -15104,7 +15127,7 @@
         <v>1268</v>
       </c>
       <c r="F134" s="1" t="s">
-        <v>2056</v>
+        <v>2058</v>
       </c>
       <c r="G134" s="1" t="s">
         <v>738</v>
@@ -15121,7 +15144,7 @@
         <v>1268</v>
       </c>
       <c r="F135" s="1" t="s">
-        <v>2057</v>
+        <v>2059</v>
       </c>
       <c r="G135" s="1" t="s">
         <v>738</v>
@@ -15138,7 +15161,7 @@
         <v>1268</v>
       </c>
       <c r="F136" s="1" t="s">
-        <v>2058</v>
+        <v>2060</v>
       </c>
       <c r="G136" s="1" t="s">
         <v>738</v>
@@ -15155,7 +15178,7 @@
         <v>1268</v>
       </c>
       <c r="F137" s="1" t="s">
-        <v>2059</v>
+        <v>2061</v>
       </c>
       <c r="G137" s="1" t="s">
         <v>738</v>
@@ -15172,7 +15195,7 @@
         <v>1268</v>
       </c>
       <c r="F138" s="1" t="s">
-        <v>2060</v>
+        <v>2062</v>
       </c>
       <c r="G138" s="1" t="s">
         <v>738</v>
@@ -15189,7 +15212,7 @@
         <v>1268</v>
       </c>
       <c r="F139" s="1" t="s">
-        <v>2061</v>
+        <v>2063</v>
       </c>
       <c r="G139" s="1" t="s">
         <v>738</v>
@@ -15206,7 +15229,7 @@
         <v>1268</v>
       </c>
       <c r="F140" s="1" t="s">
-        <v>2062</v>
+        <v>2064</v>
       </c>
       <c r="G140" s="1" t="s">
         <v>738</v>
@@ -15223,7 +15246,7 @@
         <v>1268</v>
       </c>
       <c r="F141" s="1" t="s">
-        <v>2063</v>
+        <v>2065</v>
       </c>
       <c r="G141" s="1" t="s">
         <v>738</v>
@@ -15240,7 +15263,7 @@
         <v>1268</v>
       </c>
       <c r="F142" s="1" t="s">
-        <v>2064</v>
+        <v>2066</v>
       </c>
       <c r="G142" s="1" t="s">
         <v>738</v>
@@ -15257,7 +15280,7 @@
         <v>1268</v>
       </c>
       <c r="F143" s="1" t="s">
-        <v>2065</v>
+        <v>2067</v>
       </c>
       <c r="G143" s="1" t="s">
         <v>738</v>
@@ -15274,7 +15297,7 @@
         <v>1268</v>
       </c>
       <c r="F144" s="1" t="s">
-        <v>2066</v>
+        <v>2068</v>
       </c>
       <c r="G144" s="1" t="s">
         <v>738</v>
@@ -15291,7 +15314,7 @@
         <v>1268</v>
       </c>
       <c r="F145" s="1" t="s">
-        <v>2067</v>
+        <v>2069</v>
       </c>
       <c r="G145" s="1" t="s">
         <v>738</v>
@@ -15308,7 +15331,7 @@
         <v>1268</v>
       </c>
       <c r="F146" s="1" t="s">
-        <v>2068</v>
+        <v>2070</v>
       </c>
       <c r="G146" s="1" t="s">
         <v>738</v>
@@ -15325,7 +15348,7 @@
         <v>1268</v>
       </c>
       <c r="F147" s="1" t="s">
-        <v>2069</v>
+        <v>2071</v>
       </c>
       <c r="G147" s="1" t="s">
         <v>738</v>
@@ -15342,7 +15365,7 @@
         <v>1268</v>
       </c>
       <c r="F148" s="1" t="s">
-        <v>2070</v>
+        <v>2072</v>
       </c>
       <c r="G148" s="1" t="s">
         <v>738</v>
@@ -15359,7 +15382,7 @@
         <v>1268</v>
       </c>
       <c r="F149" s="1" t="s">
-        <v>2071</v>
+        <v>2073</v>
       </c>
       <c r="G149" s="1" t="s">
         <v>738</v>
@@ -15376,7 +15399,7 @@
         <v>1268</v>
       </c>
       <c r="F150" s="1" t="s">
-        <v>2072</v>
+        <v>2074</v>
       </c>
       <c r="G150" s="1" t="s">
         <v>738</v>
@@ -15393,7 +15416,7 @@
         <v>1268</v>
       </c>
       <c r="F151" s="1" t="s">
-        <v>2073</v>
+        <v>2075</v>
       </c>
       <c r="G151" s="1" t="s">
         <v>738</v>
@@ -15410,7 +15433,7 @@
         <v>1268</v>
       </c>
       <c r="F152" s="1" t="s">
-        <v>2074</v>
+        <v>2076</v>
       </c>
       <c r="G152" s="1" t="s">
         <v>738</v>
@@ -15427,7 +15450,7 @@
         <v>1268</v>
       </c>
       <c r="F153" s="1" t="s">
-        <v>2075</v>
+        <v>2077</v>
       </c>
       <c r="G153" s="1" t="s">
         <v>738</v>
@@ -15444,7 +15467,7 @@
         <v>1268</v>
       </c>
       <c r="F154" s="1" t="s">
-        <v>2076</v>
+        <v>2078</v>
       </c>
       <c r="G154" s="1" t="s">
         <v>738</v>
@@ -15461,7 +15484,7 @@
         <v>1268</v>
       </c>
       <c r="F155" s="1" t="s">
-        <v>2077</v>
+        <v>2079</v>
       </c>
       <c r="G155" s="1" t="s">
         <v>738</v>
@@ -15478,7 +15501,7 @@
         <v>1268</v>
       </c>
       <c r="F156" s="1" t="s">
-        <v>2078</v>
+        <v>2080</v>
       </c>
       <c r="G156" s="1" t="s">
         <v>738</v>
@@ -15495,7 +15518,7 @@
         <v>1268</v>
       </c>
       <c r="F157" s="1" t="s">
-        <v>2079</v>
+        <v>2081</v>
       </c>
       <c r="G157" s="1" t="s">
         <v>738</v>
@@ -15512,7 +15535,7 @@
         <v>1268</v>
       </c>
       <c r="F158" s="1" t="s">
-        <v>2080</v>
+        <v>2082</v>
       </c>
       <c r="G158" s="1" t="s">
         <v>738</v>
@@ -15529,7 +15552,7 @@
         <v>1268</v>
       </c>
       <c r="F159" s="1" t="s">
-        <v>2081</v>
+        <v>2083</v>
       </c>
       <c r="G159" s="1" t="s">
         <v>738</v>
@@ -15546,7 +15569,7 @@
         <v>1268</v>
       </c>
       <c r="F160" s="1" t="s">
-        <v>2082</v>
+        <v>2084</v>
       </c>
       <c r="G160" s="1" t="s">
         <v>738</v>
@@ -15717,6 +15740,7 @@
   <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15807,6 +15831,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -15905,6 +15930,7 @@
   <dimension ref="A1:K37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16678,6 +16704,11 @@
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A66" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A96" sqref="A96:XFD97"/>
+    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="1">
+      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="F89" sqref="F89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18447,6 +18478,7 @@
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="A3" sqref="A3:XFD4"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18507,6 +18539,7 @@
   <dimension ref="A1:W11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18819,6 +18852,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18931,6 +18965,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19020,6 +19055,7 @@
   <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19174,6 +19210,7 @@
   <dimension ref="A1:R23"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20020,6 +20057,7 @@
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20080,6 +20118,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20157,6 +20196,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20222,6 +20262,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20292,6 +20333,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20411,6 +20453,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20644,6 +20687,7 @@
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -24658,6 +24702,7 @@
   <dimension ref="A1:J177"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -27346,6 +27391,7 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
replace transcription rate expressions k_cat_trn * min_NTPs / (K_m_trn * Avogadro * volume_c + min_NTPs) * RnaPolymerase_Protein[c] with trans_rate_func function
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4711" uniqueCount="2086">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4714" uniqueCount="2087">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -6686,6 +6686,9 @@
   </si>
   <si>
     <t>k_cat_rna_deg * Upp_Rna[c] / (Upp_Rna[c] + RNA_deg_const) * Rnase_Protein[c]</t>
+  </si>
+  <si>
+    <t>trans_rate_func</t>
   </si>
 </sst>
 </file>
@@ -7732,10 +7735,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <selection activeCell="C9" sqref="C9"/>
@@ -7866,6 +7869,17 @@
       </c>
       <c r="D9" s="26" t="s">
         <v>403</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>2086</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>2047</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>732</v>
       </c>
     </row>
   </sheetData>
@@ -12834,12 +12848,12 @@
   <dimension ref="A1:L169"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="880" topLeftCell="A60" activePane="bottomLeft"/>
+      <pane ySplit="880" topLeftCell="A84" activePane="bottomLeft"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="F88" sqref="F88"/>
+      <selection pane="bottomLeft" activeCell="F130" sqref="F130"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="1">
-      <selection activeCell="F77" sqref="F77"/>
+    <sheetView tabSelected="1" topLeftCell="A59" workbookViewId="1">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -14589,7 +14603,7 @@
         <v>1261</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G101" s="1" t="s">
         <v>732</v>
@@ -14606,7 +14620,7 @@
         <v>1261</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G102" s="1" t="s">
         <v>732</v>
@@ -14623,7 +14637,7 @@
         <v>1261</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G103" s="1" t="s">
         <v>732</v>
@@ -14640,7 +14654,7 @@
         <v>1261</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G104" s="1" t="s">
         <v>732</v>
@@ -14657,7 +14671,7 @@
         <v>1261</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G105" s="1" t="s">
         <v>732</v>
@@ -14674,7 +14688,7 @@
         <v>1261</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G106" s="1" t="s">
         <v>732</v>
@@ -14691,7 +14705,7 @@
         <v>1261</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G107" s="1" t="s">
         <v>732</v>
@@ -14708,7 +14722,7 @@
         <v>1261</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G108" s="1" t="s">
         <v>732</v>
@@ -14725,7 +14739,7 @@
         <v>1261</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G109" s="1" t="s">
         <v>732</v>
@@ -14742,7 +14756,7 @@
         <v>1261</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G110" s="1" t="s">
         <v>732</v>
@@ -14759,7 +14773,7 @@
         <v>1261</v>
       </c>
       <c r="F111" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G111" s="1" t="s">
         <v>732</v>
@@ -14776,7 +14790,7 @@
         <v>1261</v>
       </c>
       <c r="F112" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G112" s="1" t="s">
         <v>732</v>
@@ -14793,7 +14807,7 @@
         <v>1261</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G113" s="1" t="s">
         <v>732</v>
@@ -14810,7 +14824,7 @@
         <v>1261</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G114" s="1" t="s">
         <v>732</v>
@@ -14827,7 +14841,7 @@
         <v>1261</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G115" s="1" t="s">
         <v>732</v>
@@ -14844,7 +14858,7 @@
         <v>1261</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G116" s="1" t="s">
         <v>732</v>
@@ -14861,7 +14875,7 @@
         <v>1261</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G117" s="1" t="s">
         <v>732</v>
@@ -14878,7 +14892,7 @@
         <v>1261</v>
       </c>
       <c r="F118" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G118" s="1" t="s">
         <v>732</v>
@@ -14895,7 +14909,7 @@
         <v>1261</v>
       </c>
       <c r="F119" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G119" s="1" t="s">
         <v>732</v>
@@ -14912,7 +14926,7 @@
         <v>1261</v>
       </c>
       <c r="F120" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G120" s="1" t="s">
         <v>732</v>
@@ -14929,7 +14943,7 @@
         <v>1261</v>
       </c>
       <c r="F121" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G121" s="1" t="s">
         <v>732</v>
@@ -14946,7 +14960,7 @@
         <v>1261</v>
       </c>
       <c r="F122" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G122" s="1" t="s">
         <v>732</v>
@@ -14963,7 +14977,7 @@
         <v>1261</v>
       </c>
       <c r="F123" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G123" s="1" t="s">
         <v>732</v>
@@ -14980,7 +14994,7 @@
         <v>1261</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G124" s="1" t="s">
         <v>732</v>
@@ -14997,7 +15011,7 @@
         <v>1261</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G125" s="1" t="s">
         <v>732</v>
@@ -15014,7 +15028,7 @@
         <v>1261</v>
       </c>
       <c r="F126" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G126" s="1" t="s">
         <v>732</v>
@@ -15031,7 +15045,7 @@
         <v>1261</v>
       </c>
       <c r="F127" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G127" s="1" t="s">
         <v>732</v>
@@ -15048,7 +15062,7 @@
         <v>1261</v>
       </c>
       <c r="F128" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G128" s="1" t="s">
         <v>732</v>
@@ -15065,7 +15079,7 @@
         <v>1261</v>
       </c>
       <c r="F129" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G129" s="1" t="s">
         <v>732</v>
@@ -15082,7 +15096,7 @@
         <v>1261</v>
       </c>
       <c r="F130" s="1" t="s">
-        <v>2047</v>
+        <v>2086</v>
       </c>
       <c r="G130" s="1" t="s">
         <v>732</v>

</xml_diff>

<commit_message>
provide more species type structures
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2560" yWindow="460" windowWidth="25000" windowHeight="20600" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="-27180" yWindow="460" windowWidth="25000" windowHeight="20600" tabRatio="500" activeTab="6"/>
     <workbookView xWindow="-20300" yWindow="460" windowWidth="20300" windowHeight="20120" tabRatio="500" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4715" uniqueCount="2087">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4719" uniqueCount="2090">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -6689,6 +6689,15 @@
   </si>
   <si>
     <t>Best PubChem match: called Alpha-D-glucose 6-phosphate</t>
+  </si>
+  <si>
+    <t>C3H6O3</t>
+  </si>
+  <si>
+    <t>C21H28N7O14P2</t>
+  </si>
+  <si>
+    <t>C21H29N7O14P2</t>
   </si>
 </sst>
 </file>
@@ -7897,10 +7906,10 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:N178"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <pane ySplit="740" topLeftCell="A118" activePane="bottomLeft"/>
+    <sheetView topLeftCell="B3" workbookViewId="0">
+      <pane ySplit="740" topLeftCell="A123" activePane="bottomLeft"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="A159" sqref="A159"/>
+      <selection pane="bottomLeft" activeCell="B151" sqref="B151"/>
     </sheetView>
     <sheetView topLeftCell="A113" workbookViewId="1">
       <selection activeCell="A159" sqref="A159:XFD159"/>
@@ -12848,9 +12857,9 @@
   <dimension ref="A1:L169"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="880" topLeftCell="A2" activePane="bottomLeft"/>
+      <pane ySplit="880" topLeftCell="A143" activePane="bottomLeft"/>
       <selection activeCell="B2" sqref="B1:B1048576"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B1:B1048576"/>
+      <selection pane="bottomLeft" activeCell="A158" sqref="A158"/>
     </sheetView>
     <sheetView topLeftCell="A122" workbookViewId="1">
       <selection activeCell="F131" sqref="F131"/>
@@ -19232,7 +19241,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R23"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -20708,12 +20719,13 @@
   <dimension ref="A1:N146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="880" topLeftCell="A3" activePane="bottomLeft"/>
-      <selection activeCell="E1" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="M39" sqref="M39"/>
+      <pane ySplit="1600" topLeftCell="A4" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="1">
-      <selection activeCell="A39" sqref="A39:F39"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="1">
+      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -22484,9 +22496,11 @@
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
-      <c r="F63" s="1"/>
+      <c r="F63" s="26" t="s">
+        <v>2087</v>
+      </c>
       <c r="G63" s="39">
-        <v>10</v>
+        <v>90.08</v>
       </c>
       <c r="H63" s="22">
         <v>0</v>
@@ -22782,9 +22796,11 @@
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
-      <c r="F74" s="1"/>
+      <c r="F74" s="26" t="s">
+        <v>2088</v>
+      </c>
       <c r="G74" s="39">
-        <v>10</v>
+        <v>664.4</v>
       </c>
       <c r="H74" s="22">
         <v>0</v>
@@ -22812,9 +22828,11 @@
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="1"/>
+      <c r="F75" s="26" t="s">
+        <v>2089</v>
+      </c>
       <c r="G75" s="39">
-        <v>10</v>
+        <v>665.4</v>
       </c>
       <c r="H75" s="22">
         <v>0</v>
@@ -22890,9 +22908,11 @@
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
+      <c r="F78" s="1" t="s">
+        <v>261</v>
+      </c>
       <c r="G78" s="39">
-        <v>10</v>
+        <v>31.998999999999999</v>
       </c>
       <c r="H78" s="22">
         <v>0</v>
@@ -24730,10 +24750,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="C95" sqref="C95"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <pane ySplit="1040" topLeftCell="A57" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -27419,8 +27442,8 @@
   <dimension ref="A1:L128"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <pane ySplit="2" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <pane ySplit="1300" topLeftCell="A88" activePane="bottomLeft"/>

</xml_diff>

<commit_message>
add approximate MWs for all proteins
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-27180" yWindow="460" windowWidth="25000" windowHeight="20600" tabRatio="500" activeTab="6"/>
-    <workbookView xWindow="-20300" yWindow="460" windowWidth="20300" windowHeight="20120" tabRatio="500" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="-27900" yWindow="640" windowWidth="25500" windowHeight="19940" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="35320" windowHeight="19700" tabRatio="500" firstSheet="11" activeTab="21"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4719" uniqueCount="2090">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4787" uniqueCount="2098">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -6698,6 +6698,30 @@
   </si>
   <si>
     <t>C21H29N7O14P2</t>
+  </si>
+  <si>
+    <t>Approx. MW of M. pneumoniae proteins</t>
+  </si>
+  <si>
+    <t>Ref_0022</t>
+  </si>
+  <si>
+    <t>himmelreich1996complete</t>
+  </si>
+  <si>
+    <t>Complete sequence analysis of the genome of the bacterium Mycoplasma pneumoniae</t>
+  </si>
+  <si>
+    <t>Nucleic acids research</t>
+  </si>
+  <si>
+    <t>Oxford University Press</t>
+  </si>
+  <si>
+    <t>Himmelreich, et al.</t>
+  </si>
+  <si>
+    <t>URL: https://academic.oup.com/nar/article-pdf/24/22/4420/7069676/24-22-4420.pdf</t>
   </si>
 </sst>
 </file>
@@ -6707,7 +6731,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -6767,6 +6791,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -6803,11 +6833,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -6925,9 +6957,14 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7622,9 +7659,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7749,9 +7784,7 @@
     <sheetView workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -7907,13 +7940,11 @@
   <dimension ref="A1:N178"/>
   <sheetViews>
     <sheetView topLeftCell="B3" workbookViewId="0">
-      <pane ySplit="740" topLeftCell="A123" activePane="bottomLeft"/>
+      <pane ySplit="740" topLeftCell="A41" activePane="bottomLeft"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="B151" sqref="B151"/>
+      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
     </sheetView>
-    <sheetView topLeftCell="A113" workbookViewId="1">
-      <selection activeCell="A159" sqref="A159:XFD159"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -12861,9 +12892,7 @@
       <selection activeCell="B2" sqref="B1:B1048576"/>
       <selection pane="bottomLeft" activeCell="A158" sqref="A158"/>
     </sheetView>
-    <sheetView topLeftCell="A122" workbookViewId="1">
-      <selection activeCell="F131" sqref="F131"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16751,11 +16780,7 @@
       <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A65" sqref="A65:XFD65"/>
     </sheetView>
-    <sheetView topLeftCell="A2" workbookViewId="1">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B2" sqref="B2"/>
-      <selection pane="bottomLeft" activeCell="A94" sqref="A94"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -19239,18 +19264,34 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R23"/>
+  <dimension ref="A1:R24"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C30" sqref="C30:C43"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="6" width="8.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="19.1640625" style="3" customWidth="1"/>
-    <col min="8" max="18" width="8.6640625" style="3" customWidth="1"/>
+    <col min="1" max="1" width="12.33203125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="15.6640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="49.33203125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="5.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="26.83203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" style="3" customWidth="1"/>
+    <col min="11" max="11" width="4.1640625" style="3" customWidth="1"/>
+    <col min="12" max="12" width="7.33203125" style="3" customWidth="1"/>
+    <col min="13" max="15" width="8.6640625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="8.1640625" style="3" customWidth="1"/>
+    <col min="17" max="17" width="46.5" style="3" customWidth="1"/>
+    <col min="18" max="18" width="8.6640625" style="3" customWidth="1"/>
     <col min="19" max="1025" width="8.6640625" style="4" customWidth="1"/>
     <col min="1026" max="1026" width="9" style="4" customWidth="1"/>
     <col min="1027" max="16384" width="9" style="4"/>
@@ -19261,7 +19302,7 @@
         <v>1809</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="31.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:18" ht="42" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -19317,7 +19358,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:18" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>1823</v>
       </c>
@@ -19359,7 +19400,7 @@
       </c>
       <c r="R3" s="1"/>
     </row>
-    <row r="4" spans="1:18" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:18" ht="28" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>1831</v>
       </c>
@@ -19397,7 +19438,7 @@
       </c>
       <c r="R4" s="1"/>
     </row>
-    <row r="5" spans="1:18" ht="299.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:18" ht="42" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>1838</v>
       </c>
@@ -19439,7 +19480,7 @@
       </c>
       <c r="R5" s="1"/>
     </row>
-    <row r="6" spans="1:18" ht="173.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:18" ht="28" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>1846</v>
       </c>
@@ -19481,7 +19522,7 @@
       </c>
       <c r="R6" s="1"/>
     </row>
-    <row r="7" spans="1:18" ht="267.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:18" ht="42" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>1855</v>
       </c>
@@ -19521,7 +19562,7 @@
       </c>
       <c r="R7" s="1"/>
     </row>
-    <row r="8" spans="1:18" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:18" ht="28" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>1601</v>
       </c>
@@ -19557,7 +19598,7 @@
       </c>
       <c r="R8" s="1"/>
     </row>
-    <row r="9" spans="1:18" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:18" ht="56" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>1613</v>
       </c>
@@ -19595,7 +19636,7 @@
       </c>
       <c r="R9" s="1"/>
     </row>
-    <row r="10" spans="1:18" ht="220.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:18" ht="28" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>1874</v>
       </c>
@@ -19637,7 +19678,7 @@
       </c>
       <c r="R10" s="1"/>
     </row>
-    <row r="11" spans="1:18" ht="236.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:18" ht="42" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>1882</v>
       </c>
@@ -19679,7 +19720,7 @@
       </c>
       <c r="R11" s="1"/>
     </row>
-    <row r="12" spans="1:18" ht="236.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:18" ht="42" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>1890</v>
       </c>
@@ -19721,7 +19762,7 @@
       </c>
       <c r="R12" s="1"/>
     </row>
-    <row r="13" spans="1:18" ht="220.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:18" ht="28" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>1899</v>
       </c>
@@ -19763,7 +19804,7 @@
       </c>
       <c r="R13" s="1"/>
     </row>
-    <row r="14" spans="1:18" ht="283.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:18" ht="42" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>1906</v>
       </c>
@@ -19805,7 +19846,7 @@
       </c>
       <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:18" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:18" ht="28" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>114</v>
       </c>
@@ -19847,7 +19888,7 @@
       </c>
       <c r="R15" s="1"/>
     </row>
-    <row r="16" spans="1:18" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:18" ht="28" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>213</v>
       </c>
@@ -19889,7 +19930,7 @@
       </c>
       <c r="R16" s="1"/>
     </row>
-    <row r="17" spans="1:18" ht="141.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:18" ht="42" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>1929</v>
       </c>
@@ -19917,7 +19958,7 @@
       </c>
       <c r="R17" s="1"/>
     </row>
-    <row r="18" spans="1:18" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:18" ht="42" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>1933</v>
       </c>
@@ -19945,7 +19986,7 @@
       </c>
       <c r="R18" s="1"/>
     </row>
-    <row r="19" spans="1:18" ht="126" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:18" ht="42" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>1936</v>
       </c>
@@ -19973,7 +20014,7 @@
       </c>
       <c r="R19" s="1"/>
     </row>
-    <row r="20" spans="1:18" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:18" ht="42" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>1939</v>
       </c>
@@ -20001,7 +20042,7 @@
       </c>
       <c r="R20" s="1"/>
     </row>
-    <row r="21" spans="1:18" ht="63" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>154</v>
       </c>
@@ -20029,7 +20070,7 @@
       </c>
       <c r="R21" s="1"/>
     </row>
-    <row r="22" spans="1:18" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:18" ht="29" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>1944</v>
       </c>
@@ -20052,7 +20093,7 @@
         <v>1948</v>
       </c>
     </row>
-    <row r="23" spans="1:18" ht="78.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>1949</v>
       </c>
@@ -20073,6 +20114,43 @@
       </c>
       <c r="Q23" s="3" t="s">
         <v>1953</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" ht="43" x14ac:dyDescent="0.2">
+      <c r="A24" s="25" t="s">
+        <v>2091</v>
+      </c>
+      <c r="B24" s="25" t="s">
+        <v>2092</v>
+      </c>
+      <c r="C24" s="25" t="s">
+        <v>2093</v>
+      </c>
+      <c r="D24" s="25" t="s">
+        <v>2096</v>
+      </c>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25">
+        <v>1996</v>
+      </c>
+      <c r="G24" s="25" t="s">
+        <v>1827</v>
+      </c>
+      <c r="H24" s="25" t="s">
+        <v>2094</v>
+      </c>
+      <c r="I24" s="25" t="s">
+        <v>2095</v>
+      </c>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25">
+        <v>24</v>
+      </c>
+      <c r="L24" s="25">
+        <v>22</v>
+      </c>
+      <c r="Q24" s="3" t="s">
+        <v>2097</v>
       </c>
     </row>
   </sheetData>
@@ -20367,9 +20445,7 @@
   <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C4" sqref="C4"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20719,14 +20795,10 @@
   <dimension ref="A1:N146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1600" topLeftCell="A4" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="B37" sqref="B37"/>
+      <pane ySplit="1600" topLeftCell="A84" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="M116" sqref="M87:N116"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="1">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="B74" sqref="B74"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20840,23 +20912,25 @@
     </row>
     <row r="5" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="F5" s="1" t="s">
+        <v>1974</v>
+      </c>
       <c r="G5" s="39">
-        <v>10</v>
+        <v>427.2</v>
       </c>
       <c r="H5" s="22">
         <v>0</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J5" s="1"/>
       <c r="K5" s="1"/>
@@ -20866,23 +20940,25 @@
     </row>
     <row r="6" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="F6" s="1" t="s">
+        <v>1975</v>
+      </c>
       <c r="G6" s="39">
-        <v>10</v>
+        <v>89.09</v>
       </c>
       <c r="H6" s="22">
         <v>0</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -20892,19 +20968,19 @@
     </row>
     <row r="7" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>121</v>
+        <v>125</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
       <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
-        <v>1974</v>
+        <v>1976</v>
       </c>
       <c r="G7" s="39">
-        <v>427.2</v>
+        <v>160.16999999999999</v>
       </c>
       <c r="H7" s="22">
         <v>0</v>
@@ -20915,24 +20991,28 @@
       <c r="J7" s="1"/>
       <c r="K7" s="1"/>
       <c r="L7" s="1"/>
-      <c r="M7" s="1"/>
-      <c r="N7" s="1"/>
+      <c r="M7" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N7" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="8" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>122</v>
+        <v>126</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="26" t="s">
-        <v>1975</v>
+        <v>1977</v>
       </c>
       <c r="G8" s="39">
-        <v>89.09</v>
+        <v>347.22</v>
       </c>
       <c r="H8" s="22">
         <v>0</v>
@@ -20948,19 +21028,19 @@
     </row>
     <row r="9" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>132</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
       <c r="F9" s="26" t="s">
-        <v>1976</v>
+        <v>1978</v>
       </c>
       <c r="G9" s="39">
-        <v>160.16999999999999</v>
+        <v>174.2</v>
       </c>
       <c r="H9" s="22">
         <v>0</v>
@@ -20971,28 +21051,24 @@
       <c r="J9" s="1"/>
       <c r="K9" s="1"/>
       <c r="L9" s="1"/>
-      <c r="M9" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
     </row>
     <row r="10" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>126</v>
+        <v>133</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>126</v>
+        <v>134</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
       <c r="F10" s="26" t="s">
-        <v>1977</v>
+        <v>1979</v>
       </c>
       <c r="G10" s="39">
-        <v>347.22</v>
+        <v>330.39</v>
       </c>
       <c r="H10" s="22">
         <v>0</v>
@@ -21003,28 +21079,34 @@
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
       <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
-      <c r="N10" s="1"/>
+      <c r="M10" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="11" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>127</v>
+        <v>135</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>128</v>
+        <v>136</v>
       </c>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
+      <c r="F11" s="1" t="s">
+        <v>1980</v>
+      </c>
       <c r="G11" s="39">
-        <v>10</v>
+        <v>133.1</v>
       </c>
       <c r="H11" s="22">
         <v>0</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J11" s="1"/>
       <c r="K11" s="1"/>
@@ -21034,45 +21116,49 @@
     </row>
     <row r="12" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>129</v>
+        <v>137</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>130</v>
+        <v>138</v>
       </c>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
+      <c r="F12" s="1" t="s">
+        <v>1981</v>
+      </c>
       <c r="G12" s="39">
-        <v>10</v>
+        <v>246.22</v>
       </c>
       <c r="H12" s="22">
         <v>0</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1"/>
       <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
+      <c r="M12" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="N12" s="1"/>
     </row>
     <row r="13" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="26" t="s">
-        <v>1978</v>
+        <v>1982</v>
       </c>
       <c r="G13" s="39">
-        <v>174.2</v>
+        <v>132.12</v>
       </c>
       <c r="H13" s="22">
         <v>0</v>
@@ -21088,19 +21174,19 @@
     </row>
     <row r="14" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="26" t="s">
-        <v>1979</v>
+        <v>1983</v>
       </c>
       <c r="G14" s="39">
-        <v>330.39</v>
+        <v>248.19</v>
       </c>
       <c r="H14" s="22">
         <v>0</v>
@@ -21120,19 +21206,19 @@
     </row>
     <row r="15" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
       <c r="F15" s="26" t="s">
-        <v>1980</v>
+        <v>1984</v>
       </c>
       <c r="G15" s="39">
-        <v>133.1</v>
+        <v>507.18</v>
       </c>
       <c r="H15" s="22">
         <v>0</v>
@@ -21148,19 +21234,19 @@
     </row>
     <row r="16" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
-        <v>137</v>
+        <v>145</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>138</v>
+        <v>145</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" s="26" t="s">
-        <v>1981</v>
+        <v>1985</v>
       </c>
       <c r="G16" s="39">
-        <v>246.22</v>
+        <v>403.18</v>
       </c>
       <c r="H16" s="22">
         <v>0</v>
@@ -21171,26 +21257,24 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
       <c r="L16" s="1"/>
-      <c r="M16" s="1" t="s">
-        <v>139</v>
-      </c>
+      <c r="M16" s="1"/>
       <c r="N16" s="1"/>
     </row>
     <row r="17" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="26" t="s">
-        <v>1982</v>
+        <v>1986</v>
       </c>
       <c r="G17" s="39">
-        <v>132.12</v>
+        <v>323.2</v>
       </c>
       <c r="H17" s="22">
         <v>0</v>
@@ -21206,19 +21290,19 @@
     </row>
     <row r="18" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="26" t="s">
-        <v>1983</v>
+        <v>151</v>
       </c>
       <c r="G18" s="39">
-        <v>248.19</v>
+        <v>44.009</v>
       </c>
       <c r="H18" s="22">
         <v>0</v>
@@ -21230,27 +21314,27 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1" t="s">
-        <v>113</v>
+        <v>153</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>114</v>
+        <v>154</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>144</v>
+        <v>155</v>
       </c>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="26" t="s">
-        <v>1984</v>
+        <v>1987</v>
       </c>
       <c r="G19" s="39">
-        <v>507.18</v>
+        <v>483.16</v>
       </c>
       <c r="H19" s="22">
         <v>0</v>
@@ -21266,19 +21350,19 @@
     </row>
     <row r="20" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>145</v>
+        <v>156</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>145</v>
+        <v>157</v>
       </c>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
       <c r="F20" s="26" t="s">
-        <v>1985</v>
+        <v>1988</v>
       </c>
       <c r="G20" s="39">
-        <v>403.18</v>
+        <v>121.16</v>
       </c>
       <c r="H20" s="22">
         <v>0</v>
@@ -21294,71 +21378,81 @@
     </row>
     <row r="21" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
-        <v>146</v>
+        <v>158</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>147</v>
+        <v>159</v>
       </c>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
+      <c r="F21" s="1" t="s">
+        <v>1989</v>
+      </c>
       <c r="G21" s="39">
-        <v>10</v>
+        <v>224.3</v>
       </c>
       <c r="H21" s="22">
         <v>0</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J21" s="1"/>
       <c r="K21" s="1"/>
       <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
+      <c r="M21" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N21" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="22" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>148</v>
+        <v>160</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>149</v>
+        <v>161</v>
       </c>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
+      <c r="F22" s="1" t="s">
+        <v>1990</v>
+      </c>
       <c r="G22" s="39">
-        <v>10</v>
+        <v>243.22</v>
       </c>
       <c r="H22" s="22">
         <v>0</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J22" s="1"/>
       <c r="K22" s="1"/>
       <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+      <c r="M22" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="N22" s="1"/>
     </row>
     <row r="23" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
-        <v>150</v>
+        <v>162</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>150</v>
+        <v>163</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
       <c r="F23" s="26" t="s">
-        <v>1986</v>
+        <v>1991</v>
       </c>
       <c r="G23" s="39">
-        <v>323.2</v>
+        <v>266.04000000000002</v>
       </c>
       <c r="H23" s="22">
         <v>0</v>
@@ -21374,19 +21468,19 @@
     </row>
     <row r="24" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>152</v>
+        <v>165</v>
       </c>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
       <c r="F24" s="1" t="s">
-        <v>151</v>
+        <v>1992</v>
       </c>
       <c r="G24" s="39">
-        <v>44.009</v>
+        <v>200.08</v>
       </c>
       <c r="H24" s="22">
         <v>0</v>
@@ -21397,28 +21491,24 @@
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="1"/>
-      <c r="M24" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>154</v>
-      </c>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
     </row>
     <row r="25" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>155</v>
+        <v>171</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="26" t="s">
-        <v>1987</v>
+        <v>1993</v>
       </c>
       <c r="G25" s="39">
-        <v>483.16</v>
+        <v>260.14</v>
       </c>
       <c r="H25" s="22">
         <v>0</v>
@@ -21434,19 +21524,19 @@
     </row>
     <row r="26" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
-        <v>156</v>
+        <v>176</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>157</v>
+        <v>177</v>
       </c>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" s="26" t="s">
-        <v>1988</v>
+        <v>1994</v>
       </c>
       <c r="G26" s="39">
-        <v>121.16</v>
+        <v>340.12</v>
       </c>
       <c r="H26" s="22">
         <v>0</v>
@@ -21462,19 +21552,19 @@
     </row>
     <row r="27" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>158</v>
+        <v>178</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>159</v>
+        <v>179</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
       <c r="F27" s="26" t="s">
-        <v>1989</v>
+        <v>1995</v>
       </c>
       <c r="G27" s="39">
-        <v>224.3</v>
+        <v>186.06</v>
       </c>
       <c r="H27" s="22">
         <v>0</v>
@@ -21485,28 +21575,24 @@
       <c r="J27" s="1"/>
       <c r="K27" s="1"/>
       <c r="L27" s="1"/>
-      <c r="M27" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N27" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
     </row>
     <row r="28" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
-        <v>160</v>
+        <v>180</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>161</v>
+        <v>181</v>
       </c>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
       <c r="F28" s="26" t="s">
-        <v>1990</v>
+        <v>1995</v>
       </c>
       <c r="G28" s="39">
-        <v>243.22</v>
+        <v>186.06</v>
       </c>
       <c r="H28" s="22">
         <v>0</v>
@@ -21517,26 +21603,24 @@
       <c r="J28" s="1"/>
       <c r="K28" s="1"/>
       <c r="L28" s="1"/>
-      <c r="M28" s="1" t="s">
-        <v>139</v>
-      </c>
+      <c r="M28" s="1"/>
       <c r="N28" s="1"/>
     </row>
     <row r="29" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
-        <v>162</v>
+        <v>182</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>163</v>
+        <v>183</v>
       </c>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
       <c r="F29" s="26" t="s">
-        <v>1991</v>
+        <v>1993</v>
       </c>
       <c r="G29" s="39">
-        <v>266.04000000000002</v>
+        <v>260.14</v>
       </c>
       <c r="H29" s="22">
         <v>0</v>
@@ -21547,24 +21631,26 @@
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
       <c r="L29" s="1"/>
-      <c r="M29" s="1"/>
+      <c r="M29" s="1" t="s">
+        <v>2086</v>
+      </c>
       <c r="N29" s="1"/>
     </row>
     <row r="30" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
-        <v>164</v>
+        <v>188</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>165</v>
+        <v>188</v>
       </c>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
       <c r="F30" s="26" t="s">
-        <v>1992</v>
+        <v>1996</v>
       </c>
       <c r="G30" s="39">
-        <v>200.08</v>
+        <v>443.2</v>
       </c>
       <c r="H30" s="22">
         <v>0</v>
@@ -21580,49 +21666,57 @@
     </row>
     <row r="31" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
-        <v>166</v>
+        <v>193</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>167</v>
+        <v>194</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
+      <c r="F31" s="1" t="s">
+        <v>1997</v>
+      </c>
       <c r="G31" s="39">
-        <v>10</v>
+        <v>180.16</v>
       </c>
       <c r="H31" s="22">
         <v>0</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
       <c r="L31" s="1"/>
-      <c r="M31" s="1"/>
-      <c r="N31" s="1"/>
+      <c r="M31" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="N31" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="32" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="1" t="s">
-        <v>168</v>
+        <v>197</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>169</v>
+        <v>198</v>
       </c>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
+      <c r="F32" s="1" t="s">
+        <v>1998</v>
+      </c>
       <c r="G32" s="39">
-        <v>10</v>
+        <v>146.13999999999999</v>
       </c>
       <c r="H32" s="22">
         <v>0</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
@@ -21632,19 +21726,19 @@
     </row>
     <row r="33" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1" t="s">
-        <v>170</v>
+        <v>199</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>171</v>
+        <v>200</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="26" t="s">
-        <v>1993</v>
+        <v>1999</v>
       </c>
       <c r="G33" s="39">
-        <v>260.14</v>
+        <v>274.27</v>
       </c>
       <c r="H33" s="22">
         <v>0</v>
@@ -21655,28 +21749,34 @@
       <c r="J33" s="1"/>
       <c r="K33" s="1"/>
       <c r="L33" s="1"/>
-      <c r="M33" s="1"/>
-      <c r="N33" s="1"/>
+      <c r="M33" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="34" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>172</v>
+        <v>201</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>173</v>
+        <v>202</v>
       </c>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
+      <c r="F34" s="1" t="s">
+        <v>2000</v>
+      </c>
       <c r="G34" s="39">
-        <v>10</v>
+        <v>147.13</v>
       </c>
       <c r="H34" s="22">
         <v>0</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J34" s="1"/>
       <c r="K34" s="1"/>
@@ -21686,45 +21786,51 @@
     </row>
     <row r="35" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>174</v>
+        <v>203</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>175</v>
+        <v>204</v>
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
+      <c r="F35" s="1" t="s">
+        <v>2001</v>
+      </c>
       <c r="G35" s="39">
-        <v>10</v>
+        <v>276.24</v>
       </c>
       <c r="H35" s="22">
         <v>0</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
       <c r="L35" s="1"/>
-      <c r="M35" s="1"/>
-      <c r="N35" s="1"/>
+      <c r="M35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N35" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="36" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1" t="s">
-        <v>176</v>
+        <v>205</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" s="26" t="s">
-        <v>1994</v>
+        <v>2002</v>
       </c>
       <c r="G36" s="39">
-        <v>340.12</v>
+        <v>75.069999999999993</v>
       </c>
       <c r="H36" s="22">
         <v>0</v>
@@ -21740,19 +21846,17 @@
     </row>
     <row r="37" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1" t="s">
-        <v>178</v>
+        <v>207</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>179</v>
+        <v>208</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-      <c r="F37" s="26" t="s">
-        <v>1995</v>
-      </c>
+      <c r="F37" s="26"/>
       <c r="G37" s="39">
-        <v>186.06</v>
+        <v>10</v>
       </c>
       <c r="H37" s="22">
         <v>0</v>
@@ -21763,24 +21867,28 @@
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
       <c r="L37" s="1"/>
-      <c r="M37" s="1"/>
-      <c r="N37" s="1"/>
+      <c r="M37" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N37" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="38" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="1" t="s">
-        <v>180</v>
+        <v>209</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>181</v>
+        <v>209</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
       <c r="F38" s="26" t="s">
-        <v>1995</v>
+        <v>2003</v>
       </c>
       <c r="G38" s="39">
-        <v>186.06</v>
+        <v>363.22</v>
       </c>
       <c r="H38" s="22">
         <v>0</v>
@@ -21796,19 +21904,19 @@
     </row>
     <row r="39" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="1" t="s">
-        <v>182</v>
+        <v>210</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>183</v>
+        <v>211</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
       <c r="F39" s="26" t="s">
-        <v>1993</v>
+        <v>2004</v>
       </c>
       <c r="G39" s="39">
-        <v>260.14</v>
+        <v>151.13</v>
       </c>
       <c r="H39" s="22">
         <v>0</v>
@@ -21820,29 +21928,33 @@
       <c r="K39" s="1"/>
       <c r="L39" s="1"/>
       <c r="M39" s="1" t="s">
-        <v>2086</v>
-      </c>
-      <c r="N39" s="1"/>
+        <v>212</v>
+      </c>
+      <c r="N39" s="1" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="40" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="1" t="s">
-        <v>184</v>
+        <v>214</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>185</v>
+        <v>214</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
+      <c r="F40" s="1" t="s">
+        <v>2005</v>
+      </c>
       <c r="G40" s="39">
-        <v>10</v>
+        <v>523.17899999999997</v>
       </c>
       <c r="H40" s="22">
         <v>0</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J40" s="1"/>
       <c r="K40" s="1"/>
@@ -21852,45 +21964,49 @@
     </row>
     <row r="41" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="1" t="s">
-        <v>186</v>
+        <v>215</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>187</v>
+        <v>216</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
+      <c r="F41" s="1" t="s">
+        <v>215</v>
+      </c>
       <c r="G41" s="39">
-        <v>10</v>
+        <v>1.008</v>
       </c>
       <c r="H41" s="22">
         <v>0</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J41" s="1"/>
       <c r="K41" s="1"/>
       <c r="L41" s="1"/>
-      <c r="M41" s="1"/>
+      <c r="M41" s="1" t="s">
+        <v>217</v>
+      </c>
       <c r="N41" s="1"/>
     </row>
     <row r="42" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="1" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>188</v>
+        <v>218</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1" t="s">
-        <v>1996</v>
+        <v>218</v>
       </c>
       <c r="G42" s="39">
-        <v>443.2</v>
+        <v>18.015000000000001</v>
       </c>
       <c r="H42" s="22">
         <v>0</v>
@@ -21901,28 +22017,34 @@
       <c r="J42" s="1"/>
       <c r="K42" s="1"/>
       <c r="L42" s="1"/>
-      <c r="M42" s="1"/>
-      <c r="N42" s="1"/>
+      <c r="M42" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="N42" s="1" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="43" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1" t="s">
-        <v>189</v>
+        <v>219</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>190</v>
+        <v>220</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
+      <c r="F43" s="1" t="s">
+        <v>2006</v>
+      </c>
       <c r="G43" s="39">
-        <v>10</v>
+        <v>155.15</v>
       </c>
       <c r="H43" s="22">
         <v>0</v>
       </c>
       <c r="I43" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J43" s="1"/>
       <c r="K43" s="1"/>
@@ -21932,45 +22054,51 @@
     </row>
     <row r="44" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="1" t="s">
-        <v>191</v>
+        <v>221</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>192</v>
+        <v>222</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
+      <c r="F44" s="1" t="s">
+        <v>2007</v>
+      </c>
       <c r="G44" s="39">
-        <v>10</v>
+        <v>292.29000000000002</v>
       </c>
       <c r="H44" s="22">
         <v>0</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J44" s="1"/>
       <c r="K44" s="1"/>
       <c r="L44" s="1"/>
-      <c r="M44" s="1"/>
-      <c r="N44" s="1"/>
+      <c r="M44" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N44" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="45" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
-        <v>193</v>
+        <v>227</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>194</v>
+        <v>228</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
       <c r="F45" s="26" t="s">
-        <v>1997</v>
+        <v>2008</v>
       </c>
       <c r="G45" s="39">
-        <v>180.16</v>
+        <v>131.16999999999999</v>
       </c>
       <c r="H45" s="22">
         <v>0</v>
@@ -21981,28 +22109,22 @@
       <c r="J45" s="1"/>
       <c r="K45" s="1"/>
       <c r="L45" s="1"/>
-      <c r="M45" s="1" t="s">
-        <v>195</v>
-      </c>
-      <c r="N45" s="1" t="s">
-        <v>196</v>
-      </c>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
     </row>
     <row r="46" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
-        <v>197</v>
+        <v>229</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>198</v>
+        <v>230</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
-      <c r="F46" s="26" t="s">
-        <v>1998</v>
-      </c>
+      <c r="F46" s="26"/>
       <c r="G46" s="39">
-        <v>146.13999999999999</v>
+        <v>10</v>
       </c>
       <c r="H46" s="22">
         <v>0</v>
@@ -22013,24 +22135,28 @@
       <c r="J46" s="1"/>
       <c r="K46" s="1"/>
       <c r="L46" s="1"/>
-      <c r="M46" s="1"/>
-      <c r="N46" s="1"/>
+      <c r="M46" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N46" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="47" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="1" t="s">
-        <v>199</v>
+        <v>231</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>200</v>
+        <v>232</v>
       </c>
       <c r="C47" s="1"/>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
       <c r="F47" s="26" t="s">
-        <v>1999</v>
+        <v>2087</v>
       </c>
       <c r="G47" s="39">
-        <v>274.27</v>
+        <v>90.08</v>
       </c>
       <c r="H47" s="22">
         <v>0</v>
@@ -22041,28 +22167,22 @@
       <c r="J47" s="1"/>
       <c r="K47" s="1"/>
       <c r="L47" s="1"/>
-      <c r="M47" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N47" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
     </row>
     <row r="48" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="1" t="s">
-        <v>201</v>
+        <v>241</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>202</v>
+        <v>242</v>
       </c>
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="26" t="s">
-        <v>2000</v>
-      </c>
+      <c r="F48" s="26"/>
       <c r="G48" s="39">
-        <v>147.13</v>
+        <v>10</v>
       </c>
       <c r="H48" s="22">
         <v>0</v>
@@ -22078,19 +22198,17 @@
     </row>
     <row r="49" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="1" t="s">
-        <v>203</v>
+        <v>243</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>204</v>
+        <v>244</v>
       </c>
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="26" t="s">
-        <v>2001</v>
-      </c>
+      <c r="F49" s="26"/>
       <c r="G49" s="39">
-        <v>276.24</v>
+        <v>10</v>
       </c>
       <c r="H49" s="22">
         <v>0</v>
@@ -22110,19 +22228,17 @@
     </row>
     <row r="50" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1" t="s">
-        <v>205</v>
+        <v>245</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>206</v>
+        <v>246</v>
       </c>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="26" t="s">
-        <v>2002</v>
-      </c>
+      <c r="F50" s="26"/>
       <c r="G50" s="39">
-        <v>75.069999999999993</v>
+        <v>10</v>
       </c>
       <c r="H50" s="22">
         <v>0</v>
@@ -22138,10 +22254,10 @@
     </row>
     <row r="51" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="1" t="s">
-        <v>207</v>
+        <v>247</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>208</v>
+        <v>248</v>
       </c>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -22168,19 +22284,17 @@
     </row>
     <row r="52" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="1" t="s">
-        <v>209</v>
+        <v>249</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>209</v>
+        <v>250</v>
       </c>
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="26" t="s">
-        <v>2003</v>
-      </c>
+      <c r="F52" s="26"/>
       <c r="G52" s="39">
-        <v>363.22</v>
+        <v>10</v>
       </c>
       <c r="H52" s="22">
         <v>0</v>
@@ -22196,19 +22310,17 @@
     </row>
     <row r="53" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="1" t="s">
-        <v>210</v>
+        <v>251</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>211</v>
+        <v>252</v>
       </c>
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="26" t="s">
-        <v>2004</v>
-      </c>
+      <c r="F53" s="26"/>
       <c r="G53" s="39">
-        <v>151.13</v>
+        <v>10</v>
       </c>
       <c r="H53" s="22">
         <v>0</v>
@@ -22220,27 +22332,27 @@
       <c r="K53" s="1"/>
       <c r="L53" s="1"/>
       <c r="M53" s="1" t="s">
-        <v>212</v>
+        <v>113</v>
       </c>
       <c r="N53" s="1" t="s">
-        <v>213</v>
+        <v>114</v>
       </c>
     </row>
     <row r="54" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>214</v>
+        <v>253</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>214</v>
+        <v>254</v>
       </c>
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
       <c r="F54" s="26" t="s">
-        <v>2005</v>
+        <v>2088</v>
       </c>
       <c r="G54" s="39">
-        <v>523.17899999999997</v>
+        <v>664.4</v>
       </c>
       <c r="H54" s="22">
         <v>0</v>
@@ -22251,24 +22363,28 @@
       <c r="J54" s="1"/>
       <c r="K54" s="1"/>
       <c r="L54" s="1"/>
-      <c r="M54" s="1"/>
-      <c r="N54" s="1"/>
+      <c r="M54" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N54" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="55" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>215</v>
+        <v>255</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>216</v>
+        <v>256</v>
       </c>
       <c r="C55" s="1"/>
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1" t="s">
-        <v>215</v>
+        <v>2089</v>
       </c>
       <c r="G55" s="39">
-        <v>1.008</v>
+        <v>665.4</v>
       </c>
       <c r="H55" s="22">
         <v>0</v>
@@ -22279,26 +22395,24 @@
       <c r="J55" s="1"/>
       <c r="K55" s="1"/>
       <c r="L55" s="1"/>
-      <c r="M55" s="1" t="s">
-        <v>217</v>
-      </c>
+      <c r="M55" s="1"/>
       <c r="N55" s="1"/>
     </row>
     <row r="56" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>218</v>
+        <v>261</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>218</v>
+        <v>262</v>
       </c>
       <c r="C56" s="1"/>
       <c r="D56" s="1"/>
       <c r="E56" s="1"/>
       <c r="F56" s="26" t="s">
-        <v>218</v>
+        <v>261</v>
       </c>
       <c r="G56" s="39">
-        <v>18.015000000000001</v>
+        <v>31.998999999999999</v>
       </c>
       <c r="H56" s="22">
         <v>0</v>
@@ -22310,27 +22424,25 @@
       <c r="K56" s="1"/>
       <c r="L56" s="1"/>
       <c r="M56" s="1" t="s">
-        <v>195</v>
+        <v>263</v>
       </c>
       <c r="N56" s="1" t="s">
-        <v>196</v>
+        <v>154</v>
       </c>
     </row>
     <row r="57" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>219</v>
+        <v>264</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>220</v>
+        <v>265</v>
       </c>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
-      <c r="F57" s="26" t="s">
-        <v>2006</v>
-      </c>
+      <c r="F57" s="26"/>
       <c r="G57" s="39">
-        <v>155.15</v>
+        <v>10</v>
       </c>
       <c r="H57" s="22">
         <v>0</v>
@@ -22346,19 +22458,17 @@
     </row>
     <row r="58" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>221</v>
+        <v>286</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>222</v>
+        <v>287</v>
       </c>
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
-      <c r="F58" s="26" t="s">
-        <v>2007</v>
-      </c>
+      <c r="F58" s="26"/>
       <c r="G58" s="39">
-        <v>292.29000000000002</v>
+        <v>10</v>
       </c>
       <c r="H58" s="22">
         <v>0</v>
@@ -22369,19 +22479,15 @@
       <c r="J58" s="1"/>
       <c r="K58" s="1"/>
       <c r="L58" s="1"/>
-      <c r="M58" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N58" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
     </row>
     <row r="59" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>223</v>
+        <v>288</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>224</v>
+        <v>289</v>
       </c>
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
@@ -22394,20 +22500,24 @@
         <v>0</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J59" s="1"/>
       <c r="K59" s="1"/>
       <c r="L59" s="1"/>
-      <c r="M59" s="1"/>
-      <c r="N59" s="1"/>
+      <c r="M59" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N59" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="60" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>225</v>
+        <v>290</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>226</v>
+        <v>291</v>
       </c>
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
@@ -22420,29 +22530,29 @@
         <v>0</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J60" s="1"/>
       <c r="K60" s="1"/>
       <c r="L60" s="1"/>
-      <c r="M60" s="1"/>
+      <c r="M60" s="1" t="s">
+        <v>139</v>
+      </c>
       <c r="N60" s="1"/>
     </row>
     <row r="61" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>227</v>
+        <v>300</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>228</v>
+        <v>301</v>
       </c>
       <c r="C61" s="1"/>
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
-      <c r="F61" s="1" t="s">
-        <v>2008</v>
-      </c>
+      <c r="F61" s="1"/>
       <c r="G61" s="39">
-        <v>131.16999999999999</v>
+        <v>10</v>
       </c>
       <c r="H61" s="22">
         <v>0</v>
@@ -22458,10 +22568,10 @@
     </row>
     <row r="62" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>229</v>
+        <v>302</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>230</v>
+        <v>303</v>
       </c>
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
@@ -22479,28 +22589,22 @@
       <c r="J62" s="1"/>
       <c r="K62" s="1"/>
       <c r="L62" s="1"/>
-      <c r="M62" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N62" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
     </row>
     <row r="63" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>231</v>
+        <v>304</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>232</v>
+        <v>305</v>
       </c>
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
-      <c r="F63" s="26" t="s">
-        <v>2087</v>
-      </c>
+      <c r="F63" s="26"/>
       <c r="G63" s="39">
-        <v>90.08</v>
+        <v>10</v>
       </c>
       <c r="H63" s="22">
         <v>0</v>
@@ -22511,15 +22615,19 @@
       <c r="J63" s="1"/>
       <c r="K63" s="1"/>
       <c r="L63" s="1"/>
-      <c r="M63" s="1"/>
-      <c r="N63" s="1"/>
+      <c r="M63" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N63" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="64" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>233</v>
+        <v>306</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>234</v>
+        <v>307</v>
       </c>
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
@@ -22532,7 +22640,7 @@
         <v>0</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J64" s="1"/>
       <c r="K64" s="1"/>
@@ -22542,10 +22650,10 @@
     </row>
     <row r="65" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>235</v>
+        <v>320</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>236</v>
+        <v>321</v>
       </c>
       <c r="C65" s="1"/>
       <c r="D65" s="1"/>
@@ -22558,7 +22666,7 @@
         <v>0</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J65" s="1"/>
       <c r="K65" s="1"/>
@@ -22568,10 +22676,10 @@
     </row>
     <row r="66" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>237</v>
+        <v>326</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>238</v>
+        <v>327</v>
       </c>
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
@@ -22584,7 +22692,7 @@
         <v>0</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
@@ -22594,10 +22702,10 @@
     </row>
     <row r="67" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>239</v>
+        <v>332</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>240</v>
+        <v>333</v>
       </c>
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
@@ -22610,7 +22718,7 @@
         <v>0</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J67" s="1"/>
       <c r="K67" s="1"/>
@@ -22620,10 +22728,10 @@
     </row>
     <row r="68" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>241</v>
+        <v>346</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>242</v>
+        <v>347</v>
       </c>
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
@@ -22646,10 +22754,10 @@
     </row>
     <row r="69" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>243</v>
+        <v>348</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>244</v>
+        <v>349</v>
       </c>
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
@@ -22667,19 +22775,15 @@
       <c r="J69" s="1"/>
       <c r="K69" s="1"/>
       <c r="L69" s="1"/>
-      <c r="M69" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N69" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
     </row>
     <row r="70" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>245</v>
+        <v>350</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>246</v>
+        <v>351</v>
       </c>
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
@@ -22697,15 +22801,19 @@
       <c r="J70" s="1"/>
       <c r="K70" s="1"/>
       <c r="L70" s="1"/>
-      <c r="M70" s="1"/>
-      <c r="N70" s="1"/>
+      <c r="M70" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N70" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="71" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>247</v>
+        <v>352</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>248</v>
+        <v>353</v>
       </c>
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
@@ -22723,19 +22831,15 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
-      <c r="M71" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N71" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
     </row>
     <row r="72" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>249</v>
+        <v>354</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>250</v>
+        <v>355</v>
       </c>
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
@@ -22758,10 +22862,10 @@
     </row>
     <row r="73" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>251</v>
+        <v>356</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>252</v>
+        <v>357</v>
       </c>
       <c r="C73" s="1"/>
       <c r="D73" s="1"/>
@@ -22779,28 +22883,22 @@
       <c r="J73" s="1"/>
       <c r="K73" s="1"/>
       <c r="L73" s="1"/>
-      <c r="M73" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N73" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
     </row>
     <row r="74" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>253</v>
+        <v>358</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>254</v>
+        <v>359</v>
       </c>
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
-      <c r="F74" s="26" t="s">
-        <v>2088</v>
-      </c>
+      <c r="F74" s="26"/>
       <c r="G74" s="39">
-        <v>664.4</v>
+        <v>10</v>
       </c>
       <c r="H74" s="22">
         <v>0</v>
@@ -22820,19 +22918,17 @@
     </row>
     <row r="75" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>255</v>
+        <v>368</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>256</v>
+        <v>369</v>
       </c>
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="26" t="s">
-        <v>2089</v>
-      </c>
+      <c r="F75" s="26"/>
       <c r="G75" s="39">
-        <v>665.4</v>
+        <v>10</v>
       </c>
       <c r="H75" s="22">
         <v>0</v>
@@ -22848,10 +22944,10 @@
     </row>
     <row r="76" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>257</v>
+        <v>370</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>258</v>
+        <v>371</v>
       </c>
       <c r="C76" s="1"/>
       <c r="D76" s="1"/>
@@ -22864,20 +22960,24 @@
         <v>0</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J76" s="1"/>
       <c r="K76" s="1"/>
       <c r="L76" s="1"/>
-      <c r="M76" s="1"/>
-      <c r="N76" s="1"/>
+      <c r="M76" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N76" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="77" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>259</v>
+        <v>372</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>260</v>
+        <v>373</v>
       </c>
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
@@ -22890,7 +22990,7 @@
         <v>0</v>
       </c>
       <c r="I77" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J77" s="1"/>
       <c r="K77" s="1"/>
@@ -22900,19 +23000,17 @@
     </row>
     <row r="78" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>261</v>
+        <v>374</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>262</v>
+        <v>375</v>
       </c>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
-      <c r="F78" s="1" t="s">
-        <v>261</v>
-      </c>
+      <c r="F78" s="1"/>
       <c r="G78" s="39">
-        <v>31.998999999999999</v>
+        <v>10</v>
       </c>
       <c r="H78" s="22">
         <v>0</v>
@@ -22924,18 +23022,18 @@
       <c r="K78" s="1"/>
       <c r="L78" s="1"/>
       <c r="M78" s="1" t="s">
-        <v>263</v>
+        <v>113</v>
       </c>
       <c r="N78" s="1" t="s">
-        <v>154</v>
+        <v>114</v>
       </c>
     </row>
     <row r="79" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>264</v>
+        <v>380</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>265</v>
+        <v>380</v>
       </c>
       <c r="C79" s="1"/>
       <c r="D79" s="1"/>
@@ -22958,10 +23056,10 @@
     </row>
     <row r="80" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>266</v>
+        <v>381</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>267</v>
+        <v>381</v>
       </c>
       <c r="C80" s="1"/>
       <c r="D80" s="1"/>
@@ -22974,7 +23072,7 @@
         <v>0</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J80" s="1"/>
       <c r="K80" s="1"/>
@@ -22984,10 +23082,10 @@
     </row>
     <row r="81" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>268</v>
+        <v>386</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>269</v>
+        <v>387</v>
       </c>
       <c r="C81" s="1"/>
       <c r="D81" s="1"/>
@@ -23000,20 +23098,24 @@
         <v>0</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J81" s="1"/>
       <c r="K81" s="1"/>
       <c r="L81" s="1"/>
-      <c r="M81" s="1"/>
-      <c r="N81" s="1"/>
+      <c r="M81" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="N81" s="1" t="s">
+        <v>213</v>
+      </c>
     </row>
     <row r="82" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>270</v>
+        <v>389</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>271</v>
+        <v>390</v>
       </c>
       <c r="C82" s="1"/>
       <c r="D82" s="1"/>
@@ -23026,7 +23128,7 @@
         <v>0</v>
       </c>
       <c r="I82" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J82" s="1"/>
       <c r="K82" s="1"/>
@@ -23036,10 +23138,10 @@
     </row>
     <row r="83" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>272</v>
+        <v>391</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>273</v>
+        <v>391</v>
       </c>
       <c r="C83" s="1"/>
       <c r="D83" s="1"/>
@@ -23052,20 +23154,24 @@
         <v>0</v>
       </c>
       <c r="I83" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
       <c r="L83" s="1"/>
-      <c r="M83" s="1"/>
-      <c r="N83" s="1"/>
+      <c r="M83" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N83" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="84" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>274</v>
+        <v>392</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>275</v>
+        <v>393</v>
       </c>
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
@@ -23078,7 +23184,7 @@
         <v>0</v>
       </c>
       <c r="I84" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J84" s="1"/>
       <c r="K84" s="1"/>
@@ -23088,10 +23194,10 @@
     </row>
     <row r="85" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>276</v>
+        <v>394</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>277</v>
+        <v>395</v>
       </c>
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
@@ -23104,20 +23210,24 @@
         <v>0</v>
       </c>
       <c r="I85" s="1" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="J85" s="1"/>
       <c r="K85" s="1"/>
       <c r="L85" s="1"/>
-      <c r="M85" s="1"/>
-      <c r="N85" s="1"/>
+      <c r="M85" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="N85" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="86" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>278</v>
+        <v>396</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>279</v>
+        <v>397</v>
       </c>
       <c r="C86" s="1"/>
       <c r="D86" s="1"/>
@@ -23130,7 +23240,7 @@
         <v>0</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
@@ -23140,43 +23250,47 @@
     </row>
     <row r="87" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>280</v>
+        <v>115</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>281</v>
+        <v>116</v>
       </c>
       <c r="C87" s="1"/>
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
-      <c r="G87" s="39">
-        <v>10</v>
+      <c r="G87" s="41">
+        <v>40000</v>
       </c>
       <c r="H87" s="22">
         <v>0</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J87" s="1"/>
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
-      <c r="M87" s="1"/>
-      <c r="N87" s="1"/>
+      <c r="M87" s="1" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N87" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="88" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>282</v>
+        <v>127</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>283</v>
+        <v>128</v>
       </c>
       <c r="C88" s="1"/>
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
-      <c r="G88" s="39">
-        <v>10</v>
+      <c r="G88" s="41">
+        <v>40000</v>
       </c>
       <c r="H88" s="22">
         <v>0</v>
@@ -23187,132 +23301,146 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
-      <c r="M88" s="1"/>
-      <c r="N88" s="1"/>
+      <c r="M88" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N88" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="89" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>284</v>
+        <v>146</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>285</v>
+        <v>147</v>
       </c>
       <c r="C89" s="1"/>
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
-      <c r="G89" s="39">
-        <v>10</v>
+      <c r="G89" s="41">
+        <v>40000</v>
       </c>
       <c r="H89" s="22">
         <v>0</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
-      <c r="M89" s="1"/>
-      <c r="N89" s="1"/>
+      <c r="M89" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N89" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="90" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>286</v>
+        <v>166</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>287</v>
+        <v>167</v>
       </c>
       <c r="C90" s="1"/>
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
-      <c r="G90" s="39">
-        <v>10</v>
+      <c r="G90" s="41">
+        <v>40000</v>
       </c>
       <c r="H90" s="22">
         <v>0</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
       <c r="L90" s="1"/>
-      <c r="M90" s="1"/>
-      <c r="N90" s="1"/>
+      <c r="M90" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N90" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="91" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>288</v>
+        <v>172</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>289</v>
+        <v>173</v>
       </c>
       <c r="C91" s="1"/>
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
-      <c r="G91" s="39">
-        <v>10</v>
+      <c r="G91" s="41">
+        <v>40000</v>
       </c>
       <c r="H91" s="22">
         <v>0</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
       <c r="L91" s="1"/>
-      <c r="M91" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N91" s="1" t="s">
-        <v>114</v>
+      <c r="M91" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N91" s="25" t="s">
+        <v>2091</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>290</v>
+        <v>184</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>291</v>
+        <v>185</v>
       </c>
       <c r="C92" s="1"/>
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
-      <c r="G92" s="39">
-        <v>10</v>
+      <c r="G92" s="41">
+        <v>40000</v>
       </c>
       <c r="H92" s="22">
         <v>0</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
       <c r="L92" s="1"/>
-      <c r="M92" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="N92" s="1"/>
+      <c r="M92" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N92" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="93" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>292</v>
+        <v>189</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>293</v>
+        <v>190</v>
       </c>
       <c r="C93" s="1"/>
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
-      <c r="G93" s="39">
-        <v>10</v>
+      <c r="G93" s="41">
+        <v>40000</v>
       </c>
       <c r="H93" s="22">
         <v>0</v>
@@ -23323,48 +23451,56 @@
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
       <c r="L93" s="1"/>
-      <c r="M93" s="1"/>
-      <c r="N93" s="1"/>
+      <c r="M93" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N93" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="94" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>294</v>
+        <v>223</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>295</v>
+        <v>224</v>
       </c>
       <c r="C94" s="1"/>
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
-      <c r="G94" s="39">
-        <v>10</v>
+      <c r="G94" s="41">
+        <v>40000</v>
       </c>
       <c r="H94" s="22">
         <v>0</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
-      <c r="M94" s="1"/>
-      <c r="N94" s="1"/>
+      <c r="M94" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N94" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="95" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>296</v>
+        <v>233</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>297</v>
+        <v>234</v>
       </c>
       <c r="C95" s="1"/>
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
-      <c r="G95" s="39">
-        <v>10</v>
+      <c r="G95" s="41">
+        <v>40000</v>
       </c>
       <c r="H95" s="22">
         <v>0</v>
@@ -23375,156 +23511,176 @@
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
-      <c r="M95" s="1"/>
-      <c r="N95" s="1"/>
+      <c r="M95" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N95" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="96" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>298</v>
+        <v>237</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>299</v>
+        <v>238</v>
       </c>
       <c r="C96" s="1"/>
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
-      <c r="G96" s="39">
-        <v>10</v>
+      <c r="G96" s="41">
+        <v>40000</v>
       </c>
       <c r="H96" s="22">
         <v>0</v>
       </c>
       <c r="I96" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
       <c r="L96" s="1"/>
-      <c r="M96" s="1"/>
-      <c r="N96" s="1"/>
+      <c r="M96" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N96" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="97" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>300</v>
+        <v>257</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>301</v>
+        <v>258</v>
       </c>
       <c r="C97" s="1"/>
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
-      <c r="G97" s="39">
-        <v>10</v>
+      <c r="G97" s="41">
+        <v>40000</v>
       </c>
       <c r="H97" s="22">
         <v>0</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
       <c r="L97" s="1"/>
-      <c r="M97" s="1"/>
-      <c r="N97" s="1"/>
+      <c r="M97" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N97" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="98" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>302</v>
+        <v>266</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>303</v>
+        <v>267</v>
       </c>
       <c r="C98" s="1"/>
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
-      <c r="G98" s="39">
-        <v>10</v>
+      <c r="G98" s="41">
+        <v>40000</v>
       </c>
       <c r="H98" s="22">
         <v>0</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
       <c r="L98" s="1"/>
-      <c r="M98" s="1"/>
-      <c r="N98" s="1"/>
+      <c r="M98" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N98" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="99" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>304</v>
+        <v>270</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>305</v>
+        <v>271</v>
       </c>
       <c r="C99" s="1"/>
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
-      <c r="G99" s="39">
-        <v>10</v>
+      <c r="G99" s="41">
+        <v>40000</v>
       </c>
       <c r="H99" s="22">
         <v>0</v>
       </c>
       <c r="I99" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
-      <c r="M99" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N99" s="1" t="s">
-        <v>114</v>
+      <c r="M99" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N99" s="25" t="s">
+        <v>2091</v>
       </c>
     </row>
     <row r="100" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>306</v>
+        <v>274</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>307</v>
+        <v>275</v>
       </c>
       <c r="C100" s="1"/>
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
-      <c r="G100" s="39">
-        <v>10</v>
+      <c r="G100" s="41">
+        <v>40000</v>
       </c>
       <c r="H100" s="22">
         <v>0</v>
       </c>
       <c r="I100" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
-      <c r="M100" s="1"/>
-      <c r="N100" s="1"/>
+      <c r="M100" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N100" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="101" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>308</v>
+        <v>278</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>309</v>
+        <v>279</v>
       </c>
       <c r="C101" s="1"/>
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
-      <c r="G101" s="39">
-        <v>10</v>
+      <c r="G101" s="41">
+        <v>40000</v>
       </c>
       <c r="H101" s="22">
         <v>0</v>
@@ -23535,48 +23691,56 @@
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
-      <c r="M101" s="1"/>
-      <c r="N101" s="1"/>
+      <c r="M101" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N101" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="102" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>310</v>
+        <v>282</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>311</v>
+        <v>283</v>
       </c>
       <c r="C102" s="1"/>
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
-      <c r="G102" s="39">
-        <v>10</v>
+      <c r="G102" s="41">
+        <v>40000</v>
       </c>
       <c r="H102" s="22">
         <v>0</v>
       </c>
       <c r="I102" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>
-      <c r="M102" s="1"/>
-      <c r="N102" s="1"/>
+      <c r="M102" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N102" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="103" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>312</v>
+        <v>292</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>313</v>
+        <v>293</v>
       </c>
       <c r="C103" s="1"/>
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
-      <c r="G103" s="39">
-        <v>10</v>
+      <c r="G103" s="41">
+        <v>40000</v>
       </c>
       <c r="H103" s="22">
         <v>0</v>
@@ -23587,48 +23751,56 @@
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
       <c r="L103" s="1"/>
-      <c r="M103" s="1"/>
-      <c r="N103" s="1"/>
+      <c r="M103" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N103" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="104" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>314</v>
+        <v>296</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>315</v>
+        <v>297</v>
       </c>
       <c r="C104" s="1"/>
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
-      <c r="G104" s="39">
-        <v>10</v>
+      <c r="G104" s="41">
+        <v>40000</v>
       </c>
       <c r="H104" s="22">
         <v>0</v>
       </c>
       <c r="I104" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
-      <c r="M104" s="1"/>
-      <c r="N104" s="1"/>
+      <c r="M104" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N104" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="105" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>316</v>
+        <v>308</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>317</v>
+        <v>309</v>
       </c>
       <c r="C105" s="1"/>
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
-      <c r="G105" s="39">
-        <v>10</v>
+      <c r="G105" s="41">
+        <v>40000</v>
       </c>
       <c r="H105" s="22">
         <v>0</v>
@@ -23639,60 +23811,72 @@
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
       <c r="L105" s="1"/>
-      <c r="M105" s="1"/>
-      <c r="N105" s="1"/>
+      <c r="M105" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N105" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="106" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>319</v>
+        <v>313</v>
       </c>
       <c r="C106" s="1"/>
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
-      <c r="G106" s="39">
-        <v>10</v>
+      <c r="G106" s="41">
+        <v>40000</v>
       </c>
       <c r="H106" s="22">
         <v>0</v>
       </c>
       <c r="I106" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
       <c r="L106" s="1"/>
-      <c r="M106" s="1"/>
-      <c r="N106" s="1"/>
+      <c r="M106" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N106" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="107" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="C107" s="1"/>
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
-      <c r="G107" s="39">
-        <v>10</v>
+      <c r="G107" s="41">
+        <v>40000</v>
       </c>
       <c r="H107" s="22">
         <v>0</v>
       </c>
       <c r="I107" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
       <c r="L107" s="1"/>
-      <c r="M107" s="1"/>
-      <c r="N107" s="1"/>
+      <c r="M107" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N107" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="108" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
@@ -23705,8 +23889,8 @@
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
-      <c r="G108" s="39">
-        <v>10</v>
+      <c r="G108" s="41">
+        <v>40000</v>
       </c>
       <c r="H108" s="22">
         <v>0</v>
@@ -23717,74 +23901,86 @@
       <c r="J108" s="1"/>
       <c r="K108" s="1"/>
       <c r="L108" s="1"/>
-      <c r="M108" s="1"/>
-      <c r="N108" s="1"/>
+      <c r="M108" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N108" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="109" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="C109" s="1"/>
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
-      <c r="G109" s="39">
-        <v>10</v>
+      <c r="G109" s="41">
+        <v>40000</v>
       </c>
       <c r="H109" s="22">
         <v>0</v>
       </c>
       <c r="I109" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
       <c r="L109" s="1"/>
-      <c r="M109" s="1"/>
-      <c r="N109" s="1"/>
+      <c r="M109" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N109" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="110" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>326</v>
+        <v>334</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>327</v>
+        <v>335</v>
       </c>
       <c r="C110" s="1"/>
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
-      <c r="G110" s="39">
-        <v>10</v>
+      <c r="G110" s="41">
+        <v>40000</v>
       </c>
       <c r="H110" s="22">
         <v>0</v>
       </c>
       <c r="I110" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="J110" s="1"/>
       <c r="K110" s="1"/>
       <c r="L110" s="1"/>
-      <c r="M110" s="1"/>
-      <c r="N110" s="1"/>
+      <c r="M110" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N110" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="111" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
-        <v>328</v>
+        <v>338</v>
       </c>
       <c r="B111" s="1" t="s">
-        <v>329</v>
+        <v>339</v>
       </c>
       <c r="C111" s="1"/>
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
-      <c r="G111" s="39">
-        <v>10</v>
+      <c r="G111" s="41">
+        <v>40000</v>
       </c>
       <c r="H111" s="22">
         <v>0</v>
@@ -23795,74 +23991,86 @@
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
       <c r="L111" s="1"/>
-      <c r="M111" s="1"/>
-      <c r="N111" s="1"/>
+      <c r="M111" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N111" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="112" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
-        <v>330</v>
+        <v>342</v>
       </c>
       <c r="B112" s="1" t="s">
-        <v>331</v>
+        <v>343</v>
       </c>
       <c r="C112" s="1"/>
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
-      <c r="G112" s="39">
-        <v>10</v>
+      <c r="G112" s="41">
+        <v>40000</v>
       </c>
       <c r="H112" s="22">
         <v>0</v>
       </c>
       <c r="I112" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
       <c r="L112" s="1"/>
-      <c r="M112" s="1"/>
-      <c r="N112" s="1"/>
+      <c r="M112" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N112" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="113" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
-        <v>332</v>
+        <v>360</v>
       </c>
       <c r="B113" s="1" t="s">
-        <v>333</v>
+        <v>361</v>
       </c>
       <c r="C113" s="1"/>
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
-      <c r="G113" s="39">
-        <v>10</v>
+      <c r="G113" s="41">
+        <v>40000</v>
       </c>
       <c r="H113" s="22">
         <v>0</v>
       </c>
       <c r="I113" s="1" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
       <c r="L113" s="1"/>
-      <c r="M113" s="1"/>
-      <c r="N113" s="1"/>
+      <c r="M113" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N113" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="114" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
-        <v>334</v>
+        <v>364</v>
       </c>
       <c r="B114" s="1" t="s">
-        <v>335</v>
+        <v>365</v>
       </c>
       <c r="C114" s="1"/>
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
-      <c r="G114" s="39">
-        <v>10</v>
+      <c r="G114" s="41">
+        <v>40000</v>
       </c>
       <c r="H114" s="22">
         <v>0</v>
@@ -23873,48 +24081,56 @@
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
       <c r="L114" s="1"/>
-      <c r="M114" s="1"/>
-      <c r="N114" s="1"/>
+      <c r="M114" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N114" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="115" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
-        <v>336</v>
+        <v>376</v>
       </c>
       <c r="B115" s="1" t="s">
-        <v>337</v>
+        <v>377</v>
       </c>
       <c r="C115" s="1"/>
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
-      <c r="G115" s="39">
-        <v>10</v>
+      <c r="G115" s="41">
+        <v>40000</v>
       </c>
       <c r="H115" s="22">
         <v>0</v>
       </c>
       <c r="I115" s="1" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
       <c r="L115" s="1"/>
-      <c r="M115" s="1"/>
-      <c r="N115" s="1"/>
+      <c r="M115" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N115" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="116" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
-        <v>338</v>
+        <v>382</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>339</v>
+        <v>383</v>
       </c>
       <c r="C116" s="1"/>
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
-      <c r="G116" s="39">
-        <v>10</v>
+      <c r="G116" s="41">
+        <v>40000</v>
       </c>
       <c r="H116" s="22">
         <v>0</v>
@@ -23925,15 +24141,19 @@
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
       <c r="L116" s="1"/>
-      <c r="M116" s="1"/>
-      <c r="N116" s="1"/>
+      <c r="M116" s="26" t="s">
+        <v>2090</v>
+      </c>
+      <c r="N116" s="25" t="s">
+        <v>2091</v>
+      </c>
     </row>
     <row r="117" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
-        <v>340</v>
+        <v>118</v>
       </c>
       <c r="B117" s="1" t="s">
-        <v>341</v>
+        <v>119</v>
       </c>
       <c r="C117" s="1"/>
       <c r="D117" s="1"/>
@@ -23956,10 +24176,10 @@
     </row>
     <row r="118" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
-        <v>342</v>
+        <v>129</v>
       </c>
       <c r="B118" s="1" t="s">
-        <v>343</v>
+        <v>130</v>
       </c>
       <c r="C118" s="1"/>
       <c r="D118" s="1"/>
@@ -23972,7 +24192,7 @@
         <v>0</v>
       </c>
       <c r="I118" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
@@ -23982,10 +24202,10 @@
     </row>
     <row r="119" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
-        <v>344</v>
+        <v>148</v>
       </c>
       <c r="B119" s="1" t="s">
-        <v>345</v>
+        <v>149</v>
       </c>
       <c r="C119" s="1"/>
       <c r="D119" s="1"/>
@@ -24008,10 +24228,10 @@
     </row>
     <row r="120" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
-        <v>346</v>
+        <v>168</v>
       </c>
       <c r="B120" s="1" t="s">
-        <v>347</v>
+        <v>169</v>
       </c>
       <c r="C120" s="1"/>
       <c r="D120" s="1"/>
@@ -24024,7 +24244,7 @@
         <v>0</v>
       </c>
       <c r="I120" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
@@ -24034,10 +24254,10 @@
     </row>
     <row r="121" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
-        <v>348</v>
+        <v>174</v>
       </c>
       <c r="B121" s="1" t="s">
-        <v>349</v>
+        <v>175</v>
       </c>
       <c r="C121" s="1"/>
       <c r="D121" s="1"/>
@@ -24050,7 +24270,7 @@
         <v>0</v>
       </c>
       <c r="I121" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
@@ -24060,10 +24280,10 @@
     </row>
     <row r="122" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
-        <v>350</v>
+        <v>186</v>
       </c>
       <c r="B122" s="1" t="s">
-        <v>351</v>
+        <v>187</v>
       </c>
       <c r="C122" s="1"/>
       <c r="D122" s="1"/>
@@ -24076,24 +24296,20 @@
         <v>0</v>
       </c>
       <c r="I122" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
       <c r="L122" s="1"/>
-      <c r="M122" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N122" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="M122" s="1"/>
+      <c r="N122" s="1"/>
     </row>
     <row r="123" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
-        <v>352</v>
+        <v>191</v>
       </c>
       <c r="B123" s="1" t="s">
-        <v>353</v>
+        <v>192</v>
       </c>
       <c r="C123" s="1"/>
       <c r="D123" s="1"/>
@@ -24106,7 +24322,7 @@
         <v>0</v>
       </c>
       <c r="I123" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
@@ -24116,10 +24332,10 @@
     </row>
     <row r="124" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
-        <v>354</v>
+        <v>225</v>
       </c>
       <c r="B124" s="1" t="s">
-        <v>355</v>
+        <v>226</v>
       </c>
       <c r="C124" s="1"/>
       <c r="D124" s="1"/>
@@ -24132,7 +24348,7 @@
         <v>0</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
@@ -24142,10 +24358,10 @@
     </row>
     <row r="125" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
-        <v>356</v>
+        <v>235</v>
       </c>
       <c r="B125" s="1" t="s">
-        <v>357</v>
+        <v>236</v>
       </c>
       <c r="C125" s="1"/>
       <c r="D125" s="1"/>
@@ -24158,7 +24374,7 @@
         <v>0</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
@@ -24168,10 +24384,10 @@
     </row>
     <row r="126" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
-        <v>358</v>
+        <v>239</v>
       </c>
       <c r="B126" s="1" t="s">
-        <v>359</v>
+        <v>240</v>
       </c>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
@@ -24184,24 +24400,20 @@
         <v>0</v>
       </c>
       <c r="I126" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
       <c r="L126" s="1"/>
-      <c r="M126" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N126" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="M126" s="1"/>
+      <c r="N126" s="1"/>
     </row>
     <row r="127" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
-        <v>360</v>
+        <v>259</v>
       </c>
       <c r="B127" s="1" t="s">
-        <v>361</v>
+        <v>260</v>
       </c>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
@@ -24214,7 +24426,7 @@
         <v>0</v>
       </c>
       <c r="I127" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
@@ -24224,10 +24436,10 @@
     </row>
     <row r="128" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
-        <v>362</v>
+        <v>268</v>
       </c>
       <c r="B128" s="1" t="s">
-        <v>363</v>
+        <v>269</v>
       </c>
       <c r="C128" s="1"/>
       <c r="D128" s="1"/>
@@ -24250,10 +24462,10 @@
     </row>
     <row r="129" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
-        <v>364</v>
+        <v>272</v>
       </c>
       <c r="B129" s="1" t="s">
-        <v>365</v>
+        <v>273</v>
       </c>
       <c r="C129" s="1"/>
       <c r="D129" s="1"/>
@@ -24266,7 +24478,7 @@
         <v>0</v>
       </c>
       <c r="I129" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="J129" s="1"/>
       <c r="K129" s="1"/>
@@ -24276,10 +24488,10 @@
     </row>
     <row r="130" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
-        <v>366</v>
+        <v>276</v>
       </c>
       <c r="B130" s="1" t="s">
-        <v>367</v>
+        <v>277</v>
       </c>
       <c r="C130" s="1"/>
       <c r="D130" s="1"/>
@@ -24302,10 +24514,10 @@
     </row>
     <row r="131" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
-        <v>368</v>
+        <v>280</v>
       </c>
       <c r="B131" s="1" t="s">
-        <v>369</v>
+        <v>281</v>
       </c>
       <c r="C131" s="1"/>
       <c r="D131" s="1"/>
@@ -24318,7 +24530,7 @@
         <v>0</v>
       </c>
       <c r="I131" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J131" s="1"/>
       <c r="K131" s="1"/>
@@ -24328,10 +24540,10 @@
     </row>
     <row r="132" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
-        <v>370</v>
+        <v>284</v>
       </c>
       <c r="B132" s="1" t="s">
-        <v>371</v>
+        <v>285</v>
       </c>
       <c r="C132" s="1"/>
       <c r="D132" s="1"/>
@@ -24344,24 +24556,20 @@
         <v>0</v>
       </c>
       <c r="I132" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J132" s="1"/>
       <c r="K132" s="1"/>
       <c r="L132" s="1"/>
-      <c r="M132" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N132" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="M132" s="1"/>
+      <c r="N132" s="1"/>
     </row>
     <row r="133" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
-        <v>372</v>
+        <v>294</v>
       </c>
       <c r="B133" s="1" t="s">
-        <v>373</v>
+        <v>295</v>
       </c>
       <c r="C133" s="1"/>
       <c r="D133" s="1"/>
@@ -24374,7 +24582,7 @@
         <v>0</v>
       </c>
       <c r="I133" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J133" s="1"/>
       <c r="K133" s="1"/>
@@ -24384,10 +24592,10 @@
     </row>
     <row r="134" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
-        <v>374</v>
+        <v>298</v>
       </c>
       <c r="B134" s="1" t="s">
-        <v>375</v>
+        <v>299</v>
       </c>
       <c r="C134" s="1"/>
       <c r="D134" s="1"/>
@@ -24400,24 +24608,20 @@
         <v>0</v>
       </c>
       <c r="I134" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J134" s="1"/>
       <c r="K134" s="1"/>
       <c r="L134" s="1"/>
-      <c r="M134" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N134" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="M134" s="1"/>
+      <c r="N134" s="1"/>
     </row>
     <row r="135" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
-        <v>376</v>
+        <v>310</v>
       </c>
       <c r="B135" s="1" t="s">
-        <v>377</v>
+        <v>311</v>
       </c>
       <c r="C135" s="1"/>
       <c r="D135" s="1"/>
@@ -24430,7 +24634,7 @@
         <v>0</v>
       </c>
       <c r="I135" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="J135" s="1"/>
       <c r="K135" s="1"/>
@@ -24440,10 +24644,10 @@
     </row>
     <row r="136" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
-        <v>378</v>
+        <v>314</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>379</v>
+        <v>315</v>
       </c>
       <c r="C136" s="1"/>
       <c r="D136" s="1"/>
@@ -24466,10 +24670,10 @@
     </row>
     <row r="137" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
-        <v>380</v>
+        <v>318</v>
       </c>
       <c r="B137" s="1" t="s">
-        <v>380</v>
+        <v>319</v>
       </c>
       <c r="C137" s="1"/>
       <c r="D137" s="1"/>
@@ -24482,7 +24686,7 @@
         <v>0</v>
       </c>
       <c r="I137" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J137" s="1"/>
       <c r="K137" s="1"/>
@@ -24492,10 +24696,10 @@
     </row>
     <row r="138" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
-        <v>381</v>
+        <v>324</v>
       </c>
       <c r="B138" s="1" t="s">
-        <v>381</v>
+        <v>325</v>
       </c>
       <c r="C138" s="1"/>
       <c r="D138" s="1"/>
@@ -24508,7 +24712,7 @@
         <v>0</v>
       </c>
       <c r="I138" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J138" s="1"/>
       <c r="K138" s="1"/>
@@ -24518,10 +24722,10 @@
     </row>
     <row r="139" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
-        <v>382</v>
+        <v>330</v>
       </c>
       <c r="B139" s="1" t="s">
-        <v>383</v>
+        <v>331</v>
       </c>
       <c r="C139" s="1"/>
       <c r="D139" s="1"/>
@@ -24534,7 +24738,7 @@
         <v>0</v>
       </c>
       <c r="I139" s="1" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="J139" s="1"/>
       <c r="K139" s="1"/>
@@ -24544,10 +24748,10 @@
     </row>
     <row r="140" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
-        <v>384</v>
+        <v>336</v>
       </c>
       <c r="B140" s="1" t="s">
-        <v>385</v>
+        <v>337</v>
       </c>
       <c r="C140" s="1"/>
       <c r="D140" s="1"/>
@@ -24570,10 +24774,10 @@
     </row>
     <row r="141" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
-        <v>386</v>
+        <v>340</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>387</v>
+        <v>341</v>
       </c>
       <c r="C141" s="1"/>
       <c r="D141" s="1"/>
@@ -24586,24 +24790,20 @@
         <v>0</v>
       </c>
       <c r="I141" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J141" s="1"/>
       <c r="K141" s="1"/>
       <c r="L141" s="1"/>
-      <c r="M141" s="1" t="s">
-        <v>388</v>
-      </c>
-      <c r="N141" s="1" t="s">
-        <v>213</v>
-      </c>
+      <c r="M141" s="1"/>
+      <c r="N141" s="1"/>
     </row>
     <row r="142" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
-        <v>389</v>
+        <v>344</v>
       </c>
       <c r="B142" s="1" t="s">
-        <v>390</v>
+        <v>345</v>
       </c>
       <c r="C142" s="1"/>
       <c r="D142" s="1"/>
@@ -24616,7 +24816,7 @@
         <v>0</v>
       </c>
       <c r="I142" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J142" s="1"/>
       <c r="K142" s="1"/>
@@ -24626,10 +24826,10 @@
     </row>
     <row r="143" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
-        <v>391</v>
+        <v>362</v>
       </c>
       <c r="B143" s="1" t="s">
-        <v>391</v>
+        <v>363</v>
       </c>
       <c r="C143" s="1"/>
       <c r="D143" s="1"/>
@@ -24642,24 +24842,20 @@
         <v>0</v>
       </c>
       <c r="I143" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J143" s="1"/>
       <c r="K143" s="1"/>
       <c r="L143" s="1"/>
-      <c r="M143" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N143" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="M143" s="1"/>
+      <c r="N143" s="1"/>
     </row>
     <row r="144" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
-        <v>392</v>
+        <v>366</v>
       </c>
       <c r="B144" s="1" t="s">
-        <v>393</v>
+        <v>367</v>
       </c>
       <c r="C144" s="1"/>
       <c r="D144" s="1"/>
@@ -24672,7 +24868,7 @@
         <v>0</v>
       </c>
       <c r="I144" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J144" s="1"/>
       <c r="K144" s="1"/>
@@ -24682,10 +24878,10 @@
     </row>
     <row r="145" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
-        <v>394</v>
+        <v>378</v>
       </c>
       <c r="B145" s="1" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="C145" s="1"/>
       <c r="D145" s="1"/>
@@ -24698,24 +24894,20 @@
         <v>0</v>
       </c>
       <c r="I145" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J145" s="1"/>
       <c r="K145" s="1"/>
       <c r="L145" s="1"/>
-      <c r="M145" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="N145" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="M145" s="1"/>
+      <c r="N145" s="1"/>
     </row>
     <row r="146" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
-        <v>396</v>
+        <v>384</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>397</v>
+        <v>385</v>
       </c>
       <c r="C146" s="1"/>
       <c r="D146" s="1"/>
@@ -24728,7 +24920,7 @@
         <v>0</v>
       </c>
       <c r="I146" s="1" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
       <c r="J146" s="1"/>
       <c r="K146" s="1"/>
@@ -24738,6 +24930,9 @@
     </row>
   </sheetData>
   <autoFilter ref="A2:N146"/>
+  <sortState ref="A4:N146">
+    <sortCondition ref="I4:I146"/>
+  </sortState>
   <mergeCells count="1">
     <mergeCell ref="C2:H2"/>
   </mergeCells>
@@ -24750,13 +24945,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="C95" sqref="C95"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="C79" sqref="C79"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <pane ySplit="1040" topLeftCell="A57" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="C63" sqref="C63"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -27441,14 +27633,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L128"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C65" sqref="C65"/>
+    <sheetView topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K68" sqref="K68"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <pane ySplit="1300" topLeftCell="A88" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="G119" sqref="G119"/>
-    </sheetView>
+    <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
add approximate MWs of mRNAs, based on "WHICH IS BIGGER, MRNA OR THE PROTEIN IT CODES FOR?" in "Cell biology by the numbers", 2015
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4787" uniqueCount="2098">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4854" uniqueCount="2104">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -6722,6 +6722,24 @@
   </si>
   <si>
     <t>URL: https://academic.oup.com/nar/article-pdf/24/22/4420/7069676/24-22-4420.pdf</t>
+  </si>
+  <si>
+    <t>Ref_0023</t>
+  </si>
+  <si>
+    <t>milo2015cell</t>
+  </si>
+  <si>
+    <t>Cell biology by the numbers</t>
+  </si>
+  <si>
+    <t>Milo, Ron and Phillips, Rob</t>
+  </si>
+  <si>
+    <t>Approx. MW, 10x proteins</t>
+  </si>
+  <si>
+    <t>WHICH IS BIGGER, MRNA OR THE PROTEIN IT CODES FOR?</t>
   </si>
 </sst>
 </file>
@@ -6833,9 +6851,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -6961,10 +6980,11 @@
       <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Explanatory Text" xfId="1" builtinId="53"/>
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -19264,14 +19284,14 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R24"/>
+  <dimension ref="A1:R36"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C30" sqref="C30:C43"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19288,7 +19308,8 @@
     <col min="10" max="10" width="8.6640625" style="3" customWidth="1"/>
     <col min="11" max="11" width="4.1640625" style="3" customWidth="1"/>
     <col min="12" max="12" width="7.33203125" style="3" customWidth="1"/>
-    <col min="13" max="15" width="8.6640625" style="3" customWidth="1"/>
+    <col min="13" max="14" width="8.6640625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="26.83203125" style="3" customWidth="1"/>
     <col min="16" max="16" width="8.1640625" style="3" customWidth="1"/>
     <col min="17" max="17" width="46.5" style="3" customWidth="1"/>
     <col min="18" max="18" width="8.6640625" style="3" customWidth="1"/>
@@ -20152,6 +20173,61 @@
       <c r="Q24" s="3" t="s">
         <v>2097</v>
       </c>
+    </row>
+    <row r="25" spans="1:18" ht="43" x14ac:dyDescent="0.2">
+      <c r="A25" s="25" t="s">
+        <v>2098</v>
+      </c>
+      <c r="B25" s="25" t="s">
+        <v>2099</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>2100</v>
+      </c>
+      <c r="D25" s="25" t="s">
+        <v>2101</v>
+      </c>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25">
+        <v>2015</v>
+      </c>
+      <c r="G25" s="25" t="s">
+        <v>1865</v>
+      </c>
+      <c r="H25" s="25"/>
+      <c r="I25" s="25" t="s">
+        <v>1866</v>
+      </c>
+      <c r="O25" s="3" t="s">
+        <v>2103</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C28" s="25"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C29" s="25"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C30" s="25"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C32" s="25"/>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" s="25"/>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" s="25"/>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" s="25"/>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C36" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:R23"/>
@@ -20795,8 +20871,8 @@
   <dimension ref="A1:N146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1600" topLeftCell="A84" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="M116" sqref="M87:N116"/>
+      <pane ySplit="1600" topLeftCell="A109" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="M117" sqref="M117:M146"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -24159,8 +24235,8 @@
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
-      <c r="G117" s="39">
-        <v>10</v>
+      <c r="G117" s="41">
+        <v>400000</v>
       </c>
       <c r="H117" s="22">
         <v>0</v>
@@ -24171,8 +24247,12 @@
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
       <c r="L117" s="1"/>
-      <c r="M117" s="1"/>
-      <c r="N117" s="1"/>
+      <c r="M117" s="1" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N117" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="118" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
@@ -24185,8 +24265,8 @@
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
-      <c r="G118" s="39">
-        <v>10</v>
+      <c r="G118" s="41">
+        <v>400000</v>
       </c>
       <c r="H118" s="22">
         <v>0</v>
@@ -24197,8 +24277,12 @@
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
       <c r="L118" s="1"/>
-      <c r="M118" s="1"/>
-      <c r="N118" s="1"/>
+      <c r="M118" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N118" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="119" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
@@ -24211,8 +24295,8 @@
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
-      <c r="G119" s="39">
-        <v>10</v>
+      <c r="G119" s="41">
+        <v>400000</v>
       </c>
       <c r="H119" s="22">
         <v>0</v>
@@ -24223,8 +24307,12 @@
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
       <c r="L119" s="1"/>
-      <c r="M119" s="1"/>
-      <c r="N119" s="1"/>
+      <c r="M119" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N119" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="120" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
@@ -24237,8 +24325,8 @@
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
-      <c r="G120" s="39">
-        <v>10</v>
+      <c r="G120" s="41">
+        <v>400000</v>
       </c>
       <c r="H120" s="22">
         <v>0</v>
@@ -24249,8 +24337,12 @@
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
       <c r="L120" s="1"/>
-      <c r="M120" s="1"/>
-      <c r="N120" s="1"/>
+      <c r="M120" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N120" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="121" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
@@ -24263,8 +24355,8 @@
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
-      <c r="G121" s="39">
-        <v>10</v>
+      <c r="G121" s="41">
+        <v>400000</v>
       </c>
       <c r="H121" s="22">
         <v>0</v>
@@ -24275,8 +24367,12 @@
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
       <c r="L121" s="1"/>
-      <c r="M121" s="1"/>
-      <c r="N121" s="1"/>
+      <c r="M121" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N121" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="122" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
@@ -24289,8 +24385,8 @@
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
-      <c r="G122" s="39">
-        <v>10</v>
+      <c r="G122" s="41">
+        <v>400000</v>
       </c>
       <c r="H122" s="22">
         <v>0</v>
@@ -24301,8 +24397,12 @@
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
       <c r="L122" s="1"/>
-      <c r="M122" s="1"/>
-      <c r="N122" s="1"/>
+      <c r="M122" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N122" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="123" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
@@ -24315,8 +24415,8 @@
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
-      <c r="G123" s="39">
-        <v>10</v>
+      <c r="G123" s="41">
+        <v>400000</v>
       </c>
       <c r="H123" s="22">
         <v>0</v>
@@ -24327,8 +24427,12 @@
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
       <c r="L123" s="1"/>
-      <c r="M123" s="1"/>
-      <c r="N123" s="1"/>
+      <c r="M123" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N123" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="124" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
@@ -24341,8 +24445,8 @@
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
-      <c r="G124" s="39">
-        <v>10</v>
+      <c r="G124" s="41">
+        <v>400000</v>
       </c>
       <c r="H124" s="22">
         <v>0</v>
@@ -24353,8 +24457,12 @@
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
       <c r="L124" s="1"/>
-      <c r="M124" s="1"/>
-      <c r="N124" s="1"/>
+      <c r="M124" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N124" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="125" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
@@ -24367,8 +24475,8 @@
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
-      <c r="G125" s="39">
-        <v>10</v>
+      <c r="G125" s="41">
+        <v>400000</v>
       </c>
       <c r="H125" s="22">
         <v>0</v>
@@ -24379,8 +24487,12 @@
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
       <c r="L125" s="1"/>
-      <c r="M125" s="1"/>
-      <c r="N125" s="1"/>
+      <c r="M125" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N125" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="126" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
@@ -24393,8 +24505,8 @@
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
-      <c r="G126" s="39">
-        <v>10</v>
+      <c r="G126" s="41">
+        <v>400000</v>
       </c>
       <c r="H126" s="22">
         <v>0</v>
@@ -24405,8 +24517,12 @@
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
       <c r="L126" s="1"/>
-      <c r="M126" s="1"/>
-      <c r="N126" s="1"/>
+      <c r="M126" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N126" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="127" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
@@ -24419,8 +24535,8 @@
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
-      <c r="G127" s="39">
-        <v>10</v>
+      <c r="G127" s="41">
+        <v>400000</v>
       </c>
       <c r="H127" s="22">
         <v>0</v>
@@ -24431,8 +24547,12 @@
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
       <c r="L127" s="1"/>
-      <c r="M127" s="1"/>
-      <c r="N127" s="1"/>
+      <c r="M127" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N127" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="128" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
@@ -24445,8 +24565,8 @@
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
-      <c r="G128" s="39">
-        <v>10</v>
+      <c r="G128" s="41">
+        <v>400000</v>
       </c>
       <c r="H128" s="22">
         <v>0</v>
@@ -24457,8 +24577,12 @@
       <c r="J128" s="1"/>
       <c r="K128" s="1"/>
       <c r="L128" s="1"/>
-      <c r="M128" s="1"/>
-      <c r="N128" s="1"/>
+      <c r="M128" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N128" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="129" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
@@ -24471,8 +24595,8 @@
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
-      <c r="G129" s="39">
-        <v>10</v>
+      <c r="G129" s="41">
+        <v>400000</v>
       </c>
       <c r="H129" s="22">
         <v>0</v>
@@ -24483,8 +24607,12 @@
       <c r="J129" s="1"/>
       <c r="K129" s="1"/>
       <c r="L129" s="1"/>
-      <c r="M129" s="1"/>
-      <c r="N129" s="1"/>
+      <c r="M129" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N129" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="130" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
@@ -24497,8 +24625,8 @@
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
-      <c r="G130" s="39">
-        <v>10</v>
+      <c r="G130" s="41">
+        <v>400000</v>
       </c>
       <c r="H130" s="22">
         <v>0</v>
@@ -24509,8 +24637,12 @@
       <c r="J130" s="1"/>
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
-      <c r="M130" s="1"/>
-      <c r="N130" s="1"/>
+      <c r="M130" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N130" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="131" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
@@ -24523,8 +24655,8 @@
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
-      <c r="G131" s="39">
-        <v>10</v>
+      <c r="G131" s="41">
+        <v>400000</v>
       </c>
       <c r="H131" s="22">
         <v>0</v>
@@ -24535,8 +24667,12 @@
       <c r="J131" s="1"/>
       <c r="K131" s="1"/>
       <c r="L131" s="1"/>
-      <c r="M131" s="1"/>
-      <c r="N131" s="1"/>
+      <c r="M131" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N131" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="132" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
@@ -24549,8 +24685,8 @@
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
-      <c r="G132" s="39">
-        <v>10</v>
+      <c r="G132" s="41">
+        <v>400000</v>
       </c>
       <c r="H132" s="22">
         <v>0</v>
@@ -24561,8 +24697,12 @@
       <c r="J132" s="1"/>
       <c r="K132" s="1"/>
       <c r="L132" s="1"/>
-      <c r="M132" s="1"/>
-      <c r="N132" s="1"/>
+      <c r="M132" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N132" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="133" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
@@ -24575,8 +24715,8 @@
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
-      <c r="G133" s="39">
-        <v>10</v>
+      <c r="G133" s="41">
+        <v>400000</v>
       </c>
       <c r="H133" s="22">
         <v>0</v>
@@ -24587,8 +24727,12 @@
       <c r="J133" s="1"/>
       <c r="K133" s="1"/>
       <c r="L133" s="1"/>
-      <c r="M133" s="1"/>
-      <c r="N133" s="1"/>
+      <c r="M133" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N133" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="134" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
@@ -24601,8 +24745,8 @@
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
-      <c r="G134" s="39">
-        <v>10</v>
+      <c r="G134" s="41">
+        <v>400000</v>
       </c>
       <c r="H134" s="22">
         <v>0</v>
@@ -24613,8 +24757,12 @@
       <c r="J134" s="1"/>
       <c r="K134" s="1"/>
       <c r="L134" s="1"/>
-      <c r="M134" s="1"/>
-      <c r="N134" s="1"/>
+      <c r="M134" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N134" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="135" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
@@ -24627,8 +24775,8 @@
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
-      <c r="G135" s="39">
-        <v>10</v>
+      <c r="G135" s="41">
+        <v>400000</v>
       </c>
       <c r="H135" s="22">
         <v>0</v>
@@ -24639,8 +24787,12 @@
       <c r="J135" s="1"/>
       <c r="K135" s="1"/>
       <c r="L135" s="1"/>
-      <c r="M135" s="1"/>
-      <c r="N135" s="1"/>
+      <c r="M135" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N135" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="136" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
@@ -24653,8 +24805,8 @@
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
-      <c r="G136" s="39">
-        <v>10</v>
+      <c r="G136" s="41">
+        <v>400000</v>
       </c>
       <c r="H136" s="22">
         <v>0</v>
@@ -24665,8 +24817,12 @@
       <c r="J136" s="1"/>
       <c r="K136" s="1"/>
       <c r="L136" s="1"/>
-      <c r="M136" s="1"/>
-      <c r="N136" s="1"/>
+      <c r="M136" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N136" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="137" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
@@ -24679,8 +24835,8 @@
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
-      <c r="G137" s="39">
-        <v>10</v>
+      <c r="G137" s="41">
+        <v>400000</v>
       </c>
       <c r="H137" s="22">
         <v>0</v>
@@ -24691,8 +24847,12 @@
       <c r="J137" s="1"/>
       <c r="K137" s="1"/>
       <c r="L137" s="1"/>
-      <c r="M137" s="1"/>
-      <c r="N137" s="1"/>
+      <c r="M137" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N137" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="138" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
@@ -24705,8 +24865,8 @@
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
-      <c r="G138" s="39">
-        <v>10</v>
+      <c r="G138" s="41">
+        <v>400000</v>
       </c>
       <c r="H138" s="22">
         <v>0</v>
@@ -24717,8 +24877,12 @@
       <c r="J138" s="1"/>
       <c r="K138" s="1"/>
       <c r="L138" s="1"/>
-      <c r="M138" s="1"/>
-      <c r="N138" s="1"/>
+      <c r="M138" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N138" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="139" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
@@ -24731,8 +24895,8 @@
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
-      <c r="G139" s="39">
-        <v>10</v>
+      <c r="G139" s="41">
+        <v>400000</v>
       </c>
       <c r="H139" s="22">
         <v>0</v>
@@ -24743,8 +24907,12 @@
       <c r="J139" s="1"/>
       <c r="K139" s="1"/>
       <c r="L139" s="1"/>
-      <c r="M139" s="1"/>
-      <c r="N139" s="1"/>
+      <c r="M139" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N139" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="140" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
@@ -24757,8 +24925,8 @@
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
-      <c r="G140" s="39">
-        <v>10</v>
+      <c r="G140" s="41">
+        <v>400000</v>
       </c>
       <c r="H140" s="22">
         <v>0</v>
@@ -24769,8 +24937,12 @@
       <c r="J140" s="1"/>
       <c r="K140" s="1"/>
       <c r="L140" s="1"/>
-      <c r="M140" s="1"/>
-      <c r="N140" s="1"/>
+      <c r="M140" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N140" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="141" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
@@ -24783,8 +24955,8 @@
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
-      <c r="G141" s="39">
-        <v>10</v>
+      <c r="G141" s="41">
+        <v>400000</v>
       </c>
       <c r="H141" s="22">
         <v>0</v>
@@ -24795,8 +24967,12 @@
       <c r="J141" s="1"/>
       <c r="K141" s="1"/>
       <c r="L141" s="1"/>
-      <c r="M141" s="1"/>
-      <c r="N141" s="1"/>
+      <c r="M141" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N141" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="142" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
@@ -24809,8 +24985,8 @@
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
-      <c r="G142" s="39">
-        <v>10</v>
+      <c r="G142" s="41">
+        <v>400000</v>
       </c>
       <c r="H142" s="22">
         <v>0</v>
@@ -24821,8 +24997,12 @@
       <c r="J142" s="1"/>
       <c r="K142" s="1"/>
       <c r="L142" s="1"/>
-      <c r="M142" s="1"/>
-      <c r="N142" s="1"/>
+      <c r="M142" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N142" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="143" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
@@ -24835,8 +25015,8 @@
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
-      <c r="G143" s="39">
-        <v>10</v>
+      <c r="G143" s="41">
+        <v>400000</v>
       </c>
       <c r="H143" s="22">
         <v>0</v>
@@ -24847,8 +25027,12 @@
       <c r="J143" s="1"/>
       <c r="K143" s="1"/>
       <c r="L143" s="1"/>
-      <c r="M143" s="1"/>
-      <c r="N143" s="1"/>
+      <c r="M143" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N143" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="144" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
@@ -24861,8 +25045,8 @@
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
-      <c r="G144" s="39">
-        <v>10</v>
+      <c r="G144" s="41">
+        <v>400000</v>
       </c>
       <c r="H144" s="22">
         <v>0</v>
@@ -24873,8 +25057,12 @@
       <c r="J144" s="1"/>
       <c r="K144" s="1"/>
       <c r="L144" s="1"/>
-      <c r="M144" s="1"/>
-      <c r="N144" s="1"/>
+      <c r="M144" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N144" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
     <row r="145" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
@@ -24887,8 +25075,8 @@
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
-      <c r="G145" s="39">
-        <v>10</v>
+      <c r="G145" s="41">
+        <v>400000</v>
       </c>
       <c r="H145" s="22">
         <v>0</v>
@@ -24899,10 +25087,14 @@
       <c r="J145" s="1"/>
       <c r="K145" s="1"/>
       <c r="L145" s="1"/>
-      <c r="M145" s="1"/>
-      <c r="N145" s="1"/>
-    </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="M145" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N145" s="25" t="s">
+        <v>2098</v>
+      </c>
+    </row>
+    <row r="146" spans="1:14" ht="42" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>384</v>
       </c>
@@ -24913,8 +25105,8 @@
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
-      <c r="G146" s="39">
-        <v>10</v>
+      <c r="G146" s="41">
+        <v>400000</v>
       </c>
       <c r="H146" s="22">
         <v>0</v>
@@ -24925,8 +25117,12 @@
       <c r="J146" s="1"/>
       <c r="K146" s="1"/>
       <c r="L146" s="1"/>
-      <c r="M146" s="1"/>
-      <c r="N146" s="1"/>
+      <c r="M146" s="26" t="s">
+        <v>2102</v>
+      </c>
+      <c r="N146" s="25" t="s">
+        <v>2098</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:N146"/>

</xml_diff>

<commit_message>
update species type structures, esp. MW & formulas
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-27900" yWindow="640" windowWidth="25500" windowHeight="19940" tabRatio="500" activeTab="6"/>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="35320" windowHeight="19700" tabRatio="500" firstSheet="11" activeTab="21"/>
+    <workbookView xWindow="-28820" yWindow="1580" windowWidth="27420" windowHeight="19400" tabRatio="500" activeTab="6"/>
+    <workbookView minimized="1" xWindow="640" yWindow="1180" windowWidth="35320" windowHeight="19700" tabRatio="500" firstSheet="5" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4854" uniqueCount="2104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4860" uniqueCount="2109">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -6740,6 +6740,21 @@
   </si>
   <si>
     <t>WHICH IS BIGGER, MRNA OR THE PROTEIN IT CODES FOR?</t>
+  </si>
+  <si>
+    <t>C5H13O14P3</t>
+  </si>
+  <si>
+    <t>C5H11O8P</t>
+  </si>
+  <si>
+    <t>C7H13O10P</t>
+  </si>
+  <si>
+    <t>Name not in PubChem or ChEBI</t>
+  </si>
+  <si>
+    <t>C3H7O6P</t>
   </si>
 </sst>
 </file>
@@ -6858,7 +6873,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -6945,18 +6960,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -6978,6 +6981,21 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -7960,9 +7978,9 @@
   <dimension ref="A1:N178"/>
   <sheetViews>
     <sheetView topLeftCell="B3" workbookViewId="0">
-      <pane ySplit="740" topLeftCell="A41" activePane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="D52" sqref="D52"/>
+      <selection pane="bottomLeft" activeCell="D108" sqref="D108"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -7984,11 +8002,11 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="33" t="s">
+      <c r="G2" s="40" t="s">
         <v>721</v>
       </c>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -12908,9 +12926,9 @@
   <dimension ref="A1:L169"/>
   <sheetViews>
     <sheetView topLeftCell="A2" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="880" topLeftCell="A143" activePane="bottomLeft"/>
+      <pane ySplit="880" topLeftCell="A77" activePane="bottomLeft"/>
       <selection activeCell="B2" sqref="B1:B1048576"/>
-      <selection pane="bottomLeft" activeCell="A158" sqref="A158"/>
+      <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -12991,7 +13009,7 @@
       <c r="G3" s="1" t="s">
         <v>731</v>
       </c>
-      <c r="K3" s="40" t="s">
+      <c r="K3" s="36" t="s">
         <v>2048</v>
       </c>
     </row>
@@ -16797,8 +16815,8 @@
   <dimension ref="A1:K94"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A65" sqref="A65:XFD65"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -18632,26 +18650,26 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="41" t="s">
         <v>1747</v>
       </c>
-      <c r="H2" s="35"/>
-      <c r="I2" s="34" t="s">
+      <c r="H2" s="42"/>
+      <c r="I2" s="41" t="s">
         <v>1748</v>
       </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="35"/>
-      <c r="L2" s="35"/>
-      <c r="M2" s="35"/>
-      <c r="N2" s="35"/>
-      <c r="Q2" s="34" t="s">
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="L2" s="42"/>
+      <c r="M2" s="42"/>
+      <c r="N2" s="42"/>
+      <c r="Q2" s="41" t="s">
         <v>1749</v>
       </c>
-      <c r="R2" s="35"/>
-      <c r="S2" s="34" t="s">
+      <c r="R2" s="42"/>
+      <c r="S2" s="41" t="s">
         <v>1750</v>
       </c>
-      <c r="T2" s="35"/>
+      <c r="T2" s="42"/>
     </row>
     <row r="3" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -19150,10 +19168,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="34" t="s">
+      <c r="G2" s="41" t="s">
         <v>1797</v>
       </c>
-      <c r="H2" s="35"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -19289,9 +19307,9 @@
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="C14" sqref="C14"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView workbookViewId="1">
       <pane ySplit="2" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25:XFD25"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20641,7 +20659,9 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -20661,18 +20681,18 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H2" s="31" t="s">
+      <c r="H2" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="M2" s="31" t="s">
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="M2" s="38" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
     </row>
     <row r="3" spans="1:21" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -20871,8 +20891,8 @@
   <dimension ref="A1:N146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1600" topLeftCell="A109" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="M117" sqref="M117:M146"/>
+      <pane ySplit="1600" topLeftCell="A36" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -20884,7 +20904,7 @@
     <col min="4" max="4" width="7.83203125" style="3" hidden="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" style="3" hidden="1" customWidth="1"/>
     <col min="6" max="6" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5" style="36" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5" style="32" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="3" bestFit="1" customWidth="1"/>
     <col min="10" max="14" width="8.6640625" style="3" customWidth="1"/>
@@ -20897,14 +20917,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="38" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -20925,7 +20945,7 @@
       <c r="F3" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="G3" s="37" t="s">
+      <c r="G3" s="33" t="s">
         <v>107</v>
       </c>
       <c r="H3" s="2" t="s">
@@ -20967,7 +20987,7 @@
       <c r="F4" s="19" t="s">
         <v>1973</v>
       </c>
-      <c r="G4" s="38">
+      <c r="G4" s="34">
         <v>135.13</v>
       </c>
       <c r="H4" s="19">
@@ -20999,7 +21019,7 @@
       <c r="F5" s="1" t="s">
         <v>1974</v>
       </c>
-      <c r="G5" s="39">
+      <c r="G5" s="35">
         <v>427.2</v>
       </c>
       <c r="H5" s="22">
@@ -21027,7 +21047,7 @@
       <c r="F6" s="1" t="s">
         <v>1975</v>
       </c>
-      <c r="G6" s="39">
+      <c r="G6" s="35">
         <v>89.09</v>
       </c>
       <c r="H6" s="22">
@@ -21055,7 +21075,7 @@
       <c r="F7" s="1" t="s">
         <v>1976</v>
       </c>
-      <c r="G7" s="39">
+      <c r="G7" s="35">
         <v>160.16999999999999</v>
       </c>
       <c r="H7" s="22">
@@ -21087,7 +21107,7 @@
       <c r="F8" s="26" t="s">
         <v>1977</v>
       </c>
-      <c r="G8" s="39">
+      <c r="G8" s="35">
         <v>347.22</v>
       </c>
       <c r="H8" s="22">
@@ -21115,7 +21135,7 @@
       <c r="F9" s="26" t="s">
         <v>1978</v>
       </c>
-      <c r="G9" s="39">
+      <c r="G9" s="35">
         <v>174.2</v>
       </c>
       <c r="H9" s="22">
@@ -21143,7 +21163,7 @@
       <c r="F10" s="26" t="s">
         <v>1979</v>
       </c>
-      <c r="G10" s="39">
+      <c r="G10" s="35">
         <v>330.39</v>
       </c>
       <c r="H10" s="22">
@@ -21175,7 +21195,7 @@
       <c r="F11" s="1" t="s">
         <v>1980</v>
       </c>
-      <c r="G11" s="39">
+      <c r="G11" s="35">
         <v>133.1</v>
       </c>
       <c r="H11" s="22">
@@ -21203,7 +21223,7 @@
       <c r="F12" s="1" t="s">
         <v>1981</v>
       </c>
-      <c r="G12" s="39">
+      <c r="G12" s="35">
         <v>246.22</v>
       </c>
       <c r="H12" s="22">
@@ -21233,7 +21253,7 @@
       <c r="F13" s="26" t="s">
         <v>1982</v>
       </c>
-      <c r="G13" s="39">
+      <c r="G13" s="35">
         <v>132.12</v>
       </c>
       <c r="H13" s="22">
@@ -21261,7 +21281,7 @@
       <c r="F14" s="26" t="s">
         <v>1983</v>
       </c>
-      <c r="G14" s="39">
+      <c r="G14" s="35">
         <v>248.19</v>
       </c>
       <c r="H14" s="22">
@@ -21293,7 +21313,7 @@
       <c r="F15" s="26" t="s">
         <v>1984</v>
       </c>
-      <c r="G15" s="39">
+      <c r="G15" s="35">
         <v>507.18</v>
       </c>
       <c r="H15" s="22">
@@ -21321,7 +21341,7 @@
       <c r="F16" s="26" t="s">
         <v>1985</v>
       </c>
-      <c r="G16" s="39">
+      <c r="G16" s="35">
         <v>403.18</v>
       </c>
       <c r="H16" s="22">
@@ -21349,7 +21369,7 @@
       <c r="F17" s="26" t="s">
         <v>1986</v>
       </c>
-      <c r="G17" s="39">
+      <c r="G17" s="35">
         <v>323.2</v>
       </c>
       <c r="H17" s="22">
@@ -21377,7 +21397,7 @@
       <c r="F18" s="26" t="s">
         <v>151</v>
       </c>
-      <c r="G18" s="39">
+      <c r="G18" s="35">
         <v>44.009</v>
       </c>
       <c r="H18" s="22">
@@ -21409,7 +21429,7 @@
       <c r="F19" s="26" t="s">
         <v>1987</v>
       </c>
-      <c r="G19" s="39">
+      <c r="G19" s="35">
         <v>483.16</v>
       </c>
       <c r="H19" s="22">
@@ -21437,7 +21457,7 @@
       <c r="F20" s="26" t="s">
         <v>1988</v>
       </c>
-      <c r="G20" s="39">
+      <c r="G20" s="35">
         <v>121.16</v>
       </c>
       <c r="H20" s="22">
@@ -21465,7 +21485,7 @@
       <c r="F21" s="1" t="s">
         <v>1989</v>
       </c>
-      <c r="G21" s="39">
+      <c r="G21" s="35">
         <v>224.3</v>
       </c>
       <c r="H21" s="22">
@@ -21497,7 +21517,7 @@
       <c r="F22" s="1" t="s">
         <v>1990</v>
       </c>
-      <c r="G22" s="39">
+      <c r="G22" s="35">
         <v>243.22</v>
       </c>
       <c r="H22" s="22">
@@ -21527,7 +21547,7 @@
       <c r="F23" s="26" t="s">
         <v>1991</v>
       </c>
-      <c r="G23" s="39">
+      <c r="G23" s="35">
         <v>266.04000000000002</v>
       </c>
       <c r="H23" s="22">
@@ -21555,7 +21575,7 @@
       <c r="F24" s="1" t="s">
         <v>1992</v>
       </c>
-      <c r="G24" s="39">
+      <c r="G24" s="35">
         <v>200.08</v>
       </c>
       <c r="H24" s="22">
@@ -21583,7 +21603,7 @@
       <c r="F25" s="26" t="s">
         <v>1993</v>
       </c>
-      <c r="G25" s="39">
+      <c r="G25" s="35">
         <v>260.14</v>
       </c>
       <c r="H25" s="22">
@@ -21611,7 +21631,7 @@
       <c r="F26" s="26" t="s">
         <v>1994</v>
       </c>
-      <c r="G26" s="39">
+      <c r="G26" s="35">
         <v>340.12</v>
       </c>
       <c r="H26" s="22">
@@ -21639,7 +21659,7 @@
       <c r="F27" s="26" t="s">
         <v>1995</v>
       </c>
-      <c r="G27" s="39">
+      <c r="G27" s="35">
         <v>186.06</v>
       </c>
       <c r="H27" s="22">
@@ -21667,7 +21687,7 @@
       <c r="F28" s="26" t="s">
         <v>1995</v>
       </c>
-      <c r="G28" s="39">
+      <c r="G28" s="35">
         <v>186.06</v>
       </c>
       <c r="H28" s="22">
@@ -21695,7 +21715,7 @@
       <c r="F29" s="26" t="s">
         <v>1993</v>
       </c>
-      <c r="G29" s="39">
+      <c r="G29" s="35">
         <v>260.14</v>
       </c>
       <c r="H29" s="22">
@@ -21725,7 +21745,7 @@
       <c r="F30" s="26" t="s">
         <v>1996</v>
       </c>
-      <c r="G30" s="39">
+      <c r="G30" s="35">
         <v>443.2</v>
       </c>
       <c r="H30" s="22">
@@ -21753,7 +21773,7 @@
       <c r="F31" s="1" t="s">
         <v>1997</v>
       </c>
-      <c r="G31" s="39">
+      <c r="G31" s="35">
         <v>180.16</v>
       </c>
       <c r="H31" s="22">
@@ -21785,7 +21805,7 @@
       <c r="F32" s="1" t="s">
         <v>1998</v>
       </c>
-      <c r="G32" s="39">
+      <c r="G32" s="35">
         <v>146.13999999999999</v>
       </c>
       <c r="H32" s="22">
@@ -21813,7 +21833,7 @@
       <c r="F33" s="26" t="s">
         <v>1999</v>
       </c>
-      <c r="G33" s="39">
+      <c r="G33" s="35">
         <v>274.27</v>
       </c>
       <c r="H33" s="22">
@@ -21845,7 +21865,7 @@
       <c r="F34" s="1" t="s">
         <v>2000</v>
       </c>
-      <c r="G34" s="39">
+      <c r="G34" s="35">
         <v>147.13</v>
       </c>
       <c r="H34" s="22">
@@ -21873,7 +21893,7 @@
       <c r="F35" s="1" t="s">
         <v>2001</v>
       </c>
-      <c r="G35" s="39">
+      <c r="G35" s="35">
         <v>276.24</v>
       </c>
       <c r="H35" s="22">
@@ -21905,7 +21925,7 @@
       <c r="F36" s="26" t="s">
         <v>2002</v>
       </c>
-      <c r="G36" s="39">
+      <c r="G36" s="35">
         <v>75.069999999999993</v>
       </c>
       <c r="H36" s="22">
@@ -21931,7 +21951,7 @@
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
       <c r="F37" s="26"/>
-      <c r="G37" s="39">
+      <c r="G37" s="35">
         <v>10</v>
       </c>
       <c r="H37" s="22">
@@ -21963,7 +21983,7 @@
       <c r="F38" s="26" t="s">
         <v>2003</v>
       </c>
-      <c r="G38" s="39">
+      <c r="G38" s="35">
         <v>363.22</v>
       </c>
       <c r="H38" s="22">
@@ -21991,7 +22011,7 @@
       <c r="F39" s="26" t="s">
         <v>2004</v>
       </c>
-      <c r="G39" s="39">
+      <c r="G39" s="35">
         <v>151.13</v>
       </c>
       <c r="H39" s="22">
@@ -22023,7 +22043,7 @@
       <c r="F40" s="1" t="s">
         <v>2005</v>
       </c>
-      <c r="G40" s="39">
+      <c r="G40" s="35">
         <v>523.17899999999997</v>
       </c>
       <c r="H40" s="22">
@@ -22051,7 +22071,7 @@
       <c r="F41" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="G41" s="39">
+      <c r="G41" s="35">
         <v>1.008</v>
       </c>
       <c r="H41" s="22">
@@ -22081,7 +22101,7 @@
       <c r="F42" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="G42" s="39">
+      <c r="G42" s="35">
         <v>18.015000000000001</v>
       </c>
       <c r="H42" s="22">
@@ -22113,7 +22133,7 @@
       <c r="F43" s="1" t="s">
         <v>2006</v>
       </c>
-      <c r="G43" s="39">
+      <c r="G43" s="35">
         <v>155.15</v>
       </c>
       <c r="H43" s="22">
@@ -22141,7 +22161,7 @@
       <c r="F44" s="1" t="s">
         <v>2007</v>
       </c>
-      <c r="G44" s="39">
+      <c r="G44" s="35">
         <v>292.29000000000002</v>
       </c>
       <c r="H44" s="22">
@@ -22173,7 +22193,7 @@
       <c r="F45" s="26" t="s">
         <v>2008</v>
       </c>
-      <c r="G45" s="39">
+      <c r="G45" s="35">
         <v>131.16999999999999</v>
       </c>
       <c r="H45" s="22">
@@ -22199,7 +22219,7 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
       <c r="F46" s="26"/>
-      <c r="G46" s="39">
+      <c r="G46" s="35">
         <v>10</v>
       </c>
       <c r="H46" s="22">
@@ -22231,7 +22251,7 @@
       <c r="F47" s="26" t="s">
         <v>2087</v>
       </c>
-      <c r="G47" s="39">
+      <c r="G47" s="35">
         <v>90.08</v>
       </c>
       <c r="H47" s="22">
@@ -22257,7 +22277,7 @@
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
       <c r="F48" s="26"/>
-      <c r="G48" s="39">
+      <c r="G48" s="35">
         <v>10</v>
       </c>
       <c r="H48" s="22">
@@ -22283,7 +22303,7 @@
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="26"/>
-      <c r="G49" s="39">
+      <c r="G49" s="35">
         <v>10</v>
       </c>
       <c r="H49" s="22">
@@ -22313,7 +22333,7 @@
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
       <c r="F50" s="26"/>
-      <c r="G50" s="39">
+      <c r="G50" s="35">
         <v>10</v>
       </c>
       <c r="H50" s="22">
@@ -22339,7 +22359,7 @@
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
-      <c r="G51" s="39">
+      <c r="G51" s="35">
         <v>10</v>
       </c>
       <c r="H51" s="22">
@@ -22369,7 +22389,7 @@
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
       <c r="F52" s="26"/>
-      <c r="G52" s="39">
+      <c r="G52" s="35">
         <v>10</v>
       </c>
       <c r="H52" s="22">
@@ -22395,7 +22415,7 @@
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="26"/>
-      <c r="G53" s="39">
+      <c r="G53" s="35">
         <v>10</v>
       </c>
       <c r="H53" s="22">
@@ -22427,7 +22447,7 @@
       <c r="F54" s="26" t="s">
         <v>2088</v>
       </c>
-      <c r="G54" s="39">
+      <c r="G54" s="35">
         <v>664.4</v>
       </c>
       <c r="H54" s="22">
@@ -22459,7 +22479,7 @@
       <c r="F55" s="1" t="s">
         <v>2089</v>
       </c>
-      <c r="G55" s="39">
+      <c r="G55" s="35">
         <v>665.4</v>
       </c>
       <c r="H55" s="22">
@@ -22487,7 +22507,7 @@
       <c r="F56" s="26" t="s">
         <v>261</v>
       </c>
-      <c r="G56" s="39">
+      <c r="G56" s="35">
         <v>31.998999999999999</v>
       </c>
       <c r="H56" s="22">
@@ -22517,7 +22537,7 @@
       <c r="D57" s="1"/>
       <c r="E57" s="1"/>
       <c r="F57" s="26"/>
-      <c r="G57" s="39">
+      <c r="G57" s="35">
         <v>10</v>
       </c>
       <c r="H57" s="22">
@@ -22543,7 +22563,7 @@
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
       <c r="F58" s="26"/>
-      <c r="G58" s="39">
+      <c r="G58" s="35">
         <v>10</v>
       </c>
       <c r="H58" s="22">
@@ -22569,7 +22589,7 @@
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
-      <c r="G59" s="39">
+      <c r="G59" s="35">
         <v>10</v>
       </c>
       <c r="H59" s="22">
@@ -22599,7 +22619,7 @@
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
-      <c r="G60" s="39">
+      <c r="G60" s="35">
         <v>10</v>
       </c>
       <c r="H60" s="22">
@@ -22627,7 +22647,7 @@
       <c r="D61" s="1"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
-      <c r="G61" s="39">
+      <c r="G61" s="35">
         <v>10</v>
       </c>
       <c r="H61" s="22">
@@ -22653,7 +22673,7 @@
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
-      <c r="G62" s="39">
+      <c r="G62" s="35">
         <v>10</v>
       </c>
       <c r="H62" s="22">
@@ -22679,7 +22699,7 @@
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="26"/>
-      <c r="G63" s="39">
+      <c r="G63" s="35">
         <v>10</v>
       </c>
       <c r="H63" s="22">
@@ -22708,9 +22728,11 @@
       <c r="C64" s="1"/>
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="39">
-        <v>10</v>
+      <c r="F64" s="26" t="s">
+        <v>2104</v>
+      </c>
+      <c r="G64" s="35">
+        <v>390.07</v>
       </c>
       <c r="H64" s="22">
         <v>0</v>
@@ -22735,7 +22757,7 @@
       <c r="D65" s="1"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
-      <c r="G65" s="39">
+      <c r="G65" s="35">
         <v>10</v>
       </c>
       <c r="H65" s="22">
@@ -22760,9 +22782,11 @@
       <c r="C66" s="1"/>
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
-      <c r="F66" s="1"/>
-      <c r="G66" s="39">
-        <v>10</v>
+      <c r="F66" s="26" t="s">
+        <v>2105</v>
+      </c>
+      <c r="G66" s="35">
+        <v>230.11</v>
       </c>
       <c r="H66" s="22">
         <v>0</v>
@@ -22786,9 +22810,11 @@
       <c r="C67" s="1"/>
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
-      <c r="F67" s="1"/>
-      <c r="G67" s="39">
-        <v>10</v>
+      <c r="F67" s="26" t="s">
+        <v>2105</v>
+      </c>
+      <c r="G67" s="35">
+        <v>230.11</v>
       </c>
       <c r="H67" s="22">
         <v>0</v>
@@ -22812,9 +22838,11 @@
       <c r="C68" s="1"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
-      <c r="F68" s="1"/>
-      <c r="G68" s="39">
-        <v>10</v>
+      <c r="F68" s="26" t="s">
+        <v>2106</v>
+      </c>
+      <c r="G68" s="35">
+        <v>288.14999999999998</v>
       </c>
       <c r="H68" s="22">
         <v>0</v>
@@ -22839,7 +22867,7 @@
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
-      <c r="G69" s="39">
+      <c r="G69" s="35">
         <v>10</v>
       </c>
       <c r="H69" s="22">
@@ -22865,7 +22893,7 @@
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
-      <c r="G70" s="39">
+      <c r="G70" s="35">
         <v>10</v>
       </c>
       <c r="H70" s="22">
@@ -22895,7 +22923,7 @@
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
-      <c r="G71" s="39">
+      <c r="G71" s="35">
         <v>10</v>
       </c>
       <c r="H71" s="22">
@@ -22907,7 +22935,9 @@
       <c r="J71" s="1"/>
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
-      <c r="M71" s="1"/>
+      <c r="M71" s="1" t="s">
+        <v>2107</v>
+      </c>
       <c r="N71" s="1"/>
     </row>
     <row r="72" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -22920,9 +22950,11 @@
       <c r="C72" s="1"/>
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
-      <c r="F72" s="1"/>
-      <c r="G72" s="39">
-        <v>10</v>
+      <c r="F72" s="31" t="s">
+        <v>2108</v>
+      </c>
+      <c r="G72" s="35">
+        <v>170.06</v>
       </c>
       <c r="H72" s="22">
         <v>0</v>
@@ -22947,7 +22979,7 @@
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
-      <c r="G73" s="39">
+      <c r="G73" s="35">
         <v>10</v>
       </c>
       <c r="H73" s="22">
@@ -22973,7 +23005,7 @@
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="26"/>
-      <c r="G74" s="39">
+      <c r="G74" s="35">
         <v>10</v>
       </c>
       <c r="H74" s="22">
@@ -23003,7 +23035,7 @@
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
       <c r="F75" s="26"/>
-      <c r="G75" s="39">
+      <c r="G75" s="35">
         <v>10</v>
       </c>
       <c r="H75" s="22">
@@ -23029,7 +23061,7 @@
       <c r="D76" s="1"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
-      <c r="G76" s="39">
+      <c r="G76" s="35">
         <v>10</v>
       </c>
       <c r="H76" s="22">
@@ -23059,7 +23091,7 @@
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
-      <c r="G77" s="39">
+      <c r="G77" s="35">
         <v>10</v>
       </c>
       <c r="H77" s="22">
@@ -23085,7 +23117,7 @@
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
-      <c r="G78" s="39">
+      <c r="G78" s="35">
         <v>10</v>
       </c>
       <c r="H78" s="22">
@@ -23115,7 +23147,7 @@
       <c r="D79" s="1"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
-      <c r="G79" s="39">
+      <c r="G79" s="35">
         <v>10</v>
       </c>
       <c r="H79" s="22">
@@ -23141,7 +23173,7 @@
       <c r="D80" s="1"/>
       <c r="E80" s="1"/>
       <c r="F80" s="1"/>
-      <c r="G80" s="39">
+      <c r="G80" s="35">
         <v>10</v>
       </c>
       <c r="H80" s="22">
@@ -23167,7 +23199,7 @@
       <c r="D81" s="1"/>
       <c r="E81" s="1"/>
       <c r="F81" s="1"/>
-      <c r="G81" s="39">
+      <c r="G81" s="35">
         <v>10</v>
       </c>
       <c r="H81" s="22">
@@ -23197,7 +23229,7 @@
       <c r="D82" s="1"/>
       <c r="E82" s="1"/>
       <c r="F82" s="1"/>
-      <c r="G82" s="39">
+      <c r="G82" s="35">
         <v>10</v>
       </c>
       <c r="H82" s="22">
@@ -23223,7 +23255,7 @@
       <c r="D83" s="1"/>
       <c r="E83" s="1"/>
       <c r="F83" s="1"/>
-      <c r="G83" s="39">
+      <c r="G83" s="35">
         <v>10</v>
       </c>
       <c r="H83" s="22">
@@ -23253,7 +23285,7 @@
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
       <c r="F84" s="1"/>
-      <c r="G84" s="39">
+      <c r="G84" s="35">
         <v>10</v>
       </c>
       <c r="H84" s="22">
@@ -23279,7 +23311,7 @@
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="1"/>
-      <c r="G85" s="39">
+      <c r="G85" s="35">
         <v>10</v>
       </c>
       <c r="H85" s="22">
@@ -23309,7 +23341,7 @@
       <c r="D86" s="1"/>
       <c r="E86" s="1"/>
       <c r="F86" s="1"/>
-      <c r="G86" s="39">
+      <c r="G86" s="35">
         <v>10</v>
       </c>
       <c r="H86" s="22">
@@ -23335,7 +23367,7 @@
       <c r="D87" s="1"/>
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
-      <c r="G87" s="41">
+      <c r="G87" s="37">
         <v>40000</v>
       </c>
       <c r="H87" s="22">
@@ -23365,7 +23397,7 @@
       <c r="D88" s="1"/>
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
-      <c r="G88" s="41">
+      <c r="G88" s="37">
         <v>40000</v>
       </c>
       <c r="H88" s="22">
@@ -23395,7 +23427,7 @@
       <c r="D89" s="1"/>
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
-      <c r="G89" s="41">
+      <c r="G89" s="37">
         <v>40000</v>
       </c>
       <c r="H89" s="22">
@@ -23425,7 +23457,7 @@
       <c r="D90" s="1"/>
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
-      <c r="G90" s="41">
+      <c r="G90" s="37">
         <v>40000</v>
       </c>
       <c r="H90" s="22">
@@ -23455,7 +23487,7 @@
       <c r="D91" s="1"/>
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
-      <c r="G91" s="41">
+      <c r="G91" s="37">
         <v>40000</v>
       </c>
       <c r="H91" s="22">
@@ -23485,7 +23517,7 @@
       <c r="D92" s="1"/>
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
-      <c r="G92" s="41">
+      <c r="G92" s="37">
         <v>40000</v>
       </c>
       <c r="H92" s="22">
@@ -23515,7 +23547,7 @@
       <c r="D93" s="1"/>
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
-      <c r="G93" s="41">
+      <c r="G93" s="37">
         <v>40000</v>
       </c>
       <c r="H93" s="22">
@@ -23545,7 +23577,7 @@
       <c r="D94" s="1"/>
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
-      <c r="G94" s="41">
+      <c r="G94" s="37">
         <v>40000</v>
       </c>
       <c r="H94" s="22">
@@ -23575,7 +23607,7 @@
       <c r="D95" s="1"/>
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
-      <c r="G95" s="41">
+      <c r="G95" s="37">
         <v>40000</v>
       </c>
       <c r="H95" s="22">
@@ -23605,7 +23637,7 @@
       <c r="D96" s="1"/>
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
-      <c r="G96" s="41">
+      <c r="G96" s="37">
         <v>40000</v>
       </c>
       <c r="H96" s="22">
@@ -23635,7 +23667,7 @@
       <c r="D97" s="1"/>
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
-      <c r="G97" s="41">
+      <c r="G97" s="37">
         <v>40000</v>
       </c>
       <c r="H97" s="22">
@@ -23665,7 +23697,7 @@
       <c r="D98" s="1"/>
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
-      <c r="G98" s="41">
+      <c r="G98" s="37">
         <v>40000</v>
       </c>
       <c r="H98" s="22">
@@ -23695,7 +23727,7 @@
       <c r="D99" s="1"/>
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
-      <c r="G99" s="41">
+      <c r="G99" s="37">
         <v>40000</v>
       </c>
       <c r="H99" s="22">
@@ -23725,7 +23757,7 @@
       <c r="D100" s="1"/>
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
-      <c r="G100" s="41">
+      <c r="G100" s="37">
         <v>40000</v>
       </c>
       <c r="H100" s="22">
@@ -23755,7 +23787,7 @@
       <c r="D101" s="1"/>
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
-      <c r="G101" s="41">
+      <c r="G101" s="37">
         <v>40000</v>
       </c>
       <c r="H101" s="22">
@@ -23785,7 +23817,7 @@
       <c r="D102" s="1"/>
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
-      <c r="G102" s="41">
+      <c r="G102" s="37">
         <v>40000</v>
       </c>
       <c r="H102" s="22">
@@ -23815,7 +23847,7 @@
       <c r="D103" s="1"/>
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
-      <c r="G103" s="41">
+      <c r="G103" s="37">
         <v>40000</v>
       </c>
       <c r="H103" s="22">
@@ -23845,7 +23877,7 @@
       <c r="D104" s="1"/>
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
-      <c r="G104" s="41">
+      <c r="G104" s="37">
         <v>40000</v>
       </c>
       <c r="H104" s="22">
@@ -23875,7 +23907,7 @@
       <c r="D105" s="1"/>
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
-      <c r="G105" s="41">
+      <c r="G105" s="37">
         <v>40000</v>
       </c>
       <c r="H105" s="22">
@@ -23905,7 +23937,7 @@
       <c r="D106" s="1"/>
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
-      <c r="G106" s="41">
+      <c r="G106" s="37">
         <v>40000</v>
       </c>
       <c r="H106" s="22">
@@ -23935,7 +23967,7 @@
       <c r="D107" s="1"/>
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
-      <c r="G107" s="41">
+      <c r="G107" s="37">
         <v>40000</v>
       </c>
       <c r="H107" s="22">
@@ -23965,7 +23997,7 @@
       <c r="D108" s="1"/>
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
-      <c r="G108" s="41">
+      <c r="G108" s="37">
         <v>40000</v>
       </c>
       <c r="H108" s="22">
@@ -23995,7 +24027,7 @@
       <c r="D109" s="1"/>
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
-      <c r="G109" s="41">
+      <c r="G109" s="37">
         <v>40000</v>
       </c>
       <c r="H109" s="22">
@@ -24025,7 +24057,7 @@
       <c r="D110" s="1"/>
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
-      <c r="G110" s="41">
+      <c r="G110" s="37">
         <v>40000</v>
       </c>
       <c r="H110" s="22">
@@ -24055,7 +24087,7 @@
       <c r="D111" s="1"/>
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
-      <c r="G111" s="41">
+      <c r="G111" s="37">
         <v>40000</v>
       </c>
       <c r="H111" s="22">
@@ -24085,7 +24117,7 @@
       <c r="D112" s="1"/>
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
-      <c r="G112" s="41">
+      <c r="G112" s="37">
         <v>40000</v>
       </c>
       <c r="H112" s="22">
@@ -24115,7 +24147,7 @@
       <c r="D113" s="1"/>
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
-      <c r="G113" s="41">
+      <c r="G113" s="37">
         <v>40000</v>
       </c>
       <c r="H113" s="22">
@@ -24145,7 +24177,7 @@
       <c r="D114" s="1"/>
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
-      <c r="G114" s="41">
+      <c r="G114" s="37">
         <v>40000</v>
       </c>
       <c r="H114" s="22">
@@ -24175,7 +24207,7 @@
       <c r="D115" s="1"/>
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
-      <c r="G115" s="41">
+      <c r="G115" s="37">
         <v>40000</v>
       </c>
       <c r="H115" s="22">
@@ -24205,7 +24237,7 @@
       <c r="D116" s="1"/>
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
-      <c r="G116" s="41">
+      <c r="G116" s="37">
         <v>40000</v>
       </c>
       <c r="H116" s="22">
@@ -24235,7 +24267,7 @@
       <c r="D117" s="1"/>
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
-      <c r="G117" s="41">
+      <c r="G117" s="37">
         <v>400000</v>
       </c>
       <c r="H117" s="22">
@@ -24265,7 +24297,7 @@
       <c r="D118" s="1"/>
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
-      <c r="G118" s="41">
+      <c r="G118" s="37">
         <v>400000</v>
       </c>
       <c r="H118" s="22">
@@ -24295,7 +24327,7 @@
       <c r="D119" s="1"/>
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
-      <c r="G119" s="41">
+      <c r="G119" s="37">
         <v>400000</v>
       </c>
       <c r="H119" s="22">
@@ -24325,7 +24357,7 @@
       <c r="D120" s="1"/>
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
-      <c r="G120" s="41">
+      <c r="G120" s="37">
         <v>400000</v>
       </c>
       <c r="H120" s="22">
@@ -24355,7 +24387,7 @@
       <c r="D121" s="1"/>
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
-      <c r="G121" s="41">
+      <c r="G121" s="37">
         <v>400000</v>
       </c>
       <c r="H121" s="22">
@@ -24385,7 +24417,7 @@
       <c r="D122" s="1"/>
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
-      <c r="G122" s="41">
+      <c r="G122" s="37">
         <v>400000</v>
       </c>
       <c r="H122" s="22">
@@ -24415,7 +24447,7 @@
       <c r="D123" s="1"/>
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
-      <c r="G123" s="41">
+      <c r="G123" s="37">
         <v>400000</v>
       </c>
       <c r="H123" s="22">
@@ -24445,7 +24477,7 @@
       <c r="D124" s="1"/>
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
-      <c r="G124" s="41">
+      <c r="G124" s="37">
         <v>400000</v>
       </c>
       <c r="H124" s="22">
@@ -24475,7 +24507,7 @@
       <c r="D125" s="1"/>
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
-      <c r="G125" s="41">
+      <c r="G125" s="37">
         <v>400000</v>
       </c>
       <c r="H125" s="22">
@@ -24505,7 +24537,7 @@
       <c r="D126" s="1"/>
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
-      <c r="G126" s="41">
+      <c r="G126" s="37">
         <v>400000</v>
       </c>
       <c r="H126" s="22">
@@ -24535,7 +24567,7 @@
       <c r="D127" s="1"/>
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
-      <c r="G127" s="41">
+      <c r="G127" s="37">
         <v>400000</v>
       </c>
       <c r="H127" s="22">
@@ -24565,7 +24597,7 @@
       <c r="D128" s="1"/>
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
-      <c r="G128" s="41">
+      <c r="G128" s="37">
         <v>400000</v>
       </c>
       <c r="H128" s="22">
@@ -24595,7 +24627,7 @@
       <c r="D129" s="1"/>
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
-      <c r="G129" s="41">
+      <c r="G129" s="37">
         <v>400000</v>
       </c>
       <c r="H129" s="22">
@@ -24625,7 +24657,7 @@
       <c r="D130" s="1"/>
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
-      <c r="G130" s="41">
+      <c r="G130" s="37">
         <v>400000</v>
       </c>
       <c r="H130" s="22">
@@ -24655,7 +24687,7 @@
       <c r="D131" s="1"/>
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
-      <c r="G131" s="41">
+      <c r="G131" s="37">
         <v>400000</v>
       </c>
       <c r="H131" s="22">
@@ -24685,7 +24717,7 @@
       <c r="D132" s="1"/>
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
-      <c r="G132" s="41">
+      <c r="G132" s="37">
         <v>400000</v>
       </c>
       <c r="H132" s="22">
@@ -24715,7 +24747,7 @@
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
-      <c r="G133" s="41">
+      <c r="G133" s="37">
         <v>400000</v>
       </c>
       <c r="H133" s="22">
@@ -24745,7 +24777,7 @@
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
-      <c r="G134" s="41">
+      <c r="G134" s="37">
         <v>400000</v>
       </c>
       <c r="H134" s="22">
@@ -24775,7 +24807,7 @@
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
-      <c r="G135" s="41">
+      <c r="G135" s="37">
         <v>400000</v>
       </c>
       <c r="H135" s="22">
@@ -24805,7 +24837,7 @@
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
-      <c r="G136" s="41">
+      <c r="G136" s="37">
         <v>400000</v>
       </c>
       <c r="H136" s="22">
@@ -24835,7 +24867,7 @@
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
-      <c r="G137" s="41">
+      <c r="G137" s="37">
         <v>400000</v>
       </c>
       <c r="H137" s="22">
@@ -24865,7 +24897,7 @@
       <c r="D138" s="1"/>
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
-      <c r="G138" s="41">
+      <c r="G138" s="37">
         <v>400000</v>
       </c>
       <c r="H138" s="22">
@@ -24895,7 +24927,7 @@
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
-      <c r="G139" s="41">
+      <c r="G139" s="37">
         <v>400000</v>
       </c>
       <c r="H139" s="22">
@@ -24925,7 +24957,7 @@
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
-      <c r="G140" s="41">
+      <c r="G140" s="37">
         <v>400000</v>
       </c>
       <c r="H140" s="22">
@@ -24955,7 +24987,7 @@
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
-      <c r="G141" s="41">
+      <c r="G141" s="37">
         <v>400000</v>
       </c>
       <c r="H141" s="22">
@@ -24985,7 +25017,7 @@
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
-      <c r="G142" s="41">
+      <c r="G142" s="37">
         <v>400000</v>
       </c>
       <c r="H142" s="22">
@@ -25015,7 +25047,7 @@
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
-      <c r="G143" s="41">
+      <c r="G143" s="37">
         <v>400000</v>
       </c>
       <c r="H143" s="22">
@@ -25045,7 +25077,7 @@
       <c r="D144" s="1"/>
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
-      <c r="G144" s="41">
+      <c r="G144" s="37">
         <v>400000</v>
       </c>
       <c r="H144" s="22">
@@ -25075,7 +25107,7 @@
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
-      <c r="G145" s="41">
+      <c r="G145" s="37">
         <v>400000</v>
       </c>
       <c r="H145" s="22">
@@ -25105,7 +25137,7 @@
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
-      <c r="G146" s="41">
+      <c r="G146" s="37">
         <v>400000</v>
       </c>
       <c r="H146" s="22">
@@ -25141,8 +25173,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView topLeftCell="A69" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79"/>
+    <sheetView topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="C149" sqref="C149"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -27829,9 +27861,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L128"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A49" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K68" sqref="K68"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>

</xml_diff>

<commit_message>
add structure information for dipeptides missing it
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="-28820" yWindow="1580" windowWidth="27420" windowHeight="19400" tabRatio="500" activeTab="6"/>
-    <workbookView minimized="1" xWindow="640" yWindow="1180" windowWidth="35320" windowHeight="19700" tabRatio="500" firstSheet="5" activeTab="5"/>
+    <workbookView minimized="1" xWindow="640" yWindow="1180" windowWidth="35320" windowHeight="19700" tabRatio="500" firstSheet="5" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4860" uniqueCount="2109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4869" uniqueCount="2118">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -6694,9 +6694,6 @@
     <t>C3H6O3</t>
   </si>
   <si>
-    <t>C21H28N7O14P2</t>
-  </si>
-  <si>
     <t>C21H29N7O14P2</t>
   </si>
   <si>
@@ -6755,6 +6752,36 @@
   </si>
   <si>
     <t>C3H7O6P</t>
+  </si>
+  <si>
+    <t>C10H20N2O3</t>
+  </si>
+  <si>
+    <t>C18H20N2O5</t>
+  </si>
+  <si>
+    <t>C8H16N2O5</t>
+  </si>
+  <si>
+    <t>C6H12N2O5</t>
+  </si>
+  <si>
+    <t>C10H16N2O3</t>
+  </si>
+  <si>
+    <t>C18H20N2O3</t>
+  </si>
+  <si>
+    <t>C10H20N2O3S2</t>
+  </si>
+  <si>
+    <t>C12H26N4O3</t>
+  </si>
+  <si>
+    <t>C12H24N2O3</t>
+  </si>
+  <si>
+    <t>Not in PubChem</t>
   </si>
 </sst>
 </file>
@@ -20157,16 +20184,16 @@
     </row>
     <row r="24" spans="1:18" ht="43" x14ac:dyDescent="0.2">
       <c r="A24" s="25" t="s">
+        <v>2090</v>
+      </c>
+      <c r="B24" s="25" t="s">
         <v>2091</v>
       </c>
-      <c r="B24" s="25" t="s">
+      <c r="C24" s="25" t="s">
         <v>2092</v>
       </c>
-      <c r="C24" s="25" t="s">
-        <v>2093</v>
-      </c>
       <c r="D24" s="25" t="s">
-        <v>2096</v>
+        <v>2095</v>
       </c>
       <c r="E24" s="25"/>
       <c r="F24" s="25">
@@ -20176,10 +20203,10 @@
         <v>1827</v>
       </c>
       <c r="H24" s="25" t="s">
+        <v>2093</v>
+      </c>
+      <c r="I24" s="25" t="s">
         <v>2094</v>
-      </c>
-      <c r="I24" s="25" t="s">
-        <v>2095</v>
       </c>
       <c r="J24" s="25"/>
       <c r="K24" s="25">
@@ -20189,21 +20216,21 @@
         <v>22</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>2097</v>
+        <v>2096</v>
       </c>
     </row>
     <row r="25" spans="1:18" ht="43" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
+        <v>2097</v>
+      </c>
+      <c r="B25" s="25" t="s">
         <v>2098</v>
       </c>
-      <c r="B25" s="25" t="s">
+      <c r="C25" s="25" t="s">
         <v>2099</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="D25" s="25" t="s">
         <v>2100</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>2101</v>
       </c>
       <c r="E25" s="25"/>
       <c r="F25" s="25">
@@ -20217,7 +20244,7 @@
         <v>1866</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>2103</v>
+        <v>2102</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
@@ -20659,7 +20686,7 @@
   <dimension ref="A1:U5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView workbookViewId="1">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -20891,8 +20918,9 @@
   <dimension ref="A1:N146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1600" topLeftCell="A36" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="F72" sqref="F72"/>
+      <pane ySplit="1600" topLeftCell="A3" activePane="bottomLeft"/>
+      <selection activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -21962,7 +21990,9 @@
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
-      <c r="L37" s="1"/>
+      <c r="L37" s="1" t="s">
+        <v>2117</v>
+      </c>
       <c r="M37" s="1" t="s">
         <v>113</v>
       </c>
@@ -22302,9 +22332,11 @@
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
-      <c r="F49" s="26"/>
+      <c r="F49" s="31" t="s">
+        <v>2116</v>
+      </c>
       <c r="G49" s="35">
-        <v>10</v>
+        <v>244.33</v>
       </c>
       <c r="H49" s="22">
         <v>0</v>
@@ -22332,7 +22364,7 @@
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="26"/>
+      <c r="F50" s="31"/>
       <c r="G50" s="35">
         <v>10</v>
       </c>
@@ -22358,9 +22390,11 @@
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
-      <c r="F51" s="1"/>
+      <c r="F51" s="31" t="s">
+        <v>2115</v>
+      </c>
       <c r="G51" s="35">
-        <v>10</v>
+        <v>274.36</v>
       </c>
       <c r="H51" s="22">
         <v>0</v>
@@ -22388,7 +22422,7 @@
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="26"/>
+      <c r="F52" s="31"/>
       <c r="G52" s="35">
         <v>10</v>
       </c>
@@ -22414,9 +22448,11 @@
       <c r="C53" s="1"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
-      <c r="F53" s="26"/>
+      <c r="F53" s="31" t="s">
+        <v>2114</v>
+      </c>
       <c r="G53" s="35">
-        <v>10</v>
+        <v>280.39999999999998</v>
       </c>
       <c r="H53" s="22">
         <v>0</v>
@@ -22444,9 +22480,7 @@
       <c r="C54" s="1"/>
       <c r="D54" s="1"/>
       <c r="E54" s="1"/>
-      <c r="F54" s="26" t="s">
-        <v>2088</v>
-      </c>
+      <c r="F54" s="31"/>
       <c r="G54" s="35">
         <v>664.4</v>
       </c>
@@ -22477,7 +22511,7 @@
       <c r="D55" s="1"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1" t="s">
-        <v>2089</v>
+        <v>2088</v>
       </c>
       <c r="G55" s="35">
         <v>665.4</v>
@@ -22588,9 +22622,11 @@
       <c r="C59" s="1"/>
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
-      <c r="F59" s="1"/>
+      <c r="F59" s="31" t="s">
+        <v>2113</v>
+      </c>
       <c r="G59" s="35">
-        <v>10</v>
+        <v>312.39999999999998</v>
       </c>
       <c r="H59" s="22">
         <v>0</v>
@@ -22618,7 +22654,7 @@
       <c r="C60" s="1"/>
       <c r="D60" s="1"/>
       <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
+      <c r="F60" s="31"/>
       <c r="G60" s="35">
         <v>10</v>
       </c>
@@ -22698,9 +22734,11 @@
       <c r="C63" s="1"/>
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
-      <c r="F63" s="26"/>
+      <c r="F63" s="31" t="s">
+        <v>2112</v>
+      </c>
       <c r="G63" s="35">
-        <v>10</v>
+        <v>212.25</v>
       </c>
       <c r="H63" s="22">
         <v>0</v>
@@ -22729,7 +22767,7 @@
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="26" t="s">
-        <v>2104</v>
+        <v>2103</v>
       </c>
       <c r="G64" s="35">
         <v>390.07</v>
@@ -22783,7 +22821,7 @@
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="26" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="G66" s="35">
         <v>230.11</v>
@@ -22811,7 +22849,7 @@
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="26" t="s">
-        <v>2105</v>
+        <v>2104</v>
       </c>
       <c r="G67" s="35">
         <v>230.11</v>
@@ -22839,7 +22877,7 @@
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="26" t="s">
-        <v>2106</v>
+        <v>2105</v>
       </c>
       <c r="G68" s="35">
         <v>288.14999999999998</v>
@@ -22892,9 +22930,11 @@
       <c r="C70" s="1"/>
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
-      <c r="F70" s="1"/>
+      <c r="F70" s="31" t="s">
+        <v>2111</v>
+      </c>
       <c r="G70" s="35">
-        <v>10</v>
+        <v>192.17</v>
       </c>
       <c r="H70" s="22">
         <v>0</v>
@@ -22922,7 +22962,7 @@
       <c r="C71" s="1"/>
       <c r="D71" s="1"/>
       <c r="E71" s="1"/>
-      <c r="F71" s="1"/>
+      <c r="F71" s="31"/>
       <c r="G71" s="35">
         <v>10</v>
       </c>
@@ -22936,7 +22976,7 @@
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1" t="s">
-        <v>2107</v>
+        <v>2106</v>
       </c>
       <c r="N71" s="1"/>
     </row>
@@ -22951,7 +22991,7 @@
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="31" t="s">
-        <v>2108</v>
+        <v>2107</v>
       </c>
       <c r="G72" s="35">
         <v>170.06</v>
@@ -23004,9 +23044,11 @@
       <c r="C74" s="1"/>
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
-      <c r="F74" s="26"/>
+      <c r="F74" s="31" t="s">
+        <v>2110</v>
+      </c>
       <c r="G74" s="35">
-        <v>10</v>
+        <v>220.22</v>
       </c>
       <c r="H74" s="22">
         <v>0</v>
@@ -23116,9 +23158,11 @@
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
-      <c r="F78" s="1"/>
+      <c r="F78" s="31" t="s">
+        <v>2109</v>
+      </c>
       <c r="G78" s="35">
-        <v>10</v>
+        <v>344.4</v>
       </c>
       <c r="H78" s="22">
         <v>0</v>
@@ -23310,9 +23354,11 @@
       <c r="C85" s="1"/>
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
-      <c r="F85" s="1"/>
+      <c r="F85" s="31" t="s">
+        <v>2108</v>
+      </c>
       <c r="G85" s="35">
-        <v>10</v>
+        <v>216.28</v>
       </c>
       <c r="H85" s="22">
         <v>0</v>
@@ -23380,10 +23426,10 @@
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
       <c r="M87" s="1" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N87" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N87" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="88" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23410,10 +23456,10 @@
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
       <c r="M88" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N88" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N88" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="89" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23440,10 +23486,10 @@
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
       <c r="M89" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N89" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N89" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="90" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23470,10 +23516,10 @@
       <c r="K90" s="1"/>
       <c r="L90" s="1"/>
       <c r="M90" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N90" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N90" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="91" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23500,10 +23546,10 @@
       <c r="K91" s="1"/>
       <c r="L91" s="1"/>
       <c r="M91" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N91" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N91" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="92" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23530,10 +23576,10 @@
       <c r="K92" s="1"/>
       <c r="L92" s="1"/>
       <c r="M92" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N92" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N92" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="93" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23560,10 +23606,10 @@
       <c r="K93" s="1"/>
       <c r="L93" s="1"/>
       <c r="M93" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N93" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N93" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="94" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23590,10 +23636,10 @@
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
       <c r="M94" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N94" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N94" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="95" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23620,10 +23666,10 @@
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
       <c r="M95" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N95" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N95" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="96" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23650,10 +23696,10 @@
       <c r="K96" s="1"/>
       <c r="L96" s="1"/>
       <c r="M96" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N96" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N96" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="97" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23680,10 +23726,10 @@
       <c r="K97" s="1"/>
       <c r="L97" s="1"/>
       <c r="M97" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N97" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N97" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="98" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23710,10 +23756,10 @@
       <c r="K98" s="1"/>
       <c r="L98" s="1"/>
       <c r="M98" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N98" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N98" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="99" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23740,10 +23786,10 @@
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
       <c r="M99" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N99" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N99" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="100" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23770,10 +23816,10 @@
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
       <c r="M100" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N100" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N100" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="101" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23800,10 +23846,10 @@
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
       <c r="M101" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N101" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N101" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="102" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23830,10 +23876,10 @@
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>
       <c r="M102" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N102" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N102" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="103" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23860,10 +23906,10 @@
       <c r="K103" s="1"/>
       <c r="L103" s="1"/>
       <c r="M103" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N103" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N103" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="104" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23890,10 +23936,10 @@
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
       <c r="M104" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N104" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N104" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="105" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23920,10 +23966,10 @@
       <c r="K105" s="1"/>
       <c r="L105" s="1"/>
       <c r="M105" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N105" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N105" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="106" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23950,10 +23996,10 @@
       <c r="K106" s="1"/>
       <c r="L106" s="1"/>
       <c r="M106" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N106" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N106" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="107" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23980,10 +24026,10 @@
       <c r="K107" s="1"/>
       <c r="L107" s="1"/>
       <c r="M107" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N107" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N107" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="108" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24010,10 +24056,10 @@
       <c r="K108" s="1"/>
       <c r="L108" s="1"/>
       <c r="M108" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N108" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N108" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="109" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24040,10 +24086,10 @@
       <c r="K109" s="1"/>
       <c r="L109" s="1"/>
       <c r="M109" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N109" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N109" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="110" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24070,10 +24116,10 @@
       <c r="K110" s="1"/>
       <c r="L110" s="1"/>
       <c r="M110" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N110" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N110" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="111" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24100,10 +24146,10 @@
       <c r="K111" s="1"/>
       <c r="L111" s="1"/>
       <c r="M111" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N111" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N111" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="112" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24130,10 +24176,10 @@
       <c r="K112" s="1"/>
       <c r="L112" s="1"/>
       <c r="M112" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N112" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N112" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="113" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24160,10 +24206,10 @@
       <c r="K113" s="1"/>
       <c r="L113" s="1"/>
       <c r="M113" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N113" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N113" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="114" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24190,10 +24236,10 @@
       <c r="K114" s="1"/>
       <c r="L114" s="1"/>
       <c r="M114" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N114" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N114" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="115" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24220,10 +24266,10 @@
       <c r="K115" s="1"/>
       <c r="L115" s="1"/>
       <c r="M115" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N115" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N115" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="116" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24250,10 +24296,10 @@
       <c r="K116" s="1"/>
       <c r="L116" s="1"/>
       <c r="M116" s="26" t="s">
+        <v>2089</v>
+      </c>
+      <c r="N116" s="25" t="s">
         <v>2090</v>
-      </c>
-      <c r="N116" s="25" t="s">
-        <v>2091</v>
       </c>
     </row>
     <row r="117" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24280,10 +24326,10 @@
       <c r="K117" s="1"/>
       <c r="L117" s="1"/>
       <c r="M117" s="1" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N117" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="118" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24310,10 +24356,10 @@
       <c r="K118" s="1"/>
       <c r="L118" s="1"/>
       <c r="M118" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N118" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="119" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24340,10 +24386,10 @@
       <c r="K119" s="1"/>
       <c r="L119" s="1"/>
       <c r="M119" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N119" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="120" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24370,10 +24416,10 @@
       <c r="K120" s="1"/>
       <c r="L120" s="1"/>
       <c r="M120" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N120" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="121" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24400,10 +24446,10 @@
       <c r="K121" s="1"/>
       <c r="L121" s="1"/>
       <c r="M121" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N121" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="122" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24430,10 +24476,10 @@
       <c r="K122" s="1"/>
       <c r="L122" s="1"/>
       <c r="M122" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N122" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="123" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24460,10 +24506,10 @@
       <c r="K123" s="1"/>
       <c r="L123" s="1"/>
       <c r="M123" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N123" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="124" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24490,10 +24536,10 @@
       <c r="K124" s="1"/>
       <c r="L124" s="1"/>
       <c r="M124" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N124" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="125" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24520,10 +24566,10 @@
       <c r="K125" s="1"/>
       <c r="L125" s="1"/>
       <c r="M125" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N125" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="126" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24550,10 +24596,10 @@
       <c r="K126" s="1"/>
       <c r="L126" s="1"/>
       <c r="M126" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N126" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="127" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24580,10 +24626,10 @@
       <c r="K127" s="1"/>
       <c r="L127" s="1"/>
       <c r="M127" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N127" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="128" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24610,10 +24656,10 @@
       <c r="K128" s="1"/>
       <c r="L128" s="1"/>
       <c r="M128" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N128" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="129" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24640,10 +24686,10 @@
       <c r="K129" s="1"/>
       <c r="L129" s="1"/>
       <c r="M129" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N129" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="130" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24670,10 +24716,10 @@
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
       <c r="M130" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N130" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="131" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24700,10 +24746,10 @@
       <c r="K131" s="1"/>
       <c r="L131" s="1"/>
       <c r="M131" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N131" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="132" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24730,10 +24776,10 @@
       <c r="K132" s="1"/>
       <c r="L132" s="1"/>
       <c r="M132" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N132" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="133" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24760,10 +24806,10 @@
       <c r="K133" s="1"/>
       <c r="L133" s="1"/>
       <c r="M133" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N133" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="134" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24790,10 +24836,10 @@
       <c r="K134" s="1"/>
       <c r="L134" s="1"/>
       <c r="M134" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N134" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="135" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24820,10 +24866,10 @@
       <c r="K135" s="1"/>
       <c r="L135" s="1"/>
       <c r="M135" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N135" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="136" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24850,10 +24896,10 @@
       <c r="K136" s="1"/>
       <c r="L136" s="1"/>
       <c r="M136" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N136" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="137" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24880,10 +24926,10 @@
       <c r="K137" s="1"/>
       <c r="L137" s="1"/>
       <c r="M137" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N137" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="138" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24910,10 +24956,10 @@
       <c r="K138" s="1"/>
       <c r="L138" s="1"/>
       <c r="M138" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N138" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="139" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24940,10 +24986,10 @@
       <c r="K139" s="1"/>
       <c r="L139" s="1"/>
       <c r="M139" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N139" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="140" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -24970,10 +25016,10 @@
       <c r="K140" s="1"/>
       <c r="L140" s="1"/>
       <c r="M140" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N140" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="141" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -25000,10 +25046,10 @@
       <c r="K141" s="1"/>
       <c r="L141" s="1"/>
       <c r="M141" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N141" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="142" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -25030,10 +25076,10 @@
       <c r="K142" s="1"/>
       <c r="L142" s="1"/>
       <c r="M142" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N142" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="143" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -25060,10 +25106,10 @@
       <c r="K143" s="1"/>
       <c r="L143" s="1"/>
       <c r="M143" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N143" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="144" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -25090,10 +25136,10 @@
       <c r="K144" s="1"/>
       <c r="L144" s="1"/>
       <c r="M144" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N144" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="145" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -25120,10 +25166,10 @@
       <c r="K145" s="1"/>
       <c r="L145" s="1"/>
       <c r="M145" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N145" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="146" spans="1:14" ht="42" x14ac:dyDescent="0.2">
@@ -25150,10 +25196,10 @@
       <c r="K146" s="1"/>
       <c r="L146" s="1"/>
       <c r="M146" s="26" t="s">
-        <v>2102</v>
+        <v>2101</v>
       </c>
       <c r="N146" s="25" t="s">
-        <v>2098</v>
+        <v>2097</v>
       </c>
     </row>
   </sheetData>
@@ -25173,8 +25219,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView topLeftCell="A117" workbookViewId="0">
-      <selection activeCell="C149" sqref="C149"/>
+    <sheetView topLeftCell="A148" workbookViewId="0">
+      <selection activeCell="A175" sqref="A175"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -27863,9 +27909,11 @@
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="A18" sqref="A15:N18"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
Change name of D-glyceraldehdye-3-phosphate to D-glyceraldehyde-3-phosphate, based on Google match, and presence of latter but not former in PubChem
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4869" uniqueCount="2118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4870" uniqueCount="2119">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -6781,7 +6781,10 @@
     <t>C12H24N2O3</t>
   </si>
   <si>
-    <t>Not in PubChem</t>
+    <t>KTVPXOYAKDPRHY-AIHAYLRMSA-N</t>
+  </si>
+  <si>
+    <t>InChi</t>
   </si>
 </sst>
 </file>
@@ -20918,9 +20921,9 @@
   <dimension ref="A1:N146"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1600" topLeftCell="A3" activePane="bottomLeft"/>
+      <pane ySplit="1600" topLeftCell="A45" activePane="bottomLeft"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
+      <selection pane="bottomLeft" activeCell="D67" sqref="D67"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -20928,9 +20931,9 @@
   <cols>
     <col min="1" max="1" width="19.83203125" style="3" customWidth="1"/>
     <col min="2" max="2" width="44.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="22.6640625" style="3" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="7.83203125" style="3" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5" style="3" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="7.83203125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="3" customWidth="1"/>
     <col min="6" max="6" width="17.1640625" style="3" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="16.5" style="32" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="3" bestFit="1" customWidth="1"/>
@@ -21990,9 +21993,7 @@
       </c>
       <c r="J37" s="1"/>
       <c r="K37" s="1"/>
-      <c r="L37" s="1" t="s">
-        <v>2117</v>
-      </c>
+      <c r="L37" s="1"/>
       <c r="M37" s="1" t="s">
         <v>113</v>
       </c>
@@ -22817,8 +22818,12 @@
       <c r="B66" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
+      <c r="C66" s="31" t="s">
+        <v>2117</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>2118</v>
+      </c>
       <c r="E66" s="1"/>
       <c r="F66" s="26" t="s">
         <v>2104</v>

</xml_diff>

<commit_message>
add !Name !Format !Empirical formula & !Molecular weight for UDP, Uridine-5'-diphosphate
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4871" uniqueCount="2118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4874" uniqueCount="2121">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -6782,6 +6782,15 @@
   </si>
   <si>
     <t>C(C(C=O)O)OP(=O)(O)O</t>
+  </si>
+  <si>
+    <t>Uridine-5'-diphosphate</t>
+  </si>
+  <si>
+    <t>C9H14N2O12P2</t>
+  </si>
+  <si>
+    <t>C1=CN(C(=O)NC1=O)C2C(C(C(O2)COP(=O)(O)OP(=O)(O)O)O)O</t>
   </si>
 </sst>
 </file>
@@ -20919,8 +20928,8 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="1600" topLeftCell="A45" activePane="bottomLeft"/>
-      <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="D72" sqref="D72"/>
+      <selection activeCell="F1" sqref="F1"/>
+      <selection pane="bottomLeft" activeCell="A79" sqref="A79:B79"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -23188,15 +23197,21 @@
       <c r="A79" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="B79" s="1" t="s">
-        <v>379</v>
-      </c>
-      <c r="C79" s="1"/>
-      <c r="D79" s="1"/>
+      <c r="B79" s="31" t="s">
+        <v>2118</v>
+      </c>
+      <c r="C79" s="31" t="s">
+        <v>2120</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>1971</v>
+      </c>
       <c r="E79" s="1"/>
-      <c r="F79" s="1"/>
+      <c r="F79" s="1" t="s">
+        <v>2119</v>
+      </c>
       <c r="G79" s="35">
-        <v>10</v>
+        <v>404.16</v>
       </c>
       <c r="H79" s="22">
         <v>0</v>
@@ -23214,13 +23229,10 @@
       <c r="A80" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="B80" s="1" t="s">
+      <c r="B80" s="31" t="s">
         <v>380</v>
       </c>
       <c r="C80" s="1"/>
-      <c r="D80" s="1"/>
-      <c r="E80" s="1"/>
-      <c r="F80" s="1"/>
       <c r="G80" s="35">
         <v>10</v>
       </c>

</xml_diff>

<commit_message>
add !Format !Empirical formula & !Molecular weight for uridine
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4874" uniqueCount="2121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4877" uniqueCount="2123">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -6791,6 +6791,12 @@
   </si>
   <si>
     <t>C1=CN(C(=O)NC1=O)C2C(C(C(O2)COP(=O)(O)OP(=O)(O)O)O)O</t>
+  </si>
+  <si>
+    <t>C9H12N2O6</t>
+  </si>
+  <si>
+    <t>C1=CN(C(=O)NC1=O)C2C(C(C(O2)CO)O)O</t>
   </si>
 </sst>
 </file>
@@ -7731,7 +7737,7 @@
   <dimension ref="A1:I6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -8014,9 +8020,9 @@
   <dimension ref="A1:N178"/>
   <sheetViews>
     <sheetView topLeftCell="B3" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="D108" sqref="D108"/>
+      <selection pane="bottomLeft" activeCell="D92" sqref="D92"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -20929,7 +20935,7 @@
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="1600" topLeftCell="A45" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A79" sqref="A79:B79"/>
+      <selection pane="bottomLeft" activeCell="C82" sqref="C82"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -23285,12 +23291,18 @@
       <c r="B82" s="1" t="s">
         <v>389</v>
       </c>
-      <c r="C82" s="1"/>
-      <c r="D82" s="1"/>
+      <c r="C82" s="1" t="s">
+        <v>2122</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>1971</v>
+      </c>
       <c r="E82" s="1"/>
-      <c r="F82" s="1"/>
+      <c r="F82" s="1" t="s">
+        <v>2121</v>
+      </c>
       <c r="G82" s="35">
-        <v>10</v>
+        <v>244.2</v>
       </c>
       <c r="H82" s="22">
         <v>0</v>
@@ -25236,7 +25248,7 @@
   <dimension ref="A1:J177"/>
   <sheetViews>
     <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="A175" sqref="A175"/>
+      <selection activeCell="C166" sqref="C166"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -27924,8 +27936,8 @@
   <dimension ref="A1:L128"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A18" sqref="A15:N18"/>
+      <pane ySplit="2" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C120" sqref="C120"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
       <selection activeCell="C3" sqref="C3"/>

</xml_diff>

<commit_message>
add chemical formulae and MWs for LEU, LYS, MET, PHE, PRO, SER, THR, TRP, TYR, & VAL; add MWs for mRNAs and proteins, based on their ribonucleoside and amino acid content in the RNA degradation and transcription reactions, respectively
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-35600" yWindow="980" windowWidth="35460" windowHeight="19900" tabRatio="500" firstSheet="6" activeTab="8"/>
-    <workbookView xWindow="920" yWindow="1320" windowWidth="35320" windowHeight="18900" tabRatio="500" firstSheet="8" activeTab="21"/>
+    <workbookView minimized="1" xWindow="-35600" yWindow="980" windowWidth="35460" windowHeight="19900" tabRatio="500" firstSheet="6" activeTab="6"/>
+    <workbookView xWindow="920" yWindow="1300" windowWidth="35320" windowHeight="18900" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4931" uniqueCount="2165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5015" uniqueCount="2203">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -6694,48 +6694,6 @@
     <t>C21H29N7O14P2</t>
   </si>
   <si>
-    <t>Approx. MW of M. pneumoniae proteins</t>
-  </si>
-  <si>
-    <t>Ref_0022</t>
-  </si>
-  <si>
-    <t>himmelreich1996complete</t>
-  </si>
-  <si>
-    <t>Complete sequence analysis of the genome of the bacterium Mycoplasma pneumoniae</t>
-  </si>
-  <si>
-    <t>Nucleic acids research</t>
-  </si>
-  <si>
-    <t>Oxford University Press</t>
-  </si>
-  <si>
-    <t>Himmelreich, et al.</t>
-  </si>
-  <si>
-    <t>URL: https://academic.oup.com/nar/article-pdf/24/22/4420/7069676/24-22-4420.pdf</t>
-  </si>
-  <si>
-    <t>Ref_0023</t>
-  </si>
-  <si>
-    <t>milo2015cell</t>
-  </si>
-  <si>
-    <t>Cell biology by the numbers</t>
-  </si>
-  <si>
-    <t>Milo, Ron and Phillips, Rob</t>
-  </si>
-  <si>
-    <t>Approx. MW, 10x proteins</t>
-  </si>
-  <si>
-    <t>WHICH IS BIGGER, MRNA OR THE PROTEIN IT CODES FOR?</t>
-  </si>
-  <si>
     <t>C5H13O14P3</t>
   </si>
   <si>
@@ -6923,6 +6881,162 @@
   </si>
   <si>
     <t>DOI: 10.1073/pnas.0703774104</t>
+  </si>
+  <si>
+    <t>dist-init-conc-AD[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-ADP[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-CDP[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-CYTD[c]</t>
+  </si>
+  <si>
+    <t>From Escherichia coli K12 NCM3722</t>
+  </si>
+  <si>
+    <t>dist-init-conc-DPG[c]</t>
+  </si>
+  <si>
+    <t>From Homo sapiens</t>
+  </si>
+  <si>
+    <t>dist-init-conc-E4P[c]</t>
+  </si>
+  <si>
+    <t>From Escherichia coli W3110</t>
+  </si>
+  <si>
+    <t>dist-init-conc-F6P[c]</t>
+  </si>
+  <si>
+    <t>From Escherichia coli</t>
+  </si>
+  <si>
+    <t>dist-init-conc-FDP[c]</t>
+  </si>
+  <si>
+    <t>From Escherichia coli BW25113</t>
+  </si>
+  <si>
+    <t>dist-init-conc-G2P[c]</t>
+  </si>
+  <si>
+    <t>From Saccharomyces cerevisiae</t>
+  </si>
+  <si>
+    <t>dist-init-conc-G3P[c]</t>
+  </si>
+  <si>
+    <t>From Escherichia coli K12 NCM3722; median of 3 measurements</t>
+  </si>
+  <si>
+    <t>dist-init-conc-G6P[c]</t>
+  </si>
+  <si>
+    <t>Distant match: Glucosamine 6-phosphate from Escherichia coli</t>
+  </si>
+  <si>
+    <t>dist-init-conc-GN[c]</t>
+  </si>
+  <si>
+    <t>Median of 5 measurements in E. coli</t>
+  </si>
+  <si>
+    <t>dist-init-conc-LAC[c]</t>
+  </si>
+  <si>
+    <t>From https://pubchem.ncbi.nlm.nih.gov/compound/61503#section=BioAssay-Results</t>
+  </si>
+  <si>
+    <t>dist-init-conc-NAD[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-NADH[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-O2[c]</t>
+  </si>
+  <si>
+    <t>From https://pubchem.ncbi.nlm.nih.gov/bioassay/506735#sid=104251036</t>
+  </si>
+  <si>
+    <t>dist-init-conc-PEP[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-PRPP[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-R5P[c]</t>
+  </si>
+  <si>
+    <t>From Escherichia coli; for InChI KTVPXOYAKDPRHY-AIHAYLRMSA-N</t>
+  </si>
+  <si>
+    <t>dist-init-conc-RL5P[c]</t>
+  </si>
+  <si>
+    <t>Actually "Glycerol 3-phosphate" 0.956 similarity from Escherichia coli</t>
+  </si>
+  <si>
+    <t>dist-init-conc-S7P[c]</t>
+  </si>
+  <si>
+    <t>Poor match of  species name with Datanator and PubChem; measurement from E. coli</t>
+  </si>
+  <si>
+    <t>dist-init-conc-T3P1[c]</t>
+  </si>
+  <si>
+    <t>From Escherichia coli; not exact match for SMILES of species-type</t>
+  </si>
+  <si>
+    <t>dist-init-conc-T3P2[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-UDP[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-URI[c]</t>
+  </si>
+  <si>
+    <t>C9H13N2O9P</t>
+  </si>
+  <si>
+    <t>C6H14N2O2</t>
+  </si>
+  <si>
+    <t>C5H11NO2S</t>
+  </si>
+  <si>
+    <t>C9H11NO2</t>
+  </si>
+  <si>
+    <t>C5H9NO2</t>
+  </si>
+  <si>
+    <t>C3H7NO3</t>
+  </si>
+  <si>
+    <t>C11H12N2O2</t>
+  </si>
+  <si>
+    <t>C9H11NO3</t>
+  </si>
+  <si>
+    <t>C5H11NO2</t>
+  </si>
+  <si>
+    <t>C4H9NO3</t>
+  </si>
+  <si>
+    <t>based on ribonucleoside content in the RNA degradation reaction</t>
+  </si>
+  <si>
+    <t>based on AA content the transcription reaction</t>
   </si>
 </sst>
 </file>
@@ -7041,7 +7155,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -7150,6 +7264,9 @@
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7165,7 +7282,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8148,12 +8265,14 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:N178"/>
   <sheetViews>
-    <sheetView topLeftCell="B3" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="D92" sqref="D92"/>
+      <selection pane="bottomLeft" activeCell="D146" sqref="D146"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="A87" workbookViewId="1">
+      <selection activeCell="C99" sqref="C99"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -8173,11 +8292,11 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="40" t="s">
+      <c r="G2" s="41" t="s">
         <v>720</v>
       </c>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -16989,7 +17108,9 @@
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView workbookViewId="1">
+      <selection activeCell="J7" sqref="J7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -18821,26 +18942,26 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="42" t="s">
         <v>1746</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="41" t="s">
+      <c r="H2" s="43"/>
+      <c r="I2" s="42" t="s">
         <v>1747</v>
       </c>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="42"/>
-      <c r="M2" s="42"/>
-      <c r="N2" s="42"/>
-      <c r="Q2" s="41" t="s">
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="L2" s="43"/>
+      <c r="M2" s="43"/>
+      <c r="N2" s="43"/>
+      <c r="Q2" s="42" t="s">
         <v>1748</v>
       </c>
-      <c r="R2" s="42"/>
-      <c r="S2" s="41" t="s">
+      <c r="R2" s="43"/>
+      <c r="S2" s="42" t="s">
         <v>1749</v>
       </c>
-      <c r="T2" s="42"/>
+      <c r="T2" s="43"/>
     </row>
     <row r="3" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -19339,10 +19460,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="42" t="s">
         <v>1796</v>
       </c>
-      <c r="H2" s="42"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -19473,16 +19594,16 @@
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R36"/>
+  <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1580" topLeftCell="A19" activePane="bottomLeft"/>
       <selection activeCell="Q2" sqref="Q2"/>
-      <selection pane="bottomLeft" activeCell="D30" sqref="D30"/>
+      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
+    <sheetView workbookViewId="1">
       <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A32" sqref="A32"/>
+      <selection pane="bottomLeft" activeCell="A24" sqref="A24:XFD25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -20328,279 +20449,214 @@
         <v>1952</v>
       </c>
     </row>
-    <row r="24" spans="1:18" ht="43" x14ac:dyDescent="0.2">
-      <c r="A24" s="25" t="s">
-        <v>2089</v>
-      </c>
-      <c r="B24" s="25" t="s">
-        <v>2090</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>2091</v>
-      </c>
-      <c r="D24" s="25" t="s">
-        <v>2094</v>
-      </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25">
-        <v>1996</v>
-      </c>
-      <c r="G24" s="25" t="s">
+    <row r="24" spans="1:18" ht="57" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>2109</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>2110</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>2111</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>2112</v>
+      </c>
+      <c r="F24" s="3">
+        <v>2016</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>1826</v>
       </c>
-      <c r="H24" s="25" t="s">
-        <v>2092</v>
-      </c>
-      <c r="I24" s="25" t="s">
-        <v>2093</v>
-      </c>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25">
-        <v>24</v>
-      </c>
-      <c r="L24" s="25">
-        <v>22</v>
+      <c r="H24" s="3" t="s">
+        <v>2113</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>2114</v>
       </c>
       <c r="Q24" s="3" t="s">
-        <v>2095</v>
-      </c>
-    </row>
-    <row r="25" spans="1:18" ht="43" x14ac:dyDescent="0.2">
-      <c r="A25" s="25" t="s">
-        <v>2096</v>
-      </c>
-      <c r="B25" s="25" t="s">
-        <v>2097</v>
-      </c>
-      <c r="C25" s="25" t="s">
-        <v>2098</v>
-      </c>
-      <c r="D25" s="25" t="s">
-        <v>2099</v>
-      </c>
-      <c r="E25" s="25"/>
-      <c r="F25" s="25">
-        <v>2015</v>
-      </c>
-      <c r="G25" s="25" t="s">
-        <v>1864</v>
-      </c>
-      <c r="H25" s="25"/>
-      <c r="I25" s="25" t="s">
-        <v>1865</v>
-      </c>
-      <c r="O25" s="3" t="s">
-        <v>2101</v>
+        <v>2115</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>2116</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>2117</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>2118</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>2119</v>
+      </c>
+      <c r="F25" s="3">
+        <v>2020</v>
+      </c>
+      <c r="G25" s="3" t="s">
+        <v>1930</v>
+      </c>
+      <c r="Q25" s="3" t="s">
+        <v>2120</v>
       </c>
     </row>
     <row r="26" spans="1:18" ht="57" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
+        <v>2121</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>2122</v>
+      </c>
+      <c r="C26" s="25" t="s">
         <v>2123</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>2124</v>
       </c>
-      <c r="C26" s="3" t="s">
-        <v>2125</v>
-      </c>
-      <c r="D26" s="3" t="s">
-        <v>2126</v>
-      </c>
       <c r="F26" s="3">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="G26" s="3" t="s">
         <v>1826</v>
       </c>
       <c r="H26" s="3" t="s">
+        <v>2125</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>2126</v>
+      </c>
+      <c r="Q26" s="3" t="s">
         <v>2127</v>
       </c>
-      <c r="I26" s="3" t="s">
+    </row>
+    <row r="27" spans="1:18" ht="113" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>2128</v>
       </c>
-      <c r="Q26" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>2129</v>
       </c>
-    </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A27" s="3" t="s">
+      <c r="C27" s="25" t="s">
         <v>2130</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="D27" s="3" t="s">
         <v>2131</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="F27" s="3">
+        <v>2007</v>
+      </c>
+      <c r="G27" s="3" t="s">
+        <v>1826</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>1923</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>2132</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="Q27" s="3" t="s">
         <v>2133</v>
       </c>
-      <c r="F27" s="3">
-        <v>2020</v>
-      </c>
-      <c r="G27" s="3" t="s">
-        <v>1930</v>
-      </c>
-      <c r="Q27" s="3" t="s">
+    </row>
+    <row r="28" spans="1:18" ht="113" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>2134</v>
       </c>
-    </row>
-    <row r="28" spans="1:18" ht="57" x14ac:dyDescent="0.2">
-      <c r="A28" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>2135</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="C28" s="25" t="s">
         <v>2136</v>
       </c>
-      <c r="C28" s="25" t="s">
+      <c r="D28" s="3" t="s">
         <v>2137</v>
       </c>
-      <c r="D28" s="3" t="s">
-        <v>2138</v>
-      </c>
       <c r="F28" s="3">
-        <v>2011</v>
+        <v>2009</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>1826</v>
       </c>
       <c r="H28" s="3" t="s">
+        <v>2113</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>2114</v>
+      </c>
+      <c r="L28" s="3" t="s">
+        <v>2138</v>
+      </c>
+      <c r="Q28" s="3" t="s">
+        <v>2138</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" ht="43" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
         <v>2139</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="B29" s="3" t="s">
         <v>2140</v>
       </c>
-      <c r="Q28" s="3" t="s">
+      <c r="C29" s="25" t="s">
         <v>2141</v>
       </c>
-    </row>
-    <row r="29" spans="1:18" ht="113" x14ac:dyDescent="0.2">
-      <c r="A29" s="3" t="s">
+      <c r="D29" s="3" t="s">
+        <v>1514</v>
+      </c>
+      <c r="F29" s="3">
+        <v>2018</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>1930</v>
+      </c>
+      <c r="H29" s="3" t="s">
         <v>2142</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="Q29" s="3" t="s">
         <v>2143</v>
       </c>
-      <c r="C29" s="25" t="s">
+    </row>
+    <row r="30" spans="1:18" ht="57" x14ac:dyDescent="0.2">
+      <c r="A30" s="3" t="s">
         <v>2144</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="B30" s="3" t="s">
         <v>2145</v>
       </c>
-      <c r="F29" s="3">
+      <c r="C30" s="25" t="s">
+        <v>2146</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>2147</v>
+      </c>
+      <c r="F30" s="3">
         <v>2007</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>1826</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>1923</v>
-      </c>
-      <c r="I29" s="3" t="s">
-        <v>2146</v>
-      </c>
-      <c r="Q29" s="3" t="s">
-        <v>2147</v>
-      </c>
-    </row>
-    <row r="30" spans="1:18" ht="113" x14ac:dyDescent="0.2">
-      <c r="A30" s="3" t="s">
-        <v>2148</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>2149</v>
-      </c>
-      <c r="C30" s="25" t="s">
-        <v>2150</v>
-      </c>
-      <c r="D30" s="3" t="s">
-        <v>2151</v>
-      </c>
-      <c r="F30" s="3">
-        <v>2009</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>1826</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>2127</v>
+        <v>2148</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>2128</v>
-      </c>
-      <c r="L30" s="3" t="s">
-        <v>2152</v>
+        <v>2149</v>
       </c>
       <c r="Q30" s="3" t="s">
-        <v>2152</v>
-      </c>
-    </row>
-    <row r="31" spans="1:18" ht="43" x14ac:dyDescent="0.2">
-      <c r="A31" s="3" t="s">
-        <v>2153</v>
-      </c>
-      <c r="B31" s="3" t="s">
-        <v>2154</v>
-      </c>
-      <c r="C31" s="25" t="s">
-        <v>2155</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>1514</v>
-      </c>
-      <c r="F31" s="3">
-        <v>2018</v>
-      </c>
-      <c r="G31" s="3" t="s">
-        <v>1930</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>2156</v>
-      </c>
-      <c r="Q31" s="3" t="s">
-        <v>2157</v>
-      </c>
-    </row>
-    <row r="32" spans="1:18" ht="57" x14ac:dyDescent="0.2">
-      <c r="A32" s="3" t="s">
-        <v>2158</v>
-      </c>
-      <c r="B32" s="3" t="s">
-        <v>2159</v>
-      </c>
-      <c r="C32" s="25" t="s">
-        <v>2160</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>2161</v>
-      </c>
-      <c r="F32" s="3">
-        <v>2007</v>
-      </c>
-      <c r="G32" s="3" t="s">
-        <v>1826</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>2162</v>
-      </c>
-      <c r="I32" s="3" t="s">
-        <v>2163</v>
-      </c>
-      <c r="Q32" s="3" t="s">
-        <v>2164</v>
-      </c>
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C31" s="25"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="C32" s="25"/>
     </row>
     <row r="33" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C33" s="25"/>
     </row>
     <row r="34" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C34" s="25"/>
-    </row>
-    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C35" s="25"/>
-    </row>
-    <row r="36" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C36" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:R23"/>
@@ -21036,18 +21092,18 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H2" s="38" t="s">
+      <c r="H2" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="M2" s="38" t="s">
+      <c r="I2" s="40"/>
+      <c r="J2" s="40"/>
+      <c r="K2" s="40"/>
+      <c r="M2" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
+      <c r="N2" s="40"/>
+      <c r="O2" s="40"/>
+      <c r="P2" s="40"/>
     </row>
     <row r="3" spans="1:21" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -21245,13 +21301,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N146"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1600" topLeftCell="A45" activePane="bottomLeft"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="1600" topLeftCell="A85" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="C58" sqref="C58"/>
+      <selection pane="bottomLeft" activeCell="M117" sqref="M117"/>
     </sheetView>
-    <sheetView topLeftCell="A52" workbookViewId="1">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="1">
+      <selection activeCell="G65" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21275,14 +21331,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="38" t="s">
+      <c r="C2" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -22634,9 +22690,11 @@
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
-      <c r="F48" s="26"/>
+      <c r="F48" s="26" t="s">
+        <v>2007</v>
+      </c>
       <c r="G48" s="35">
-        <v>10</v>
+        <v>131.16999999999999</v>
       </c>
       <c r="H48" s="22">
         <v>0</v>
@@ -22661,7 +22719,7 @@
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
       <c r="F49" s="31" t="s">
-        <v>2115</v>
+        <v>2101</v>
       </c>
       <c r="G49" s="35">
         <v>244.33</v>
@@ -22692,9 +22750,11 @@
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
-      <c r="F50" s="31"/>
+      <c r="F50" s="31" t="s">
+        <v>2192</v>
+      </c>
       <c r="G50" s="35">
-        <v>10</v>
+        <v>146.19</v>
       </c>
       <c r="H50" s="22">
         <v>0</v>
@@ -22719,7 +22779,7 @@
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
       <c r="F51" s="31" t="s">
-        <v>2114</v>
+        <v>2100</v>
       </c>
       <c r="G51" s="35">
         <v>274.36</v>
@@ -22750,9 +22810,11 @@
       <c r="C52" s="1"/>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
-      <c r="F52" s="31"/>
+      <c r="F52" s="31" t="s">
+        <v>2193</v>
+      </c>
       <c r="G52" s="35">
-        <v>10</v>
+        <v>149.21</v>
       </c>
       <c r="H52" s="22">
         <v>0</v>
@@ -22777,7 +22839,7 @@
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="31" t="s">
-        <v>2113</v>
+        <v>2099</v>
       </c>
       <c r="G53" s="35">
         <v>280.39999999999998</v>
@@ -22924,9 +22986,11 @@
       <c r="C58" s="1"/>
       <c r="D58" s="1"/>
       <c r="E58" s="1"/>
-      <c r="F58" s="26"/>
+      <c r="F58" s="26" t="s">
+        <v>2194</v>
+      </c>
       <c r="G58" s="35">
-        <v>10</v>
+        <v>165.19</v>
       </c>
       <c r="H58" s="22">
         <v>0</v>
@@ -22951,7 +23015,7 @@
       <c r="D59" s="1"/>
       <c r="E59" s="1"/>
       <c r="F59" s="31" t="s">
-        <v>2112</v>
+        <v>2098</v>
       </c>
       <c r="G59" s="35">
         <v>312.39999999999998</v>
@@ -23036,9 +23100,11 @@
       <c r="C62" s="1"/>
       <c r="D62" s="1"/>
       <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
+      <c r="F62" s="1" t="s">
+        <v>2195</v>
+      </c>
       <c r="G62" s="35">
-        <v>10</v>
+        <v>115.13</v>
       </c>
       <c r="H62" s="22">
         <v>0</v>
@@ -23063,7 +23129,7 @@
       <c r="D63" s="1"/>
       <c r="E63" s="1"/>
       <c r="F63" s="31" t="s">
-        <v>2111</v>
+        <v>2097</v>
       </c>
       <c r="G63" s="35">
         <v>212.25</v>
@@ -23095,7 +23161,7 @@
       <c r="D64" s="1"/>
       <c r="E64" s="1"/>
       <c r="F64" s="26" t="s">
-        <v>2102</v>
+        <v>2088</v>
       </c>
       <c r="G64" s="35">
         <v>390.07</v>
@@ -23149,7 +23215,7 @@
       <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="26" t="s">
-        <v>2103</v>
+        <v>2089</v>
       </c>
       <c r="G66" s="35">
         <v>230.11</v>
@@ -23177,7 +23243,7 @@
       <c r="D67" s="1"/>
       <c r="E67" s="1"/>
       <c r="F67" s="26" t="s">
-        <v>2103</v>
+        <v>2089</v>
       </c>
       <c r="G67" s="35">
         <v>230.11</v>
@@ -23205,7 +23271,7 @@
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="26" t="s">
-        <v>2104</v>
+        <v>2090</v>
       </c>
       <c r="G68" s="35">
         <v>288.14999999999998</v>
@@ -23232,9 +23298,11 @@
       <c r="C69" s="1"/>
       <c r="D69" s="1"/>
       <c r="E69" s="1"/>
-      <c r="F69" s="1"/>
+      <c r="F69" s="1" t="s">
+        <v>2196</v>
+      </c>
       <c r="G69" s="35">
-        <v>10</v>
+        <v>105.09</v>
       </c>
       <c r="H69" s="22">
         <v>0</v>
@@ -23259,7 +23327,7 @@
       <c r="D70" s="1"/>
       <c r="E70" s="1"/>
       <c r="F70" s="31" t="s">
-        <v>2110</v>
+        <v>2096</v>
       </c>
       <c r="G70" s="35">
         <v>192.17</v>
@@ -23285,17 +23353,17 @@
         <v>352</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>2116</v>
+        <v>2102</v>
       </c>
       <c r="C71" s="31" t="s">
-        <v>2117</v>
+        <v>2103</v>
       </c>
       <c r="D71" s="1" t="s">
         <v>1971</v>
       </c>
       <c r="E71" s="1"/>
       <c r="F71" s="31" t="s">
-        <v>2106</v>
+        <v>2092</v>
       </c>
       <c r="G71" s="35">
         <v>170.06</v>
@@ -23310,7 +23378,7 @@
       <c r="K71" s="1"/>
       <c r="L71" s="1"/>
       <c r="M71" s="1" t="s">
-        <v>2105</v>
+        <v>2091</v>
       </c>
       <c r="N71" s="1"/>
     </row>
@@ -23325,7 +23393,7 @@
       <c r="D72" s="1"/>
       <c r="E72" s="1"/>
       <c r="F72" s="31" t="s">
-        <v>2106</v>
+        <v>2092</v>
       </c>
       <c r="G72" s="35">
         <v>170.06</v>
@@ -23352,9 +23420,11 @@
       <c r="C73" s="31"/>
       <c r="D73" s="1"/>
       <c r="E73" s="1"/>
-      <c r="F73" s="1"/>
+      <c r="F73" s="1" t="s">
+        <v>2200</v>
+      </c>
       <c r="G73" s="35">
-        <v>10</v>
+        <v>119.12</v>
       </c>
       <c r="H73" s="22">
         <v>0</v>
@@ -23379,7 +23449,7 @@
       <c r="D74" s="1"/>
       <c r="E74" s="1"/>
       <c r="F74" s="31" t="s">
-        <v>2109</v>
+        <v>2095</v>
       </c>
       <c r="G74" s="35">
         <v>220.22</v>
@@ -23410,9 +23480,11 @@
       <c r="C75" s="1"/>
       <c r="D75" s="1"/>
       <c r="E75" s="1"/>
-      <c r="F75" s="26"/>
+      <c r="F75" s="26" t="s">
+        <v>2197</v>
+      </c>
       <c r="G75" s="35">
-        <v>10</v>
+        <v>204.22</v>
       </c>
       <c r="H75" s="22">
         <v>0</v>
@@ -23466,9 +23538,11 @@
       <c r="C77" s="1"/>
       <c r="D77" s="1"/>
       <c r="E77" s="1"/>
-      <c r="F77" s="1"/>
+      <c r="F77" s="1" t="s">
+        <v>2198</v>
+      </c>
       <c r="G77" s="35">
-        <v>10</v>
+        <v>181.19</v>
       </c>
       <c r="H77" s="22">
         <v>0</v>
@@ -23493,7 +23567,7 @@
       <c r="D78" s="1"/>
       <c r="E78" s="1"/>
       <c r="F78" s="31" t="s">
-        <v>2108</v>
+        <v>2094</v>
       </c>
       <c r="G78" s="35">
         <v>344.4</v>
@@ -23519,17 +23593,17 @@
         <v>379</v>
       </c>
       <c r="B79" s="31" t="s">
-        <v>2118</v>
+        <v>2104</v>
       </c>
       <c r="C79" s="31" t="s">
-        <v>2120</v>
+        <v>2106</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>1971</v>
       </c>
       <c r="E79" s="1"/>
       <c r="F79" s="1" t="s">
-        <v>2119</v>
+        <v>2105</v>
       </c>
       <c r="G79" s="35">
         <v>404.16</v>
@@ -23554,8 +23628,11 @@
         <v>380</v>
       </c>
       <c r="C80" s="1"/>
+      <c r="F80" s="3" t="s">
+        <v>2191</v>
+      </c>
       <c r="G80" s="35">
-        <v>10</v>
+        <v>324.18</v>
       </c>
       <c r="H80" s="22">
         <v>0</v>
@@ -23607,14 +23684,14 @@
         <v>389</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>2122</v>
+        <v>2108</v>
       </c>
       <c r="D82" s="1" t="s">
         <v>1971</v>
       </c>
       <c r="E82" s="1"/>
       <c r="F82" s="1" t="s">
-        <v>2121</v>
+        <v>2107</v>
       </c>
       <c r="G82" s="35">
         <v>244.2</v>
@@ -23671,9 +23748,11 @@
       <c r="C84" s="1"/>
       <c r="D84" s="1"/>
       <c r="E84" s="1"/>
-      <c r="F84" s="1"/>
+      <c r="F84" s="1" t="s">
+        <v>2199</v>
+      </c>
       <c r="G84" s="35">
-        <v>10</v>
+        <v>117.15</v>
       </c>
       <c r="H84" s="22">
         <v>0</v>
@@ -23698,7 +23777,7 @@
       <c r="D85" s="1"/>
       <c r="E85" s="1"/>
       <c r="F85" s="31" t="s">
-        <v>2107</v>
+        <v>2093</v>
       </c>
       <c r="G85" s="35">
         <v>216.28</v>
@@ -23757,7 +23836,7 @@
       <c r="E87" s="1"/>
       <c r="F87" s="1"/>
       <c r="G87" s="37">
-        <v>40000</v>
+        <v>12993</v>
       </c>
       <c r="H87" s="22">
         <v>0</v>
@@ -23769,11 +23848,9 @@
       <c r="K87" s="1"/>
       <c r="L87" s="1"/>
       <c r="M87" s="1" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N87" s="25" t="s">
-        <v>2089</v>
-      </c>
+        <v>2202</v>
+      </c>
+      <c r="N87" s="25"/>
     </row>
     <row r="88" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
@@ -23787,7 +23864,7 @@
       <c r="E88" s="1"/>
       <c r="F88" s="1"/>
       <c r="G88" s="37">
-        <v>40000</v>
+        <v>13373</v>
       </c>
       <c r="H88" s="22">
         <v>0</v>
@@ -23798,12 +23875,10 @@
       <c r="J88" s="1"/>
       <c r="K88" s="1"/>
       <c r="L88" s="1"/>
-      <c r="M88" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N88" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M88" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N88" s="25"/>
     </row>
     <row r="89" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
@@ -23817,7 +23892,7 @@
       <c r="E89" s="1"/>
       <c r="F89" s="1"/>
       <c r="G89" s="37">
-        <v>40000</v>
+        <v>13082</v>
       </c>
       <c r="H89" s="22">
         <v>0</v>
@@ -23828,12 +23903,10 @@
       <c r="J89" s="1"/>
       <c r="K89" s="1"/>
       <c r="L89" s="1"/>
-      <c r="M89" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N89" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M89" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N89" s="25"/>
     </row>
     <row r="90" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
@@ -23847,7 +23920,7 @@
       <c r="E90" s="1"/>
       <c r="F90" s="1"/>
       <c r="G90" s="37">
-        <v>40000</v>
+        <v>13273</v>
       </c>
       <c r="H90" s="22">
         <v>0</v>
@@ -23858,12 +23931,10 @@
       <c r="J90" s="1"/>
       <c r="K90" s="1"/>
       <c r="L90" s="1"/>
-      <c r="M90" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N90" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M90" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N90" s="25"/>
     </row>
     <row r="91" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
@@ -23877,7 +23948,7 @@
       <c r="E91" s="1"/>
       <c r="F91" s="1"/>
       <c r="G91" s="37">
-        <v>40000</v>
+        <v>13041</v>
       </c>
       <c r="H91" s="22">
         <v>0</v>
@@ -23888,12 +23959,10 @@
       <c r="J91" s="1"/>
       <c r="K91" s="1"/>
       <c r="L91" s="1"/>
-      <c r="M91" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N91" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M91" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N91" s="25"/>
     </row>
     <row r="92" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
@@ -23907,7 +23976,7 @@
       <c r="E92" s="1"/>
       <c r="F92" s="1"/>
       <c r="G92" s="37">
-        <v>40000</v>
+        <v>13344</v>
       </c>
       <c r="H92" s="22">
         <v>0</v>
@@ -23918,12 +23987,10 @@
       <c r="J92" s="1"/>
       <c r="K92" s="1"/>
       <c r="L92" s="1"/>
-      <c r="M92" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N92" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M92" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N92" s="25"/>
     </row>
     <row r="93" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
@@ -23937,7 +24004,7 @@
       <c r="E93" s="1"/>
       <c r="F93" s="1"/>
       <c r="G93" s="37">
-        <v>40000</v>
+        <v>12484</v>
       </c>
       <c r="H93" s="22">
         <v>0</v>
@@ -23948,12 +24015,10 @@
       <c r="J93" s="1"/>
       <c r="K93" s="1"/>
       <c r="L93" s="1"/>
-      <c r="M93" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N93" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M93" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N93" s="25"/>
     </row>
     <row r="94" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
@@ -23967,7 +24032,7 @@
       <c r="E94" s="1"/>
       <c r="F94" s="1"/>
       <c r="G94" s="37">
-        <v>40000</v>
+        <v>13037</v>
       </c>
       <c r="H94" s="22">
         <v>0</v>
@@ -23978,12 +24043,10 @@
       <c r="J94" s="1"/>
       <c r="K94" s="1"/>
       <c r="L94" s="1"/>
-      <c r="M94" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N94" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M94" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N94" s="25"/>
     </row>
     <row r="95" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
@@ -23997,7 +24060,7 @@
       <c r="E95" s="1"/>
       <c r="F95" s="1"/>
       <c r="G95" s="37">
-        <v>40000</v>
+        <v>12685</v>
       </c>
       <c r="H95" s="22">
         <v>0</v>
@@ -24008,12 +24071,10 @@
       <c r="J95" s="1"/>
       <c r="K95" s="1"/>
       <c r="L95" s="1"/>
-      <c r="M95" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N95" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M95" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N95" s="25"/>
     </row>
     <row r="96" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
@@ -24027,7 +24088,7 @@
       <c r="E96" s="1"/>
       <c r="F96" s="1"/>
       <c r="G96" s="37">
-        <v>40000</v>
+        <v>12975</v>
       </c>
       <c r="H96" s="22">
         <v>0</v>
@@ -24038,12 +24099,10 @@
       <c r="J96" s="1"/>
       <c r="K96" s="1"/>
       <c r="L96" s="1"/>
-      <c r="M96" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N96" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M96" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N96" s="25"/>
     </row>
     <row r="97" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
@@ -24057,7 +24116,7 @@
       <c r="E97" s="1"/>
       <c r="F97" s="1"/>
       <c r="G97" s="37">
-        <v>40000</v>
+        <v>12911</v>
       </c>
       <c r="H97" s="22">
         <v>0</v>
@@ -24068,12 +24127,10 @@
       <c r="J97" s="1"/>
       <c r="K97" s="1"/>
       <c r="L97" s="1"/>
-      <c r="M97" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N97" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M97" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N97" s="25"/>
     </row>
     <row r="98" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
@@ -24087,7 +24144,7 @@
       <c r="E98" s="1"/>
       <c r="F98" s="1"/>
       <c r="G98" s="37">
-        <v>40000</v>
+        <v>13040</v>
       </c>
       <c r="H98" s="22">
         <v>0</v>
@@ -24098,12 +24155,10 @@
       <c r="J98" s="1"/>
       <c r="K98" s="1"/>
       <c r="L98" s="1"/>
-      <c r="M98" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N98" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M98" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N98" s="25"/>
     </row>
     <row r="99" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
@@ -24117,7 +24172,7 @@
       <c r="E99" s="1"/>
       <c r="F99" s="1"/>
       <c r="G99" s="37">
-        <v>40000</v>
+        <v>13202</v>
       </c>
       <c r="H99" s="22">
         <v>0</v>
@@ -24128,12 +24183,10 @@
       <c r="J99" s="1"/>
       <c r="K99" s="1"/>
       <c r="L99" s="1"/>
-      <c r="M99" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N99" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M99" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N99" s="25"/>
     </row>
     <row r="100" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
@@ -24147,7 +24200,7 @@
       <c r="E100" s="1"/>
       <c r="F100" s="1"/>
       <c r="G100" s="37">
-        <v>40000</v>
+        <v>12940</v>
       </c>
       <c r="H100" s="22">
         <v>0</v>
@@ -24158,12 +24211,10 @@
       <c r="J100" s="1"/>
       <c r="K100" s="1"/>
       <c r="L100" s="1"/>
-      <c r="M100" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N100" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M100" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N100" s="25"/>
     </row>
     <row r="101" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
@@ -24177,7 +24228,7 @@
       <c r="E101" s="1"/>
       <c r="F101" s="1"/>
       <c r="G101" s="37">
-        <v>40000</v>
+        <v>12616</v>
       </c>
       <c r="H101" s="22">
         <v>0</v>
@@ -24188,12 +24239,10 @@
       <c r="J101" s="1"/>
       <c r="K101" s="1"/>
       <c r="L101" s="1"/>
-      <c r="M101" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N101" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M101" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N101" s="25"/>
     </row>
     <row r="102" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
@@ -24207,7 +24256,7 @@
       <c r="E102" s="1"/>
       <c r="F102" s="1"/>
       <c r="G102" s="37">
-        <v>40000</v>
+        <v>13205</v>
       </c>
       <c r="H102" s="22">
         <v>0</v>
@@ -24218,12 +24267,10 @@
       <c r="J102" s="1"/>
       <c r="K102" s="1"/>
       <c r="L102" s="1"/>
-      <c r="M102" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N102" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M102" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N102" s="25"/>
     </row>
     <row r="103" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
@@ -24237,7 +24284,7 @@
       <c r="E103" s="1"/>
       <c r="F103" s="1"/>
       <c r="G103" s="37">
-        <v>40000</v>
+        <v>12592</v>
       </c>
       <c r="H103" s="22">
         <v>0</v>
@@ -24248,12 +24295,10 @@
       <c r="J103" s="1"/>
       <c r="K103" s="1"/>
       <c r="L103" s="1"/>
-      <c r="M103" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N103" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M103" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N103" s="25"/>
     </row>
     <row r="104" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
@@ -24267,7 +24312,7 @@
       <c r="E104" s="1"/>
       <c r="F104" s="1"/>
       <c r="G104" s="37">
-        <v>40000</v>
+        <v>13464</v>
       </c>
       <c r="H104" s="22">
         <v>0</v>
@@ -24278,12 +24323,10 @@
       <c r="J104" s="1"/>
       <c r="K104" s="1"/>
       <c r="L104" s="1"/>
-      <c r="M104" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N104" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M104" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N104" s="25"/>
     </row>
     <row r="105" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
@@ -24297,7 +24340,7 @@
       <c r="E105" s="1"/>
       <c r="F105" s="1"/>
       <c r="G105" s="37">
-        <v>40000</v>
+        <v>12879</v>
       </c>
       <c r="H105" s="22">
         <v>0</v>
@@ -24308,12 +24351,10 @@
       <c r="J105" s="1"/>
       <c r="K105" s="1"/>
       <c r="L105" s="1"/>
-      <c r="M105" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N105" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M105" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N105" s="25"/>
     </row>
     <row r="106" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
@@ -24327,7 +24368,7 @@
       <c r="E106" s="1"/>
       <c r="F106" s="1"/>
       <c r="G106" s="37">
-        <v>40000</v>
+        <v>12813</v>
       </c>
       <c r="H106" s="22">
         <v>0</v>
@@ -24338,12 +24379,10 @@
       <c r="J106" s="1"/>
       <c r="K106" s="1"/>
       <c r="L106" s="1"/>
-      <c r="M106" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N106" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M106" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N106" s="25"/>
     </row>
     <row r="107" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
@@ -24357,7 +24396,7 @@
       <c r="E107" s="1"/>
       <c r="F107" s="1"/>
       <c r="G107" s="37">
-        <v>40000</v>
+        <v>12971</v>
       </c>
       <c r="H107" s="22">
         <v>0</v>
@@ -24368,12 +24407,10 @@
       <c r="J107" s="1"/>
       <c r="K107" s="1"/>
       <c r="L107" s="1"/>
-      <c r="M107" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N107" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M107" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N107" s="25"/>
     </row>
     <row r="108" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
@@ -24387,7 +24424,7 @@
       <c r="E108" s="1"/>
       <c r="F108" s="1"/>
       <c r="G108" s="37">
-        <v>40000</v>
+        <v>12981</v>
       </c>
       <c r="H108" s="22">
         <v>0</v>
@@ -24398,12 +24435,10 @@
       <c r="J108" s="1"/>
       <c r="K108" s="1"/>
       <c r="L108" s="1"/>
-      <c r="M108" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N108" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M108" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N108" s="25"/>
     </row>
     <row r="109" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
@@ -24417,7 +24452,7 @@
       <c r="E109" s="1"/>
       <c r="F109" s="1"/>
       <c r="G109" s="37">
-        <v>40000</v>
+        <v>12964</v>
       </c>
       <c r="H109" s="22">
         <v>0</v>
@@ -24428,12 +24463,10 @@
       <c r="J109" s="1"/>
       <c r="K109" s="1"/>
       <c r="L109" s="1"/>
-      <c r="M109" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N109" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M109" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N109" s="25"/>
     </row>
     <row r="110" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
@@ -24447,7 +24480,7 @@
       <c r="E110" s="1"/>
       <c r="F110" s="1"/>
       <c r="G110" s="37">
-        <v>40000</v>
+        <v>13822</v>
       </c>
       <c r="H110" s="22">
         <v>0</v>
@@ -24458,12 +24491,10 @@
       <c r="J110" s="1"/>
       <c r="K110" s="1"/>
       <c r="L110" s="1"/>
-      <c r="M110" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N110" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M110" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N110" s="25"/>
     </row>
     <row r="111" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="1" t="s">
@@ -24477,7 +24508,7 @@
       <c r="E111" s="1"/>
       <c r="F111" s="1"/>
       <c r="G111" s="37">
-        <v>40000</v>
+        <v>13181</v>
       </c>
       <c r="H111" s="22">
         <v>0</v>
@@ -24488,12 +24519,10 @@
       <c r="J111" s="1"/>
       <c r="K111" s="1"/>
       <c r="L111" s="1"/>
-      <c r="M111" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N111" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M111" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N111" s="25"/>
     </row>
     <row r="112" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="1" t="s">
@@ -24507,7 +24536,7 @@
       <c r="E112" s="1"/>
       <c r="F112" s="1"/>
       <c r="G112" s="37">
-        <v>40000</v>
+        <v>13339</v>
       </c>
       <c r="H112" s="22">
         <v>0</v>
@@ -24518,12 +24547,10 @@
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
       <c r="L112" s="1"/>
-      <c r="M112" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N112" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M112" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N112" s="25"/>
     </row>
     <row r="113" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="1" t="s">
@@ -24537,7 +24564,7 @@
       <c r="E113" s="1"/>
       <c r="F113" s="1"/>
       <c r="G113" s="37">
-        <v>40000</v>
+        <v>13216</v>
       </c>
       <c r="H113" s="22">
         <v>0</v>
@@ -24548,12 +24575,10 @@
       <c r="J113" s="1"/>
       <c r="K113" s="1"/>
       <c r="L113" s="1"/>
-      <c r="M113" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N113" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M113" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N113" s="25"/>
     </row>
     <row r="114" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="1" t="s">
@@ -24567,7 +24592,7 @@
       <c r="E114" s="1"/>
       <c r="F114" s="1"/>
       <c r="G114" s="37">
-        <v>40000</v>
+        <v>12672</v>
       </c>
       <c r="H114" s="22">
         <v>0</v>
@@ -24578,12 +24603,10 @@
       <c r="J114" s="1"/>
       <c r="K114" s="1"/>
       <c r="L114" s="1"/>
-      <c r="M114" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N114" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M114" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N114" s="25"/>
     </row>
     <row r="115" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="1" t="s">
@@ -24597,7 +24620,7 @@
       <c r="E115" s="1"/>
       <c r="F115" s="1"/>
       <c r="G115" s="37">
-        <v>40000</v>
+        <v>12588</v>
       </c>
       <c r="H115" s="22">
         <v>0</v>
@@ -24608,12 +24631,10 @@
       <c r="J115" s="1"/>
       <c r="K115" s="1"/>
       <c r="L115" s="1"/>
-      <c r="M115" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N115" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M115" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N115" s="25"/>
     </row>
     <row r="116" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="1" t="s">
@@ -24627,7 +24648,7 @@
       <c r="E116" s="1"/>
       <c r="F116" s="1"/>
       <c r="G116" s="37">
-        <v>40000</v>
+        <v>12946</v>
       </c>
       <c r="H116" s="22">
         <v>0</v>
@@ -24638,12 +24659,10 @@
       <c r="J116" s="1"/>
       <c r="K116" s="1"/>
       <c r="L116" s="1"/>
-      <c r="M116" s="26" t="s">
-        <v>2088</v>
-      </c>
-      <c r="N116" s="25" t="s">
-        <v>2089</v>
-      </c>
+      <c r="M116" s="38" t="s">
+        <v>2202</v>
+      </c>
+      <c r="N116" s="25"/>
     </row>
     <row r="117" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="1" t="s">
@@ -24657,7 +24676,7 @@
       <c r="E117" s="1"/>
       <c r="F117" s="1"/>
       <c r="G117" s="37">
-        <v>400000</v>
+        <v>103377</v>
       </c>
       <c r="H117" s="22">
         <v>0</v>
@@ -24668,12 +24687,10 @@
       <c r="J117" s="1"/>
       <c r="K117" s="1"/>
       <c r="L117" s="1"/>
-      <c r="M117" s="1" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N117" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M117" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N117" s="25"/>
     </row>
     <row r="118" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="1" t="s">
@@ -24687,7 +24704,7 @@
       <c r="E118" s="1"/>
       <c r="F118" s="1"/>
       <c r="G118" s="37">
-        <v>400000</v>
+        <v>102347</v>
       </c>
       <c r="H118" s="22">
         <v>0</v>
@@ -24698,12 +24715,10 @@
       <c r="J118" s="1"/>
       <c r="K118" s="1"/>
       <c r="L118" s="1"/>
-      <c r="M118" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N118" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M118" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N118" s="25"/>
     </row>
     <row r="119" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="1" t="s">
@@ -24717,7 +24732,7 @@
       <c r="E119" s="1"/>
       <c r="F119" s="1"/>
       <c r="G119" s="37">
-        <v>400000</v>
+        <v>102839</v>
       </c>
       <c r="H119" s="22">
         <v>0</v>
@@ -24728,12 +24743,10 @@
       <c r="J119" s="1"/>
       <c r="K119" s="1"/>
       <c r="L119" s="1"/>
-      <c r="M119" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N119" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M119" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N119" s="25"/>
     </row>
     <row r="120" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="1" t="s">
@@ -24747,7 +24760,7 @@
       <c r="E120" s="1"/>
       <c r="F120" s="1"/>
       <c r="G120" s="37">
-        <v>400000</v>
+        <v>102660</v>
       </c>
       <c r="H120" s="22">
         <v>0</v>
@@ -24758,12 +24771,10 @@
       <c r="J120" s="1"/>
       <c r="K120" s="1"/>
       <c r="L120" s="1"/>
-      <c r="M120" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N120" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M120" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N120" s="25"/>
     </row>
     <row r="121" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="1" t="s">
@@ -24777,7 +24788,7 @@
       <c r="E121" s="1"/>
       <c r="F121" s="1"/>
       <c r="G121" s="37">
-        <v>400000</v>
+        <v>102747</v>
       </c>
       <c r="H121" s="22">
         <v>0</v>
@@ -24788,12 +24799,10 @@
       <c r="J121" s="1"/>
       <c r="K121" s="1"/>
       <c r="L121" s="1"/>
-      <c r="M121" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N121" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M121" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N121" s="25"/>
     </row>
     <row r="122" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="1" t="s">
@@ -24807,7 +24816,7 @@
       <c r="E122" s="1"/>
       <c r="F122" s="1"/>
       <c r="G122" s="37">
-        <v>400000</v>
+        <v>102674</v>
       </c>
       <c r="H122" s="22">
         <v>0</v>
@@ -24818,12 +24827,10 @@
       <c r="J122" s="1"/>
       <c r="K122" s="1"/>
       <c r="L122" s="1"/>
-      <c r="M122" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N122" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M122" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N122" s="25"/>
     </row>
     <row r="123" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="1" t="s">
@@ -24837,7 +24844,7 @@
       <c r="E123" s="1"/>
       <c r="F123" s="1"/>
       <c r="G123" s="37">
-        <v>400000</v>
+        <v>102683</v>
       </c>
       <c r="H123" s="22">
         <v>0</v>
@@ -24848,12 +24855,10 @@
       <c r="J123" s="1"/>
       <c r="K123" s="1"/>
       <c r="L123" s="1"/>
-      <c r="M123" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N123" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M123" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N123" s="25"/>
     </row>
     <row r="124" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="1" t="s">
@@ -24867,7 +24872,7 @@
       <c r="E124" s="1"/>
       <c r="F124" s="1"/>
       <c r="G124" s="37">
-        <v>400000</v>
+        <v>103220</v>
       </c>
       <c r="H124" s="22">
         <v>0</v>
@@ -24878,12 +24883,10 @@
       <c r="J124" s="1"/>
       <c r="K124" s="1"/>
       <c r="L124" s="1"/>
-      <c r="M124" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N124" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M124" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N124" s="25"/>
     </row>
     <row r="125" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="1" t="s">
@@ -24897,7 +24900,7 @@
       <c r="E125" s="1"/>
       <c r="F125" s="1"/>
       <c r="G125" s="37">
-        <v>400000</v>
+        <v>102958</v>
       </c>
       <c r="H125" s="22">
         <v>0</v>
@@ -24908,12 +24911,10 @@
       <c r="J125" s="1"/>
       <c r="K125" s="1"/>
       <c r="L125" s="1"/>
-      <c r="M125" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N125" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M125" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N125" s="25"/>
     </row>
     <row r="126" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="1" t="s">
@@ -24927,7 +24928,7 @@
       <c r="E126" s="1"/>
       <c r="F126" s="1"/>
       <c r="G126" s="37">
-        <v>400000</v>
+        <v>102891</v>
       </c>
       <c r="H126" s="22">
         <v>0</v>
@@ -24938,12 +24939,10 @@
       <c r="J126" s="1"/>
       <c r="K126" s="1"/>
       <c r="L126" s="1"/>
-      <c r="M126" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N126" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M126" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N126" s="25"/>
     </row>
     <row r="127" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A127" s="1" t="s">
@@ -24957,7 +24956,7 @@
       <c r="E127" s="1"/>
       <c r="F127" s="1"/>
       <c r="G127" s="37">
-        <v>400000</v>
+        <v>102763</v>
       </c>
       <c r="H127" s="22">
         <v>0</v>
@@ -24968,12 +24967,10 @@
       <c r="J127" s="1"/>
       <c r="K127" s="1"/>
       <c r="L127" s="1"/>
-      <c r="M127" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N127" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M127" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N127" s="25"/>
     </row>
     <row r="128" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A128" s="1" t="s">
@@ -24987,7 +24984,7 @@
       <c r="E128" s="1"/>
       <c r="F128" s="1"/>
       <c r="G128" s="37">
-        <v>400000</v>
+        <v>102817</v>
       </c>
       <c r="H128" s="22">
         <v>0</v>
@@ -24998,12 +24995,10 @@
       <c r="J128" s="1"/>
       <c r="K128" s="1"/>
       <c r="L128" s="1"/>
-      <c r="M128" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N128" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M128" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N128" s="25"/>
     </row>
     <row r="129" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="1" t="s">
@@ -25017,7 +25012,7 @@
       <c r="E129" s="1"/>
       <c r="F129" s="1"/>
       <c r="G129" s="37">
-        <v>400000</v>
+        <v>102594</v>
       </c>
       <c r="H129" s="22">
         <v>0</v>
@@ -25028,12 +25023,10 @@
       <c r="J129" s="1"/>
       <c r="K129" s="1"/>
       <c r="L129" s="1"/>
-      <c r="M129" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N129" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M129" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N129" s="25"/>
     </row>
     <row r="130" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="1" t="s">
@@ -25047,7 +25040,7 @@
       <c r="E130" s="1"/>
       <c r="F130" s="1"/>
       <c r="G130" s="37">
-        <v>400000</v>
+        <v>103200</v>
       </c>
       <c r="H130" s="22">
         <v>0</v>
@@ -25058,12 +25051,10 @@
       <c r="J130" s="1"/>
       <c r="K130" s="1"/>
       <c r="L130" s="1"/>
-      <c r="M130" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N130" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M130" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N130" s="25"/>
     </row>
     <row r="131" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="1" t="s">
@@ -25077,7 +25068,7 @@
       <c r="E131" s="1"/>
       <c r="F131" s="1"/>
       <c r="G131" s="37">
-        <v>400000</v>
+        <v>102608</v>
       </c>
       <c r="H131" s="22">
         <v>0</v>
@@ -25088,12 +25079,10 @@
       <c r="J131" s="1"/>
       <c r="K131" s="1"/>
       <c r="L131" s="1"/>
-      <c r="M131" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N131" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M131" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N131" s="25"/>
     </row>
     <row r="132" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="1" t="s">
@@ -25107,7 +25096,7 @@
       <c r="E132" s="1"/>
       <c r="F132" s="1"/>
       <c r="G132" s="37">
-        <v>400000</v>
+        <v>102639</v>
       </c>
       <c r="H132" s="22">
         <v>0</v>
@@ -25118,12 +25107,10 @@
       <c r="J132" s="1"/>
       <c r="K132" s="1"/>
       <c r="L132" s="1"/>
-      <c r="M132" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N132" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M132" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N132" s="25"/>
     </row>
     <row r="133" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="1" t="s">
@@ -25137,7 +25124,7 @@
       <c r="E133" s="1"/>
       <c r="F133" s="1"/>
       <c r="G133" s="37">
-        <v>400000</v>
+        <v>102733</v>
       </c>
       <c r="H133" s="22">
         <v>0</v>
@@ -25148,12 +25135,10 @@
       <c r="J133" s="1"/>
       <c r="K133" s="1"/>
       <c r="L133" s="1"/>
-      <c r="M133" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N133" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M133" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N133" s="25"/>
     </row>
     <row r="134" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="1" t="s">
@@ -25167,7 +25152,7 @@
       <c r="E134" s="1"/>
       <c r="F134" s="1"/>
       <c r="G134" s="37">
-        <v>400000</v>
+        <v>102633</v>
       </c>
       <c r="H134" s="22">
         <v>0</v>
@@ -25178,12 +25163,10 @@
       <c r="J134" s="1"/>
       <c r="K134" s="1"/>
       <c r="L134" s="1"/>
-      <c r="M134" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N134" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M134" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N134" s="25"/>
     </row>
     <row r="135" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="1" t="s">
@@ -25197,7 +25180,7 @@
       <c r="E135" s="1"/>
       <c r="F135" s="1"/>
       <c r="G135" s="37">
-        <v>400000</v>
+        <v>103058</v>
       </c>
       <c r="H135" s="22">
         <v>0</v>
@@ -25208,12 +25191,10 @@
       <c r="J135" s="1"/>
       <c r="K135" s="1"/>
       <c r="L135" s="1"/>
-      <c r="M135" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N135" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M135" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N135" s="25"/>
     </row>
     <row r="136" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="1" t="s">
@@ -25227,7 +25208,7 @@
       <c r="E136" s="1"/>
       <c r="F136" s="1"/>
       <c r="G136" s="37">
-        <v>400000</v>
+        <v>102607</v>
       </c>
       <c r="H136" s="22">
         <v>0</v>
@@ -25238,12 +25219,10 @@
       <c r="J136" s="1"/>
       <c r="K136" s="1"/>
       <c r="L136" s="1"/>
-      <c r="M136" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N136" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M136" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N136" s="25"/>
     </row>
     <row r="137" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1" t="s">
@@ -25257,7 +25236,7 @@
       <c r="E137" s="1"/>
       <c r="F137" s="1"/>
       <c r="G137" s="37">
-        <v>400000</v>
+        <v>102843</v>
       </c>
       <c r="H137" s="22">
         <v>0</v>
@@ -25268,12 +25247,10 @@
       <c r="J137" s="1"/>
       <c r="K137" s="1"/>
       <c r="L137" s="1"/>
-      <c r="M137" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N137" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M137" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N137" s="25"/>
     </row>
     <row r="138" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="1" t="s">
@@ -25287,7 +25264,7 @@
       <c r="E138" s="1"/>
       <c r="F138" s="1"/>
       <c r="G138" s="37">
-        <v>400000</v>
+        <v>102243</v>
       </c>
       <c r="H138" s="22">
         <v>0</v>
@@ -25298,12 +25275,10 @@
       <c r="J138" s="1"/>
       <c r="K138" s="1"/>
       <c r="L138" s="1"/>
-      <c r="M138" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N138" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M138" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N138" s="25"/>
     </row>
     <row r="139" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="1" t="s">
@@ -25317,7 +25292,7 @@
       <c r="E139" s="1"/>
       <c r="F139" s="1"/>
       <c r="G139" s="37">
-        <v>400000</v>
+        <v>102482</v>
       </c>
       <c r="H139" s="22">
         <v>0</v>
@@ -25328,12 +25303,10 @@
       <c r="J139" s="1"/>
       <c r="K139" s="1"/>
       <c r="L139" s="1"/>
-      <c r="M139" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N139" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M139" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N139" s="25"/>
     </row>
     <row r="140" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="1" t="s">
@@ -25347,7 +25320,7 @@
       <c r="E140" s="1"/>
       <c r="F140" s="1"/>
       <c r="G140" s="37">
-        <v>400000</v>
+        <v>102713</v>
       </c>
       <c r="H140" s="22">
         <v>0</v>
@@ -25358,12 +25331,10 @@
       <c r="J140" s="1"/>
       <c r="K140" s="1"/>
       <c r="L140" s="1"/>
-      <c r="M140" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N140" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M140" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N140" s="25"/>
     </row>
     <row r="141" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="1" t="s">
@@ -25377,7 +25348,7 @@
       <c r="E141" s="1"/>
       <c r="F141" s="1"/>
       <c r="G141" s="37">
-        <v>400000</v>
+        <v>102884</v>
       </c>
       <c r="H141" s="22">
         <v>0</v>
@@ -25388,12 +25359,10 @@
       <c r="J141" s="1"/>
       <c r="K141" s="1"/>
       <c r="L141" s="1"/>
-      <c r="M141" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N141" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M141" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N141" s="25"/>
     </row>
     <row r="142" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="1" t="s">
@@ -25407,7 +25376,7 @@
       <c r="E142" s="1"/>
       <c r="F142" s="1"/>
       <c r="G142" s="37">
-        <v>400000</v>
+        <v>103336</v>
       </c>
       <c r="H142" s="22">
         <v>0</v>
@@ -25418,12 +25387,10 @@
       <c r="J142" s="1"/>
       <c r="K142" s="1"/>
       <c r="L142" s="1"/>
-      <c r="M142" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N142" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M142" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N142" s="25"/>
     </row>
     <row r="143" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="1" t="s">
@@ -25437,7 +25404,7 @@
       <c r="E143" s="1"/>
       <c r="F143" s="1"/>
       <c r="G143" s="37">
-        <v>400000</v>
+        <v>102770</v>
       </c>
       <c r="H143" s="22">
         <v>0</v>
@@ -25448,12 +25415,10 @@
       <c r="J143" s="1"/>
       <c r="K143" s="1"/>
       <c r="L143" s="1"/>
-      <c r="M143" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N143" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M143" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N143" s="25"/>
     </row>
     <row r="144" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="1" t="s">
@@ -25467,7 +25432,7 @@
       <c r="E144" s="1"/>
       <c r="F144" s="1"/>
       <c r="G144" s="37">
-        <v>400000</v>
+        <v>102618</v>
       </c>
       <c r="H144" s="22">
         <v>0</v>
@@ -25478,12 +25443,10 @@
       <c r="J144" s="1"/>
       <c r="K144" s="1"/>
       <c r="L144" s="1"/>
-      <c r="M144" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N144" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M144" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N144" s="25"/>
     </row>
     <row r="145" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="1" t="s">
@@ -25497,7 +25460,7 @@
       <c r="E145" s="1"/>
       <c r="F145" s="1"/>
       <c r="G145" s="37">
-        <v>400000</v>
+        <v>103049</v>
       </c>
       <c r="H145" s="22">
         <v>0</v>
@@ -25508,14 +25471,12 @@
       <c r="J145" s="1"/>
       <c r="K145" s="1"/>
       <c r="L145" s="1"/>
-      <c r="M145" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N145" s="25" t="s">
-        <v>2096</v>
-      </c>
-    </row>
-    <row r="146" spans="1:14" ht="42" x14ac:dyDescent="0.2">
+      <c r="M145" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N145" s="25"/>
+    </row>
+    <row r="146" spans="1:14" ht="22" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="1" t="s">
         <v>383</v>
       </c>
@@ -25527,7 +25488,7 @@
       <c r="E146" s="1"/>
       <c r="F146" s="1"/>
       <c r="G146" s="37">
-        <v>400000</v>
+        <v>102425</v>
       </c>
       <c r="H146" s="22">
         <v>0</v>
@@ -25538,17 +25499,15 @@
       <c r="J146" s="1"/>
       <c r="K146" s="1"/>
       <c r="L146" s="1"/>
-      <c r="M146" s="26" t="s">
-        <v>2100</v>
-      </c>
-      <c r="N146" s="25" t="s">
-        <v>2096</v>
-      </c>
+      <c r="M146" s="38" t="s">
+        <v>2201</v>
+      </c>
+      <c r="N146" s="25"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:N146"/>
-  <sortState ref="A4:N146">
-    <sortCondition ref="I4:I146"/>
+  <sortState ref="A87:N116">
+    <sortCondition ref="A87:A116"/>
   </sortState>
   <mergeCells count="1">
     <mergeCell ref="C2:H2"/>
@@ -28248,14 +28207,14 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L129"/>
+  <dimension ref="A1:L152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A101" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F129" sqref="F129"/>
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E140" sqref="E140"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="A107" workbookViewId="1">
+      <selection activeCell="E152" sqref="E152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -31685,10 +31644,648 @@
       </c>
     </row>
     <row r="128" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D128" s="12"/>
-    </row>
-    <row r="129" spans="6:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="F129" s="43"/>
+      <c r="A128" s="3" t="s">
+        <v>2151</v>
+      </c>
+      <c r="C128" s="3" t="s">
+        <v>400</v>
+      </c>
+      <c r="D128" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="E128" s="44">
+        <v>3.4499999999999998E-5</v>
+      </c>
+      <c r="F128" s="44">
+        <v>5.8736700000000001E-3</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="L128" s="3" t="s">
+        <v>2144</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="3" t="s">
+        <v>2152</v>
+      </c>
+      <c r="C129" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="D129" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E129" s="44">
+        <v>2.62E-5</v>
+      </c>
+      <c r="F129" s="44">
+        <v>5.1185900000000001E-3</v>
+      </c>
+      <c r="G129" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="L129" s="3" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="3" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C130" s="3" t="s">
+        <v>422</v>
+      </c>
+      <c r="D130" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E130" s="44">
+        <v>1.44E-4</v>
+      </c>
+      <c r="F130" s="44">
+        <v>1.2E-2</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K130" s="28" t="s">
+        <v>2163</v>
+      </c>
+      <c r="L130" s="3" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="131" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A131" s="3" t="s">
+        <v>2154</v>
+      </c>
+      <c r="C131" s="3" t="s">
+        <v>432</v>
+      </c>
+      <c r="D131" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E131" s="44">
+        <v>2.5900000000000002E-6</v>
+      </c>
+      <c r="F131" s="44">
+        <v>1.6093500000000001E-3</v>
+      </c>
+      <c r="G131" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K131" s="28" t="s">
+        <v>2155</v>
+      </c>
+      <c r="L131" s="3" t="s">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A132" s="3" t="s">
+        <v>2156</v>
+      </c>
+      <c r="C132" s="3" t="s">
+        <v>434</v>
+      </c>
+      <c r="D132" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E132" s="44">
+        <v>2.241537559E-6</v>
+      </c>
+      <c r="F132" s="44">
+        <v>1.4971800000000001E-3</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K132" s="28" t="s">
+        <v>2157</v>
+      </c>
+      <c r="L132" s="3" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A133" s="3" t="s">
+        <v>2158</v>
+      </c>
+      <c r="C133" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="D133" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E133" s="44">
+        <v>2.7999999999999999E-6</v>
+      </c>
+      <c r="F133" s="44">
+        <v>1.6733200000000001E-3</v>
+      </c>
+      <c r="G133" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K133" s="28" t="s">
+        <v>2159</v>
+      </c>
+      <c r="L133" s="3" t="s">
+        <v>2121</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A134" s="3" t="s">
+        <v>2160</v>
+      </c>
+      <c r="C134" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="D134" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E134" s="44">
+        <v>2.5240096860000001E-3</v>
+      </c>
+      <c r="F134" s="44">
+        <v>5.0239499999999999E-2</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K134" s="28" t="s">
+        <v>2161</v>
+      </c>
+      <c r="L134" s="3" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="135" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="3" t="s">
+        <v>2162</v>
+      </c>
+      <c r="C135" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="D135" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E135" s="44">
+        <v>1.52E-2</v>
+      </c>
+      <c r="F135" s="44">
+        <v>0.12328799999999999</v>
+      </c>
+      <c r="G135" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K135" s="28" t="s">
+        <v>2161</v>
+      </c>
+      <c r="L135" s="3" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="136" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A136" s="3" t="s">
+        <v>2164</v>
+      </c>
+      <c r="C136" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="D136" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E136" s="44">
+        <v>2.3839486979999999E-5</v>
+      </c>
+      <c r="F136" s="44">
+        <v>4.8825700000000001E-3</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K136" s="28" t="s">
+        <v>2165</v>
+      </c>
+      <c r="L136" s="3" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="137" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A137" s="3" t="s">
+        <v>2166</v>
+      </c>
+      <c r="C137" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="D137" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E137" s="44">
+        <v>1.5399999999999999E-3</v>
+      </c>
+      <c r="F137" s="44">
+        <v>3.9242800000000001E-2</v>
+      </c>
+      <c r="G137" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K137" s="28" t="s">
+        <v>2167</v>
+      </c>
+      <c r="L137" s="3" t="s">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="138" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="3" t="s">
+        <v>2168</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="D138" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E138" s="44">
+        <v>1.15E-3</v>
+      </c>
+      <c r="F138" s="44">
+        <v>3.39116E-2</v>
+      </c>
+      <c r="G138" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K138" s="28" t="s">
+        <v>2169</v>
+      </c>
+      <c r="L138" s="3" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="139" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="3" t="s">
+        <v>2170</v>
+      </c>
+      <c r="C139" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="D139" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E139" s="44">
+        <v>6.5099999999999997E-5</v>
+      </c>
+      <c r="F139" s="44">
+        <v>8.0684599999999995E-3</v>
+      </c>
+      <c r="G139" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K139" s="28" t="s">
+        <v>2171</v>
+      </c>
+      <c r="L139" s="3" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="140" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A140" s="3" t="s">
+        <v>2172</v>
+      </c>
+      <c r="C140" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="D140" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E140" s="44">
+        <v>4.7952699999999999E-5</v>
+      </c>
+      <c r="F140" s="44">
+        <v>6.9247900000000001E-3</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K140" s="28" t="s">
+        <v>2173</v>
+      </c>
+      <c r="L140" s="3" t="s">
+        <v>2116</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A141" s="3" t="s">
+        <v>2174</v>
+      </c>
+      <c r="C141" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="D141" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E141" s="44">
+        <v>2.5500000000000002E-3</v>
+      </c>
+      <c r="F141" s="44">
+        <v>5.0497500000000001E-2</v>
+      </c>
+      <c r="G141" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K141" s="28" t="s">
+        <v>2161</v>
+      </c>
+      <c r="L141" s="3" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A142" s="3" t="s">
+        <v>2175</v>
+      </c>
+      <c r="C142" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="D142" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E142" s="44">
+        <v>8.3617231179999998E-5</v>
+      </c>
+      <c r="F142" s="44">
+        <v>9.1442499999999996E-3</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K142" s="28" t="s">
+        <v>2161</v>
+      </c>
+      <c r="L142" s="3" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="143" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="3" t="s">
+        <v>2176</v>
+      </c>
+      <c r="C143" s="3" t="s">
+        <v>496</v>
+      </c>
+      <c r="D143" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E143" s="44">
+        <v>4.0000000000000003E-5</v>
+      </c>
+      <c r="F143" s="44">
+        <v>6.3245599999999999E-3</v>
+      </c>
+      <c r="G143" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K143" s="28" t="s">
+        <v>2177</v>
+      </c>
+      <c r="L143" s="3" t="s">
+        <v>2139</v>
+      </c>
+    </row>
+    <row r="144" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="3" t="s">
+        <v>2178</v>
+      </c>
+      <c r="C144" s="3" t="s">
+        <v>498</v>
+      </c>
+      <c r="D144" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E144" s="44">
+        <v>1.84E-4</v>
+      </c>
+      <c r="F144" s="44">
+        <v>1.3564700000000001E-2</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K144" s="28" t="s">
+        <v>2161</v>
+      </c>
+      <c r="L144" s="3" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="145" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A145" s="3" t="s">
+        <v>2179</v>
+      </c>
+      <c r="C145" s="3" t="s">
+        <v>522</v>
+      </c>
+      <c r="D145" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E145" s="44">
+        <v>1.5300000000000001E-4</v>
+      </c>
+      <c r="F145" s="44">
+        <v>1.23693E-2</v>
+      </c>
+      <c r="G145" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K145" s="28" t="s">
+        <v>2167</v>
+      </c>
+      <c r="L145" s="3" t="s">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="146" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A146" s="3" t="s">
+        <v>2180</v>
+      </c>
+      <c r="C146" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="D146" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E146" s="44">
+        <v>7.8659453649999997E-4</v>
+      </c>
+      <c r="F146" s="44">
+        <v>2.80463E-2</v>
+      </c>
+      <c r="G146" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K146" s="28" t="s">
+        <v>2181</v>
+      </c>
+      <c r="L146" s="3" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="147" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A147" s="3" t="s">
+        <v>2182</v>
+      </c>
+      <c r="C147" s="3" t="s">
+        <v>535</v>
+      </c>
+      <c r="D147" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E147" s="44">
+        <v>4.8999999999999998E-5</v>
+      </c>
+      <c r="F147" s="44">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="G147" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K147" s="28" t="s">
+        <v>2183</v>
+      </c>
+      <c r="L147" s="3" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="148" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A148" s="3" t="s">
+        <v>2184</v>
+      </c>
+      <c r="C148" s="3" t="s">
+        <v>542</v>
+      </c>
+      <c r="D148" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E148" s="44">
+        <v>8.8224787479999997E-4</v>
+      </c>
+      <c r="F148" s="44">
+        <v>2.9702699999999999E-2</v>
+      </c>
+      <c r="G148" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K148" s="28" t="s">
+        <v>2185</v>
+      </c>
+      <c r="L148" s="3" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="149" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="3" t="s">
+        <v>2186</v>
+      </c>
+      <c r="C149" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="D149" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E149" s="44">
+        <v>2.711074079E-4</v>
+      </c>
+      <c r="F149" s="44">
+        <v>1.6465299999999999E-2</v>
+      </c>
+      <c r="G149" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K149" s="28" t="s">
+        <v>2187</v>
+      </c>
+      <c r="L149" s="3" t="s">
+        <v>2109</v>
+      </c>
+    </row>
+    <row r="150" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A150" s="3" t="s">
+        <v>2188</v>
+      </c>
+      <c r="C150" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="D150" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E150" s="44">
+        <v>3.7399999999999998E-4</v>
+      </c>
+      <c r="F150" s="44">
+        <v>1.9339100000000001E-2</v>
+      </c>
+      <c r="G150" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K150" s="28" t="s">
+        <v>2167</v>
+      </c>
+      <c r="L150" s="3" t="s">
+        <v>2134</v>
+      </c>
+    </row>
+    <row r="151" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A151" s="3" t="s">
+        <v>2189</v>
+      </c>
+      <c r="C151" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="D151" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E151" s="44">
+        <v>3.86E-4</v>
+      </c>
+      <c r="F151" s="44">
+        <v>1.9646899999999998E-2</v>
+      </c>
+      <c r="G151" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K151" s="28" t="s">
+        <v>2163</v>
+      </c>
+      <c r="L151" s="3" t="s">
+        <v>2128</v>
+      </c>
+    </row>
+    <row r="152" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="3" t="s">
+        <v>2190</v>
+      </c>
+      <c r="C152" s="3" t="s">
+        <v>569</v>
+      </c>
+      <c r="D152" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E152" s="44">
+        <v>2.0899999999999998E-3</v>
+      </c>
+      <c r="F152" s="44">
+        <v>4.57165E-2</v>
+      </c>
+      <c r="G152" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K152" s="28" t="s">
+        <v>2155</v>
+      </c>
+      <c r="L152" s="3" t="s">
+        <v>2134</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="C1:L127"/>

</xml_diff>

<commit_message>
add trace init. concentrations for AlaAla[c], ArgArg[c], AsnAsn[c], AspAsp[c], CysCys[c], GlnGln[c], GluGlu[c], GlyGly[c], HisHis[c], IleIle[c], LeuLeu[c], LysLys[c], MetMet[c], PhePhe[c], ProPro[c], SerSer[c], ThrThr[c], TrpTrp[c], TyrTyr[c], ValVal[c] and LAC[e]
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="-35600" yWindow="980" windowWidth="35460" windowHeight="19900" tabRatio="500" firstSheet="6" activeTab="6"/>
-    <workbookView xWindow="920" yWindow="1300" windowWidth="35320" windowHeight="18900" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="-38380" yWindow="620" windowWidth="29040" windowHeight="20980" tabRatio="500" activeTab="11"/>
+    <workbookView minimized="1" xWindow="24640" yWindow="1000" windowWidth="13220" windowHeight="20380" tabRatio="500" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5015" uniqueCount="2203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5120" uniqueCount="2225">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -7037,6 +7037,72 @@
   </si>
   <si>
     <t>based on AA content the transcription reaction</t>
+  </si>
+  <si>
+    <t>dist-init-conc-AlaAla[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-ArgArg[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-AsnAsn[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-AspAsp[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-CysCys[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-GlnGln[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-GluGlu[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-GlyGly[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-HisHis[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-IleIle[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-LeuLeu[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-LysLys[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-MetMet[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-PhePhe[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-ProPro[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-SerSer[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-ThrThr[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-TrpTrp[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-TyrTyr[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-ValVal[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-LAC[e]</t>
+  </si>
+  <si>
+    <t>Trace amount estimated from other rare species</t>
   </si>
 </sst>
 </file>
@@ -7155,7 +7221,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -7267,6 +7333,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7282,7 +7351,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -8265,13 +8334,14 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:N178"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozenSplit"/>
-      <selection activeCell="A3" sqref="A3"/>
-      <selection pane="bottomLeft" activeCell="D146" sqref="D146"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="1600" topLeftCell="A30" activePane="bottomLeft"/>
+      <selection activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
-    <sheetView topLeftCell="A87" workbookViewId="1">
-      <selection activeCell="C99" sqref="C99"/>
+    <sheetView workbookViewId="1">
+      <pane ySplit="1340" topLeftCell="A11" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8292,11 +8362,11 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="42" t="s">
         <v>720</v>
       </c>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -13220,7 +13290,10 @@
       <selection activeCell="B2" sqref="B1:B1048576"/>
       <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
+      <pane ySplit="1240" topLeftCell="A3" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -16233,7 +16306,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0"/>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16332,7 +16405,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K37"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18942,26 +19017,26 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="43" t="s">
         <v>1746</v>
       </c>
-      <c r="H2" s="43"/>
-      <c r="I2" s="42" t="s">
+      <c r="H2" s="44"/>
+      <c r="I2" s="43" t="s">
         <v>1747</v>
       </c>
-      <c r="J2" s="43"/>
-      <c r="K2" s="43"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="43"/>
-      <c r="N2" s="43"/>
-      <c r="Q2" s="42" t="s">
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="Q2" s="43" t="s">
         <v>1748</v>
       </c>
-      <c r="R2" s="43"/>
-      <c r="S2" s="42" t="s">
+      <c r="R2" s="44"/>
+      <c r="S2" s="43" t="s">
         <v>1749</v>
       </c>
-      <c r="T2" s="43"/>
+      <c r="T2" s="44"/>
     </row>
     <row r="3" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -19460,10 +19535,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="43" t="s">
         <v>1796</v>
       </c>
-      <c r="H2" s="43"/>
+      <c r="H2" s="44"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -21092,18 +21167,18 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H2" s="39" t="s">
+      <c r="H2" s="40" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="M2" s="39" t="s">
+      <c r="I2" s="41"/>
+      <c r="J2" s="41"/>
+      <c r="K2" s="41"/>
+      <c r="M2" s="40" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
+      <c r="N2" s="41"/>
+      <c r="O2" s="41"/>
+      <c r="P2" s="41"/>
     </row>
     <row r="3" spans="1:21" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -21301,13 +21376,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N146"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1600" topLeftCell="A85" activePane="bottomLeft"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="1600" topLeftCell="A3" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="M117" sqref="M117"/>
+      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="1">
-      <selection activeCell="G65" sqref="G65"/>
+    <sheetView topLeftCell="A104" workbookViewId="1">
+      <selection activeCell="B123" sqref="B123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21331,14 +21406,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="40" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -25521,8 +25596,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J177"/>
   <sheetViews>
-    <sheetView topLeftCell="A148" workbookViewId="0">
-      <selection activeCell="C166" sqref="C166"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1040" topLeftCell="A53" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="A79" sqref="A79"/>
     </sheetView>
     <sheetView workbookViewId="1"/>
   </sheetViews>
@@ -28207,14 +28283,14 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L152"/>
+  <dimension ref="A1:L173"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A111" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E140" sqref="E140"/>
+      <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C173" sqref="C173"/>
     </sheetView>
     <sheetView topLeftCell="A107" workbookViewId="1">
-      <selection activeCell="E152" sqref="E152"/>
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -31653,10 +31729,10 @@
       <c r="D128" s="12" t="s">
         <v>90</v>
       </c>
-      <c r="E128" s="44">
+      <c r="E128" s="39">
         <v>3.4499999999999998E-5</v>
       </c>
-      <c r="F128" s="44">
+      <c r="F128" s="39">
         <v>5.8736700000000001E-3</v>
       </c>
       <c r="G128" s="3" t="s">
@@ -31676,10 +31752,10 @@
       <c r="D129" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E129" s="44">
+      <c r="E129" s="39">
         <v>2.62E-5</v>
       </c>
-      <c r="F129" s="44">
+      <c r="F129" s="39">
         <v>5.1185900000000001E-3</v>
       </c>
       <c r="G129" s="3" t="s">
@@ -31699,10 +31775,10 @@
       <c r="D130" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E130" s="44">
+      <c r="E130" s="39">
         <v>1.44E-4</v>
       </c>
-      <c r="F130" s="44">
+      <c r="F130" s="39">
         <v>1.2E-2</v>
       </c>
       <c r="G130" s="3" t="s">
@@ -31725,10 +31801,10 @@
       <c r="D131" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E131" s="44">
+      <c r="E131" s="39">
         <v>2.5900000000000002E-6</v>
       </c>
-      <c r="F131" s="44">
+      <c r="F131" s="39">
         <v>1.6093500000000001E-3</v>
       </c>
       <c r="G131" s="3" t="s">
@@ -31751,10 +31827,10 @@
       <c r="D132" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E132" s="44">
+      <c r="E132" s="39">
         <v>2.241537559E-6</v>
       </c>
-      <c r="F132" s="44">
+      <c r="F132" s="39">
         <v>1.4971800000000001E-3</v>
       </c>
       <c r="G132" s="3" t="s">
@@ -31777,10 +31853,10 @@
       <c r="D133" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E133" s="44">
+      <c r="E133" s="39">
         <v>2.7999999999999999E-6</v>
       </c>
-      <c r="F133" s="44">
+      <c r="F133" s="39">
         <v>1.6733200000000001E-3</v>
       </c>
       <c r="G133" s="3" t="s">
@@ -31803,10 +31879,10 @@
       <c r="D134" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E134" s="44">
+      <c r="E134" s="39">
         <v>2.5240096860000001E-3</v>
       </c>
-      <c r="F134" s="44">
+      <c r="F134" s="39">
         <v>5.0239499999999999E-2</v>
       </c>
       <c r="G134" s="3" t="s">
@@ -31829,10 +31905,10 @@
       <c r="D135" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E135" s="44">
+      <c r="E135" s="39">
         <v>1.52E-2</v>
       </c>
-      <c r="F135" s="44">
+      <c r="F135" s="39">
         <v>0.12328799999999999</v>
       </c>
       <c r="G135" s="3" t="s">
@@ -31855,10 +31931,10 @@
       <c r="D136" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E136" s="44">
+      <c r="E136" s="39">
         <v>2.3839486979999999E-5</v>
       </c>
-      <c r="F136" s="44">
+      <c r="F136" s="39">
         <v>4.8825700000000001E-3</v>
       </c>
       <c r="G136" s="3" t="s">
@@ -31881,10 +31957,10 @@
       <c r="D137" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E137" s="44">
+      <c r="E137" s="39">
         <v>1.5399999999999999E-3</v>
       </c>
-      <c r="F137" s="44">
+      <c r="F137" s="39">
         <v>3.9242800000000001E-2</v>
       </c>
       <c r="G137" s="3" t="s">
@@ -31907,10 +31983,10 @@
       <c r="D138" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E138" s="44">
+      <c r="E138" s="39">
         <v>1.15E-3</v>
       </c>
-      <c r="F138" s="44">
+      <c r="F138" s="39">
         <v>3.39116E-2</v>
       </c>
       <c r="G138" s="3" t="s">
@@ -31933,10 +32009,10 @@
       <c r="D139" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E139" s="44">
+      <c r="E139" s="39">
         <v>6.5099999999999997E-5</v>
       </c>
-      <c r="F139" s="44">
+      <c r="F139" s="39">
         <v>8.0684599999999995E-3</v>
       </c>
       <c r="G139" s="3" t="s">
@@ -31959,10 +32035,10 @@
       <c r="D140" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E140" s="44">
+      <c r="E140" s="39">
         <v>4.7952699999999999E-5</v>
       </c>
-      <c r="F140" s="44">
+      <c r="F140" s="39">
         <v>6.9247900000000001E-3</v>
       </c>
       <c r="G140" s="3" t="s">
@@ -31985,10 +32061,10 @@
       <c r="D141" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E141" s="44">
+      <c r="E141" s="39">
         <v>2.5500000000000002E-3</v>
       </c>
-      <c r="F141" s="44">
+      <c r="F141" s="39">
         <v>5.0497500000000001E-2</v>
       </c>
       <c r="G141" s="3" t="s">
@@ -32011,10 +32087,10 @@
       <c r="D142" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E142" s="44">
+      <c r="E142" s="39">
         <v>8.3617231179999998E-5</v>
       </c>
-      <c r="F142" s="44">
+      <c r="F142" s="39">
         <v>9.1442499999999996E-3</v>
       </c>
       <c r="G142" s="3" t="s">
@@ -32037,10 +32113,10 @@
       <c r="D143" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E143" s="44">
+      <c r="E143" s="39">
         <v>4.0000000000000003E-5</v>
       </c>
-      <c r="F143" s="44">
+      <c r="F143" s="39">
         <v>6.3245599999999999E-3</v>
       </c>
       <c r="G143" s="3" t="s">
@@ -32063,10 +32139,10 @@
       <c r="D144" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E144" s="44">
+      <c r="E144" s="39">
         <v>1.84E-4</v>
       </c>
-      <c r="F144" s="44">
+      <c r="F144" s="39">
         <v>1.3564700000000001E-2</v>
       </c>
       <c r="G144" s="3" t="s">
@@ -32089,10 +32165,10 @@
       <c r="D145" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E145" s="44">
+      <c r="E145" s="39">
         <v>1.5300000000000001E-4</v>
       </c>
-      <c r="F145" s="44">
+      <c r="F145" s="39">
         <v>1.23693E-2</v>
       </c>
       <c r="G145" s="3" t="s">
@@ -32115,10 +32191,10 @@
       <c r="D146" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E146" s="44">
+      <c r="E146" s="39">
         <v>7.8659453649999997E-4</v>
       </c>
-      <c r="F146" s="44">
+      <c r="F146" s="39">
         <v>2.80463E-2</v>
       </c>
       <c r="G146" s="3" t="s">
@@ -32141,10 +32217,10 @@
       <c r="D147" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E147" s="44">
+      <c r="E147" s="39">
         <v>4.8999999999999998E-5</v>
       </c>
-      <c r="F147" s="44">
+      <c r="F147" s="39">
         <v>7.0000000000000001E-3</v>
       </c>
       <c r="G147" s="3" t="s">
@@ -32167,10 +32243,10 @@
       <c r="D148" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E148" s="44">
+      <c r="E148" s="39">
         <v>8.8224787479999997E-4</v>
       </c>
-      <c r="F148" s="44">
+      <c r="F148" s="39">
         <v>2.9702699999999999E-2</v>
       </c>
       <c r="G148" s="3" t="s">
@@ -32193,10 +32269,10 @@
       <c r="D149" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E149" s="44">
+      <c r="E149" s="39">
         <v>2.711074079E-4</v>
       </c>
-      <c r="F149" s="44">
+      <c r="F149" s="39">
         <v>1.6465299999999999E-2</v>
       </c>
       <c r="G149" s="3" t="s">
@@ -32219,10 +32295,10 @@
       <c r="D150" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E150" s="44">
+      <c r="E150" s="39">
         <v>3.7399999999999998E-4</v>
       </c>
-      <c r="F150" s="44">
+      <c r="F150" s="39">
         <v>1.9339100000000001E-2</v>
       </c>
       <c r="G150" s="3" t="s">
@@ -32245,10 +32321,10 @@
       <c r="D151" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E151" s="44">
+      <c r="E151" s="39">
         <v>3.86E-4</v>
       </c>
-      <c r="F151" s="44">
+      <c r="F151" s="39">
         <v>1.9646899999999998E-2</v>
       </c>
       <c r="G151" s="3" t="s">
@@ -32271,10 +32347,10 @@
       <c r="D152" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E152" s="44">
+      <c r="E152" s="39">
         <v>2.0899999999999998E-3</v>
       </c>
-      <c r="F152" s="44">
+      <c r="F152" s="39">
         <v>4.57165E-2</v>
       </c>
       <c r="G152" s="3" t="s">
@@ -32285,6 +32361,489 @@
       </c>
       <c r="L152" s="3" t="s">
         <v>2134</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="3" t="s">
+        <v>2203</v>
+      </c>
+      <c r="C153" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="D153" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E153" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F153" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G153" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K153" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A154" s="3" t="s">
+        <v>2204</v>
+      </c>
+      <c r="C154" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="D154" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E154" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F154" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G154" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K154" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="155" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A155" s="3" t="s">
+        <v>2205</v>
+      </c>
+      <c r="C155" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="D155" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E155" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F155" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G155" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K155" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="156" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A156" s="3" t="s">
+        <v>2206</v>
+      </c>
+      <c r="C156" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="D156" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E156" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F156" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G156" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K156" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="3" t="s">
+        <v>2207</v>
+      </c>
+      <c r="C157" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="D157" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E157" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F157" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G157" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K157" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="3" t="s">
+        <v>2208</v>
+      </c>
+      <c r="C158" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="D158" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E158" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F158" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G158" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K158" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A159" s="3" t="s">
+        <v>2209</v>
+      </c>
+      <c r="C159" s="3" t="s">
+        <v>455</v>
+      </c>
+      <c r="D159" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E159" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F159" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G159" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K159" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A160" s="3" t="s">
+        <v>2210</v>
+      </c>
+      <c r="C160" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="D160" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E160" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F160" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G160" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K160" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A161" s="3" t="s">
+        <v>2211</v>
+      </c>
+      <c r="C161" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="D161" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E161" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F161" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G161" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K161" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A162" s="3" t="s">
+        <v>2212</v>
+      </c>
+      <c r="C162" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="D162" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E162" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F162" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G162" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K162" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="163" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="3" t="s">
+        <v>2213</v>
+      </c>
+      <c r="C163" s="3" t="s">
+        <v>483</v>
+      </c>
+      <c r="D163" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E163" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F163" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G163" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K163" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="164" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A164" s="3" t="s">
+        <v>2214</v>
+      </c>
+      <c r="C164" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="D164" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E164" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F164" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G164" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K164" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="165" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A165" s="3" t="s">
+        <v>2215</v>
+      </c>
+      <c r="C165" s="3" t="s">
+        <v>489</v>
+      </c>
+      <c r="D165" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E165" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F165" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G165" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K165" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="166" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="3" t="s">
+        <v>2216</v>
+      </c>
+      <c r="C166" s="3" t="s">
+        <v>510</v>
+      </c>
+      <c r="D166" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E166" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F166" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G166" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K166" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="167" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="3" t="s">
+        <v>2217</v>
+      </c>
+      <c r="C167" s="3" t="s">
+        <v>520</v>
+      </c>
+      <c r="D167" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E167" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F167" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G167" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K167" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="168" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A168" s="3" t="s">
+        <v>2218</v>
+      </c>
+      <c r="C168" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="D168" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E168" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F168" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G168" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K168" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="169" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A169" s="3" t="s">
+        <v>2219</v>
+      </c>
+      <c r="C169" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="D169" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E169" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F169" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G169" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K169" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="170" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A170" s="3" t="s">
+        <v>2220</v>
+      </c>
+      <c r="C170" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="D170" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E170" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F170" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G170" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K170" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="171" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="3" t="s">
+        <v>2221</v>
+      </c>
+      <c r="C171" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="D171" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E171" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F171" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G171" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K171" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="172" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="3" t="s">
+        <v>2222</v>
+      </c>
+      <c r="C172" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="D172" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E172" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F172" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G172" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K172" s="28" t="s">
+        <v>2224</v>
+      </c>
+    </row>
+    <row r="173" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A173" s="3" t="s">
+        <v>2223</v>
+      </c>
+      <c r="C173" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="D173" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E173" s="45">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="F173" s="3">
+        <v>1E-3</v>
+      </c>
+      <c r="G173" s="3" t="s">
+        <v>579</v>
+      </c>
+      <c r="K173" s="28" t="s">
+        <v>2224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
actually add trace init. concentrations for AlaAla[c], ArgArg[c], AsnAsn[c], AspAsp[c], CysCys[c], GlnGln[c], GluGlu[c], GlyGly[c], HisHis[c], IleIle[c], LeuLeu[c], LysLys[c], MetMet[c], PhePhe[c], ProPro[c], SerSer[c], ThrThr[c], TrpTrp[c], TyrTyr[c], ValVal[c] and LAC[e]
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38380" yWindow="620" windowWidth="29040" windowHeight="20980" tabRatio="500" activeTab="11"/>
+    <workbookView xWindow="-38380" yWindow="620" windowWidth="29040" windowHeight="20980" tabRatio="500" activeTab="8"/>
     <workbookView minimized="1" xWindow="24640" yWindow="1000" windowWidth="13220" windowHeight="20380" tabRatio="500" firstSheet="9" activeTab="12"/>
   </bookViews>
   <sheets>
@@ -8334,7 +8334,7 @@
   <sheetPr filterMode="1" enableFormatConditionsCalculation="0"/>
   <dimension ref="A1:N178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="1600" topLeftCell="A30" activePane="bottomLeft"/>
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
@@ -28285,7 +28285,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L173"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C173" sqref="C173"/>
     </sheetView>

</xml_diff>

<commit_message>
add comment on low population of H[c]
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-38380" yWindow="620" windowWidth="29040" windowHeight="20980" tabRatio="500" activeTab="8"/>
-    <workbookView minimized="1" xWindow="24640" yWindow="1000" windowWidth="13220" windowHeight="20380" tabRatio="500" firstSheet="9" activeTab="12"/>
+    <workbookView minimized="1" xWindow="-38380" yWindow="620" windowWidth="29040" windowHeight="20980" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="3320" yWindow="960" windowWidth="29880" windowHeight="20380" tabRatio="500" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5120" uniqueCount="2225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5121" uniqueCount="2226">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -7103,6 +7103,9 @@
   </si>
   <si>
     <t>Trace amount estimated from other rare species</t>
+  </si>
+  <si>
+    <t>Probably too small, as provides only 0.309 molecules</t>
   </si>
 </sst>
 </file>
@@ -7336,6 +7339,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -7350,9 +7356,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -8340,8 +8343,8 @@
       <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
     <sheetView workbookViewId="1">
-      <pane ySplit="1340" topLeftCell="A11" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
+      <pane ySplit="1340" topLeftCell="A42" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8362,11 +8365,11 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="42" t="s">
+      <c r="G2" s="43" t="s">
         <v>720</v>
       </c>
-      <c r="H2" s="41"/>
-      <c r="I2" s="41"/>
+      <c r="H2" s="42"/>
+      <c r="I2" s="42"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -13290,9 +13293,9 @@
       <selection activeCell="B2" sqref="B1:B1048576"/>
       <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
     </sheetView>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
-      <pane ySplit="1240" topLeftCell="A3" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="A41" sqref="A41"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
+      <pane ySplit="1240" topLeftCell="A33" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C55" sqref="C55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19017,26 +19020,26 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="44" t="s">
         <v>1746</v>
       </c>
-      <c r="H2" s="44"/>
-      <c r="I2" s="43" t="s">
+      <c r="H2" s="45"/>
+      <c r="I2" s="44" t="s">
         <v>1747</v>
       </c>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="M2" s="44"/>
-      <c r="N2" s="44"/>
-      <c r="Q2" s="43" t="s">
+      <c r="J2" s="45"/>
+      <c r="K2" s="45"/>
+      <c r="L2" s="45"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="45"/>
+      <c r="Q2" s="44" t="s">
         <v>1748</v>
       </c>
-      <c r="R2" s="44"/>
-      <c r="S2" s="43" t="s">
+      <c r="R2" s="45"/>
+      <c r="S2" s="44" t="s">
         <v>1749</v>
       </c>
-      <c r="T2" s="44"/>
+      <c r="T2" s="45"/>
     </row>
     <row r="3" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -19535,10 +19538,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="44" t="s">
         <v>1796</v>
       </c>
-      <c r="H2" s="44"/>
+      <c r="H2" s="45"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -21167,18 +21170,18 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="41"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="41"/>
-      <c r="M2" s="40" t="s">
+      <c r="I2" s="42"/>
+      <c r="J2" s="42"/>
+      <c r="K2" s="42"/>
+      <c r="M2" s="41" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="41"/>
-      <c r="O2" s="41"/>
-      <c r="P2" s="41"/>
+      <c r="N2" s="42"/>
+      <c r="O2" s="42"/>
+      <c r="P2" s="42"/>
     </row>
     <row r="3" spans="1:21" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -21406,14 +21409,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="41" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
-      <c r="G2" s="41"/>
-      <c r="H2" s="41"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="42"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -28289,8 +28292,9 @@
       <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C173" sqref="C173"/>
     </sheetView>
-    <sheetView topLeftCell="A107" workbookViewId="1">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <pane ySplit="1300" topLeftCell="A12" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -29568,7 +29572,9 @@
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
-      <c r="K47" s="30"/>
+      <c r="K47" s="30" t="s">
+        <v>2225</v>
+      </c>
       <c r="L47" s="1"/>
     </row>
     <row r="48" spans="1:12" ht="24" x14ac:dyDescent="0.2">
@@ -32373,7 +32379,7 @@
       <c r="D153" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E153" s="45">
+      <c r="E153" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F153" s="3">
@@ -32396,7 +32402,7 @@
       <c r="D154" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E154" s="45">
+      <c r="E154" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F154" s="3">
@@ -32419,7 +32425,7 @@
       <c r="D155" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E155" s="45">
+      <c r="E155" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F155" s="3">
@@ -32442,7 +32448,7 @@
       <c r="D156" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E156" s="45">
+      <c r="E156" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F156" s="3">
@@ -32465,7 +32471,7 @@
       <c r="D157" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E157" s="45">
+      <c r="E157" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F157" s="3">
@@ -32488,7 +32494,7 @@
       <c r="D158" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E158" s="45">
+      <c r="E158" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F158" s="3">
@@ -32511,7 +32517,7 @@
       <c r="D159" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E159" s="45">
+      <c r="E159" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F159" s="3">
@@ -32534,7 +32540,7 @@
       <c r="D160" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E160" s="45">
+      <c r="E160" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F160" s="3">
@@ -32557,7 +32563,7 @@
       <c r="D161" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E161" s="45">
+      <c r="E161" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F161" s="3">
@@ -32580,7 +32586,7 @@
       <c r="D162" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E162" s="45">
+      <c r="E162" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F162" s="3">
@@ -32603,7 +32609,7 @@
       <c r="D163" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E163" s="45">
+      <c r="E163" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F163" s="3">
@@ -32626,7 +32632,7 @@
       <c r="D164" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E164" s="45">
+      <c r="E164" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F164" s="3">
@@ -32649,7 +32655,7 @@
       <c r="D165" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E165" s="45">
+      <c r="E165" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F165" s="3">
@@ -32672,7 +32678,7 @@
       <c r="D166" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E166" s="45">
+      <c r="E166" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F166" s="3">
@@ -32695,7 +32701,7 @@
       <c r="D167" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E167" s="45">
+      <c r="E167" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F167" s="3">
@@ -32718,7 +32724,7 @@
       <c r="D168" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E168" s="45">
+      <c r="E168" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F168" s="3">
@@ -32741,7 +32747,7 @@
       <c r="D169" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E169" s="45">
+      <c r="E169" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F169" s="3">
@@ -32764,7 +32770,7 @@
       <c r="D170" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E170" s="45">
+      <c r="E170" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F170" s="3">
@@ -32787,7 +32793,7 @@
       <c r="D171" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E171" s="45">
+      <c r="E171" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F171" s="3">
@@ -32810,7 +32816,7 @@
       <c r="D172" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E172" s="45">
+      <c r="E172" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F172" s="3">
@@ -32833,7 +32839,7 @@
       <c r="D173" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="E173" s="45">
+      <c r="E173" s="40">
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="F173" s="3">

</xml_diff>

<commit_message>
add pyruvate, uracil & X5P structures & MWs; add D-Ribulose 5-phosphate smiles
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="-38380" yWindow="620" windowWidth="29040" windowHeight="20980" tabRatio="500" activeTab="8"/>
-    <workbookView xWindow="3320" yWindow="960" windowWidth="29880" windowHeight="20380" tabRatio="500" activeTab="8"/>
+    <workbookView minimized="1" xWindow="7420" yWindow="22060" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="8"/>
+    <workbookView xWindow="-21520" yWindow="640" windowWidth="21400" windowHeight="20540" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5121" uniqueCount="2226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5134" uniqueCount="2233">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -7106,6 +7106,27 @@
   </si>
   <si>
     <t>Probably too small, as provides only 0.309 molecules</t>
+  </si>
+  <si>
+    <t>C3H3O3</t>
+  </si>
+  <si>
+    <t>CC(=O)C(=O)[O-]</t>
+  </si>
+  <si>
+    <t>C(C(C(C(=O)CO)O)O)OP(=O)(O)O</t>
+  </si>
+  <si>
+    <t>Distinction from RL5P unclear in PubChem</t>
+  </si>
+  <si>
+    <t>C4H4N2O2</t>
+  </si>
+  <si>
+    <t>C1=CNC(=O)NC1=O</t>
+  </si>
+  <si>
+    <t>Datanator thinks this is Xylulose 5-phosphate</t>
   </si>
 </sst>
 </file>
@@ -7224,7 +7245,7 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -7341,6 +7362,9 @@
     </xf>
     <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -8342,9 +8366,9 @@
       <selection activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="D51" sqref="D51"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <pane ySplit="1340" topLeftCell="A42" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="D60" sqref="D60"/>
+    <sheetView topLeftCell="C1" workbookViewId="1">
+      <pane ySplit="1340" topLeftCell="A76" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="D110" sqref="D110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -8365,11 +8389,11 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="43" t="s">
+      <c r="G2" s="44" t="s">
         <v>720</v>
       </c>
-      <c r="H2" s="42"/>
-      <c r="I2" s="42"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -13294,8 +13318,8 @@
       <selection pane="bottomLeft" activeCell="F100" sqref="F100"/>
     </sheetView>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="1">
-      <pane ySplit="1240" topLeftCell="A33" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="C55" sqref="C55"/>
+      <pane ySplit="1240" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -19020,26 +19044,26 @@
       </c>
     </row>
     <row r="2" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="45" t="s">
         <v>1746</v>
       </c>
-      <c r="H2" s="45"/>
-      <c r="I2" s="44" t="s">
+      <c r="H2" s="46"/>
+      <c r="I2" s="45" t="s">
         <v>1747</v>
       </c>
-      <c r="J2" s="45"/>
-      <c r="K2" s="45"/>
-      <c r="L2" s="45"/>
-      <c r="M2" s="45"/>
-      <c r="N2" s="45"/>
-      <c r="Q2" s="44" t="s">
+      <c r="J2" s="46"/>
+      <c r="K2" s="46"/>
+      <c r="L2" s="46"/>
+      <c r="M2" s="46"/>
+      <c r="N2" s="46"/>
+      <c r="Q2" s="45" t="s">
         <v>1748</v>
       </c>
-      <c r="R2" s="45"/>
-      <c r="S2" s="44" t="s">
+      <c r="R2" s="46"/>
+      <c r="S2" s="45" t="s">
         <v>1749</v>
       </c>
-      <c r="T2" s="45"/>
+      <c r="T2" s="46"/>
     </row>
     <row r="3" spans="1:23" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -19538,10 +19562,10 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="G2" s="44" t="s">
+      <c r="G2" s="45" t="s">
         <v>1796</v>
       </c>
-      <c r="H2" s="45"/>
+      <c r="H2" s="46"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
@@ -21170,18 +21194,18 @@
       </c>
     </row>
     <row r="2" spans="1:21" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="H2" s="41" t="s">
+      <c r="H2" s="42" t="s">
         <v>71</v>
       </c>
-      <c r="I2" s="42"/>
-      <c r="J2" s="42"/>
-      <c r="K2" s="42"/>
-      <c r="M2" s="41" t="s">
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="43"/>
+      <c r="M2" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="N2" s="42"/>
-      <c r="O2" s="42"/>
-      <c r="P2" s="42"/>
+      <c r="N2" s="43"/>
+      <c r="O2" s="43"/>
+      <c r="P2" s="43"/>
     </row>
     <row r="3" spans="1:21" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -21384,8 +21408,9 @@
       <selection activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
-    <sheetView topLeftCell="A104" workbookViewId="1">
-      <selection activeCell="B123" sqref="B123"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="1">
+      <pane ySplit="1340" topLeftCell="A54" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="M87" sqref="M87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -21409,14 +21434,14 @@
       </c>
     </row>
     <row r="2" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="42" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
-      <c r="H2" s="42"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
     </row>
     <row r="3" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -23263,12 +23288,18 @@
       <c r="B65" s="1" t="s">
         <v>321</v>
       </c>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
+      <c r="C65" s="41" t="s">
+        <v>2227</v>
+      </c>
+      <c r="D65" s="41" t="s">
+        <v>1971</v>
+      </c>
       <c r="E65" s="1"/>
-      <c r="F65" s="1"/>
+      <c r="F65" s="41" t="s">
+        <v>2226</v>
+      </c>
       <c r="G65" s="35">
-        <v>10</v>
+        <v>87.05</v>
       </c>
       <c r="H65" s="22">
         <v>0</v>
@@ -23289,8 +23320,6 @@
       <c r="B66" s="1" t="s">
         <v>327</v>
       </c>
-      <c r="C66" s="31"/>
-      <c r="D66" s="1"/>
       <c r="E66" s="1"/>
       <c r="F66" s="26" t="s">
         <v>2089</v>
@@ -23307,7 +23336,9 @@
       <c r="J66" s="1"/>
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
-      <c r="M66" s="1"/>
+      <c r="M66" s="1" t="s">
+        <v>2229</v>
+      </c>
       <c r="N66" s="1"/>
     </row>
     <row r="67" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -23317,8 +23348,12 @@
       <c r="B67" s="1" t="s">
         <v>333</v>
       </c>
-      <c r="C67" s="1"/>
-      <c r="D67" s="1"/>
+      <c r="C67" s="41" t="s">
+        <v>2228</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>1971</v>
+      </c>
       <c r="E67" s="1"/>
       <c r="F67" s="26" t="s">
         <v>2089</v>
@@ -23345,7 +23380,7 @@
       <c r="B68" s="1" t="s">
         <v>347</v>
       </c>
-      <c r="C68" s="1"/>
+      <c r="C68" s="41"/>
       <c r="D68" s="1"/>
       <c r="E68" s="1"/>
       <c r="F68" s="26" t="s">
@@ -23731,12 +23766,18 @@
       <c r="B81" s="1" t="s">
         <v>386</v>
       </c>
-      <c r="C81" s="1"/>
-      <c r="D81" s="1"/>
+      <c r="C81" s="1" t="s">
+        <v>2231</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>1971</v>
+      </c>
       <c r="E81" s="1"/>
-      <c r="F81" s="1"/>
+      <c r="F81" s="1" t="s">
+        <v>2230</v>
+      </c>
       <c r="G81" s="35">
-        <v>10</v>
+        <v>112.09</v>
       </c>
       <c r="H81" s="22">
         <v>0</v>
@@ -23883,12 +23924,18 @@
       <c r="B86" s="1" t="s">
         <v>396</v>
       </c>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1"/>
+      <c r="C86" s="1" t="s">
+        <v>2228</v>
+      </c>
+      <c r="D86" s="41" t="s">
+        <v>1971</v>
+      </c>
       <c r="E86" s="1"/>
-      <c r="F86" s="1"/>
+      <c r="F86" s="1" t="s">
+        <v>2089</v>
+      </c>
       <c r="G86" s="35">
-        <v>10</v>
+        <v>230.11</v>
       </c>
       <c r="H86" s="22">
         <v>0</v>
@@ -23899,7 +23946,9 @@
       <c r="J86" s="1"/>
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
-      <c r="M86" s="1"/>
+      <c r="M86" s="1" t="s">
+        <v>2232</v>
+      </c>
       <c r="N86" s="1"/>
     </row>
     <row r="87" spans="1:14" ht="15.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -25603,7 +25652,9 @@
       <pane ySplit="1040" topLeftCell="A53" activePane="bottomLeft"/>
       <selection pane="bottomLeft" activeCell="A79" sqref="A79"/>
     </sheetView>
-    <sheetView workbookViewId="1"/>
+    <sheetView topLeftCell="A140" workbookViewId="1">
+      <selection activeCell="C177" sqref="C177"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -28292,9 +28343,9 @@
       <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C173" sqref="C173"/>
     </sheetView>
-    <sheetView tabSelected="1" workbookViewId="1">
-      <pane ySplit="1300" topLeftCell="A12" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="F47" sqref="F47"/>
+    <sheetView workbookViewId="1">
+      <pane ySplit="1300" topLeftCell="A99" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C123" sqref="C123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fix smiles for pyruvate
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -7111,9 +7111,6 @@
     <t>C3H3O3</t>
   </si>
   <si>
-    <t>CC(=O)C(=O)[O-]</t>
-  </si>
-  <si>
     <t>C(C(C(C(=O)CO)O)O)OP(=O)(O)O</t>
   </si>
   <si>
@@ -7127,6 +7124,9 @@
   </si>
   <si>
     <t>Datanator thinks this is Xylulose 5-phosphate</t>
+  </si>
+  <si>
+    <t>CC(=O)C(=O)[O]</t>
   </si>
 </sst>
 </file>
@@ -21410,7 +21410,7 @@
     </sheetView>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="1">
       <pane ySplit="1340" topLeftCell="A54" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="M87" sqref="M87"/>
+      <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -23289,7 +23289,7 @@
         <v>321</v>
       </c>
       <c r="C65" s="41" t="s">
-        <v>2227</v>
+        <v>2232</v>
       </c>
       <c r="D65" s="41" t="s">
         <v>1971</v>
@@ -23337,7 +23337,7 @@
       <c r="K66" s="1"/>
       <c r="L66" s="1"/>
       <c r="M66" s="1" t="s">
-        <v>2229</v>
+        <v>2228</v>
       </c>
       <c r="N66" s="1"/>
     </row>
@@ -23349,7 +23349,7 @@
         <v>333</v>
       </c>
       <c r="C67" s="41" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>1971</v>
@@ -23767,14 +23767,14 @@
         <v>386</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>2231</v>
+        <v>2230</v>
       </c>
       <c r="D81" s="1" t="s">
         <v>1971</v>
       </c>
       <c r="E81" s="1"/>
       <c r="F81" s="1" t="s">
-        <v>2230</v>
+        <v>2229</v>
       </c>
       <c r="G81" s="35">
         <v>112.09</v>
@@ -23925,7 +23925,7 @@
         <v>396</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>2228</v>
+        <v>2227</v>
       </c>
       <c r="D86" s="41" t="s">
         <v>1971</v>
@@ -23947,7 +23947,7 @@
       <c r="K86" s="1"/>
       <c r="L86" s="1"/>
       <c r="M86" s="1" t="s">
-        <v>2232</v>
+        <v>2231</v>
       </c>
       <c r="N86" s="1"/>
     </row>

</xml_diff>

<commit_message>
add init. concs. for PYR[c], URA[c] & X5P[c]
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <bookViews>
     <workbookView minimized="1" xWindow="7420" yWindow="22060" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="8"/>
-    <workbookView xWindow="-21520" yWindow="640" windowWidth="21400" windowHeight="20540" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="-21520" yWindow="640" windowWidth="21400" windowHeight="20540" tabRatio="500" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5134" uniqueCount="2233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5146" uniqueCount="2236">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -7127,6 +7127,15 @@
   </si>
   <si>
     <t>CC(=O)C(=O)[O]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-PYR[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-URA[c]</t>
+  </si>
+  <si>
+    <t>dist-init-conc-X5P[c]</t>
   </si>
 </sst>
 </file>
@@ -21408,7 +21417,7 @@
       <selection activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
     </sheetView>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="1">
+    <sheetView topLeftCell="B1" workbookViewId="1">
       <pane ySplit="1340" topLeftCell="A54" activePane="bottomLeft"/>
       <selection pane="bottomLeft" activeCell="C66" sqref="C66"/>
     </sheetView>
@@ -28337,15 +28346,15 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L173"/>
+  <dimension ref="A1:L176"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C173" sqref="C173"/>
     </sheetView>
-    <sheetView workbookViewId="1">
-      <pane ySplit="1300" topLeftCell="A99" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="C123" sqref="C123"/>
+    <sheetView tabSelected="1" workbookViewId="1">
+      <pane ySplit="1300" topLeftCell="A125" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C174" sqref="C174:C176"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -32903,6 +32912,66 @@
         <v>2224</v>
       </c>
     </row>
+    <row r="174" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A174" s="3" t="s">
+        <v>2233</v>
+      </c>
+      <c r="C174" s="3" t="s">
+        <v>529</v>
+      </c>
+      <c r="D174" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E174" s="40">
+        <v>2.7000000000000001E-7</v>
+      </c>
+      <c r="F174" s="3">
+        <v>5.1961524227099999E-4</v>
+      </c>
+      <c r="G174" s="3" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="175" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="3" t="s">
+        <v>2234</v>
+      </c>
+      <c r="C175" s="3" t="s">
+        <v>567</v>
+      </c>
+      <c r="D175" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E175" s="3">
+        <v>1.013E-3</v>
+      </c>
+      <c r="F175" s="40">
+        <v>9.8999999999999994E-5</v>
+      </c>
+      <c r="G175" s="3" t="s">
+        <v>579</v>
+      </c>
+    </row>
+    <row r="176" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="3" t="s">
+        <v>2235</v>
+      </c>
+      <c r="C176" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="D176" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="E176" s="40">
+        <v>1.0200000000000001E-3</v>
+      </c>
+      <c r="F176" s="3">
+        <v>3.1937438845343002E-2</v>
+      </c>
+      <c r="G176" s="3" t="s">
+        <v>579</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="C1:L127"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
add !References for init. concs. for PYR[c], URA[c] & X5P[c]
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -9,8 +9,8 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="7420" yWindow="22060" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="8"/>
-    <workbookView xWindow="-21520" yWindow="640" windowWidth="21400" windowHeight="20540" tabRatio="500" firstSheet="1" activeTab="8"/>
+    <workbookView xWindow="-19200" yWindow="800" windowWidth="18420" windowHeight="20440" tabRatio="500" firstSheet="16" activeTab="21"/>
+    <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="21400" windowHeight="15540" tabRatio="500" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="!!_Table of contents" sheetId="1" r:id="rId1"/>
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5146" uniqueCount="2236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5167" uniqueCount="2244">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -7136,6 +7136,30 @@
   </si>
   <si>
     <t>dist-init-conc-X5P[c]</t>
+  </si>
+  <si>
+    <t>Ref_0031</t>
+  </si>
+  <si>
+    <t>PubChemAID_977611</t>
+  </si>
+  <si>
+    <t>Experimentally measured binding affinity data (Kd) for protein-ligand complexes derived from PDB</t>
+  </si>
+  <si>
+    <t>Shanghai Institute of Organic Chemistry</t>
+  </si>
+  <si>
+    <t>URL: https://pubchem.ncbi.nlm.nih.gov/compound/107735#section=BioAssay-Results</t>
+  </si>
+  <si>
+    <t>Ref_0032</t>
+  </si>
+  <si>
+    <t>Ref_0033</t>
+  </si>
+  <si>
+    <t>DOI: 10.1038/nchembio.186</t>
   </si>
 </sst>
 </file>
@@ -19707,10 +19731,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1580" topLeftCell="A19" activePane="bottomLeft"/>
       <selection activeCell="Q2" sqref="Q2"/>
-      <selection pane="bottomLeft" activeCell="A25" sqref="A25"/>
+      <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
     </sheetView>
     <sheetView workbookViewId="1">
       <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
@@ -20670,7 +20694,7 @@
         <v>2133</v>
       </c>
     </row>
-    <row r="28" spans="1:18" ht="113" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:18" ht="57" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>2134</v>
       </c>
@@ -20694,9 +20718,6 @@
       </c>
       <c r="I28" s="3" t="s">
         <v>2114</v>
-      </c>
-      <c r="L28" s="3" t="s">
-        <v>2138</v>
       </c>
       <c r="Q28" s="3" t="s">
         <v>2138</v>
@@ -20757,16 +20778,88 @@
         <v>2150</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C31" s="25"/>
-    </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="C32" s="25"/>
-    </row>
-    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C33" s="25"/>
-    </row>
-    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:18" ht="43" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>2236</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>2237</v>
+      </c>
+      <c r="C31" s="25" t="s">
+        <v>2238</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>2239</v>
+      </c>
+      <c r="F31" s="3">
+        <v>2014</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>1930</v>
+      </c>
+      <c r="Q31" s="3" t="s">
+        <v>2240</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="57" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>2241</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>2145</v>
+      </c>
+      <c r="C32" s="25" t="s">
+        <v>2146</v>
+      </c>
+      <c r="D32" s="3" t="s">
+        <v>2147</v>
+      </c>
+      <c r="F32" s="3">
+        <v>2007</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>1826</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>2148</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>2149</v>
+      </c>
+      <c r="Q32" s="3" t="s">
+        <v>2150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="57" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>2242</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>2135</v>
+      </c>
+      <c r="C33" s="25" t="s">
+        <v>2136</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>2137</v>
+      </c>
+      <c r="F33" s="3">
+        <v>2009</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>1826</v>
+      </c>
+      <c r="H33" s="3" t="s">
+        <v>2113</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>2114</v>
+      </c>
+      <c r="Q33" s="3" t="s">
+        <v>2243</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.2">
       <c r="C34" s="25"/>
     </row>
   </sheetData>
@@ -21413,9 +21506,9 @@
   <dimension ref="A1:N146"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1600" topLeftCell="A3" activePane="bottomLeft"/>
+      <pane ySplit="1600" topLeftCell="A45" activePane="bottomLeft"/>
       <selection activeCell="F1" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="B7" sqref="B7"/>
+      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
     </sheetView>
     <sheetView topLeftCell="B1" workbookViewId="1">
       <pane ySplit="1340" topLeftCell="A54" activePane="bottomLeft"/>
@@ -28348,13 +28441,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L176"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="C173" sqref="C173"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
-      <pane ySplit="1300" topLeftCell="A125" activePane="bottomLeft"/>
-      <selection pane="bottomLeft" activeCell="C174" sqref="C174:C176"/>
+      <pane ySplit="1300" topLeftCell="A136" activePane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E185" sqref="E185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
finish "add !References for init. concs. for PYR[c], URA[c] & X5P[c]"
</commit_message>
<xml_diff>
--- a/tests/submodels/fixtures/4_submodel_MP_model.xlsx
+++ b/tests/submodels/fixtures/4_submodel_MP_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-19200" yWindow="800" windowWidth="18420" windowHeight="20440" tabRatio="500" firstSheet="16" activeTab="21"/>
+    <workbookView xWindow="-19200" yWindow="800" windowWidth="18420" windowHeight="20440" tabRatio="500" firstSheet="8" activeTab="8"/>
     <workbookView minimized="1" xWindow="0" yWindow="460" windowWidth="21400" windowHeight="15540" tabRatio="500" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
@@ -426,7 +426,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5167" uniqueCount="2244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5173" uniqueCount="2246">
   <si>
     <t>!!!ObjTables objTablesVersion='0.0.8'</t>
   </si>
@@ -7160,6 +7160,12 @@
   </si>
   <si>
     <t>DOI: 10.1038/nchembio.186</t>
+  </si>
+  <si>
+    <t>Cannot clearly identify in Datanator</t>
+  </si>
+  <si>
+    <t>From Escherichia coli BL21 DE3</t>
   </si>
 </sst>
 </file>
@@ -19731,7 +19737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1580" topLeftCell="A19" activePane="bottomLeft"/>
       <selection activeCell="Q2" sqref="Q2"/>
       <selection pane="bottomLeft" activeCell="A31" sqref="A31"/>
@@ -28441,9 +28447,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L176"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A129" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C173" sqref="C173"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A132" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A174" sqref="A174"/>
     </sheetView>
     <sheetView tabSelected="1" workbookViewId="1">
       <pane ySplit="1300" topLeftCell="A136" activePane="bottomLeft"/>
@@ -32706,7 +32712,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="161" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A161" s="3" t="s">
         <v>2211</v>
       </c>
@@ -32729,7 +32735,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="162" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A162" s="3" t="s">
         <v>2212</v>
       </c>
@@ -32752,7 +32758,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="163" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="3" t="s">
         <v>2213</v>
       </c>
@@ -32775,7 +32781,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="164" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="3" t="s">
         <v>2214</v>
       </c>
@@ -32798,7 +32804,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="165" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A165" s="3" t="s">
         <v>2215</v>
       </c>
@@ -32821,7 +32827,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="166" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A166" s="3" t="s">
         <v>2216</v>
       </c>
@@ -32844,7 +32850,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="167" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A167" s="3" t="s">
         <v>2217</v>
       </c>
@@ -32867,7 +32873,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="168" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="3" t="s">
         <v>2218</v>
       </c>
@@ -32890,7 +32896,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="169" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="3" t="s">
         <v>2219</v>
       </c>
@@ -32913,7 +32919,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="170" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A170" s="3" t="s">
         <v>2220</v>
       </c>
@@ -32936,7 +32942,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="171" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A171" s="3" t="s">
         <v>2221</v>
       </c>
@@ -32959,7 +32965,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="172" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A172" s="3" t="s">
         <v>2222</v>
       </c>
@@ -32982,7 +32988,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="173" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="3" t="s">
         <v>2223</v>
       </c>
@@ -33005,7 +33011,7 @@
         <v>2224</v>
       </c>
     </row>
-    <row r="174" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="3" t="s">
         <v>2233</v>
       </c>
@@ -33024,8 +33030,14 @@
       <c r="G174" s="3" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="175" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K174" s="28" t="s">
+        <v>2244</v>
+      </c>
+      <c r="L174" s="3" t="s">
+        <v>2236</v>
+      </c>
+    </row>
+    <row r="175" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A175" s="3" t="s">
         <v>2234</v>
       </c>
@@ -33044,8 +33056,14 @@
       <c r="G175" s="3" t="s">
         <v>579</v>
       </c>
-    </row>
-    <row r="176" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="K175" s="28" t="s">
+        <v>2245</v>
+      </c>
+      <c r="L175" s="3" t="s">
+        <v>2241</v>
+      </c>
+    </row>
+    <row r="176" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A176" s="3" t="s">
         <v>2235</v>
       </c>
@@ -33063,6 +33081,12 @@
       </c>
       <c r="G176" s="3" t="s">
         <v>579</v>
+      </c>
+      <c r="K176" s="28" t="s">
+        <v>2155</v>
+      </c>
+      <c r="L176" s="3" t="s">
+        <v>2242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>